<commit_message>
add two commented pictures
</commit_message>
<xml_diff>
--- a/photos.xlsx
+++ b/photos.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cedri\Documents\web\araignees_idf\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3BD33140-B331-474A-BFA4-9500116799CC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{145E0451-82A3-42C8-B961-9E743842C836}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-105" yWindow="0" windowWidth="19410" windowHeight="15585" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="852" uniqueCount="844">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="667" uniqueCount="659">
   <si>
     <t>taxon</t>
   </si>
@@ -1963,576 +1963,15 @@
     <t>Zoropsis spinimana</t>
   </si>
   <si>
-    <t>https://geonature.arb-idf.fr/geonature/api//media/attachments/4/79560_P1663592.jpg</t>
-  </si>
-  <si>
-    <t>https://geonature.arb-idf.fr/geonature/api//media/attachments/4/87632_P1710683.jpg</t>
-  </si>
-  <si>
-    <t>https://inaturalist-open-data.s3.amazonaws.com/photos/170022520/original.jpg</t>
-  </si>
-  <si>
-    <t>https://inaturalist-open-data.s3.amazonaws.com/photos/79099930/original.jpeg</t>
-  </si>
-  <si>
-    <t>https://inaturalist-open-data.s3.amazonaws.com/photos/328806724/original.jpg</t>
-  </si>
-  <si>
-    <t>https://inaturalist-open-data.s3.amazonaws.com/photos/388672931/original.jpg</t>
-  </si>
-  <si>
-    <t>https://inaturalist-open-data.s3.amazonaws.com/photos/370594043/original.jpg</t>
-  </si>
-  <si>
-    <t>https://geonature.arb-idf.fr/geonature/api//media/attachments/4/92650_P1802168.jpg</t>
-  </si>
-  <si>
-    <t>https://geonature.arb-idf.fr/geonature/api//media/attachments/4/45258_rect58_04.jpg</t>
-  </si>
-  <si>
-    <t>https://geonature.arb-idf.fr/geonature/api//media/attachments/4/58407_P1661506.jpg</t>
-  </si>
-  <si>
-    <t>https://geonature.arb-idf.fr/geonature/api//media/attachments/4/59017_P1661925.jpg</t>
-  </si>
-  <si>
-    <t>https://geonature.arb-idf.fr/geonature/api//media/attachments/4/82918_P1662900.jpg</t>
-  </si>
-  <si>
-    <t>https://inaturalist-open-data.s3.amazonaws.com/photos/442093819/original.jpg</t>
-  </si>
-  <si>
-    <t>https://inaturalist-open-data.s3.amazonaws.com/photos/79100177/original.jpeg</t>
-  </si>
-  <si>
-    <t>https://geonature.arb-idf.fr/geonature/api//media/attachments/4/88719_P1732556.jpg</t>
-  </si>
-  <si>
-    <t>https://geonature.arb-idf.fr/geonature/api//media/attachments/4/88488_P1732105.jpg</t>
-  </si>
-  <si>
-    <t>https://geonature.arb-idf.fr/geonature/api//media/attachments/4/45012_P1636003.jpg</t>
-  </si>
-  <si>
-    <t>https://geonature.arb-idf.fr/geonature/api//media/attachments/4/58081_P1661472.jpg</t>
-  </si>
-  <si>
-    <t>https://geonature.arb-idf.fr/geonature/api//media/attachments/4/90535_P1766557.jpg</t>
-  </si>
-  <si>
-    <t>https://geonature.arb-idf.fr/geonature/api//media/attachments/4/45005_P1636078_02.jpg</t>
-  </si>
-  <si>
-    <t>https://geonature.arb-idf.fr/geonature/api//media/attachments/4/45299_rect582.jpg</t>
-  </si>
-  <si>
-    <t>https://geonature.arb-idf.fr/geonature/api//media/attachments/4/48458_P1628508.jpg</t>
-  </si>
-  <si>
-    <t>https://inaturalist-open-data.s3.amazonaws.com/photos/34062971/original.jpg</t>
-  </si>
-  <si>
-    <t>https://inaturalist-open-data.s3.amazonaws.com/photos/345567970/original.jpg</t>
-  </si>
-  <si>
-    <t>https://geonature.arb-idf.fr/geonature/api//media/attachments/4/86959_P1709828.jpg</t>
-  </si>
-  <si>
-    <t>https://inaturalist-open-data.s3.amazonaws.com/photos/226888388/original.jpg</t>
-  </si>
-  <si>
-    <t>https://geonature.arb-idf.fr/geonature/api//media/attachments/4/45606_P1638690.jpg</t>
-  </si>
-  <si>
-    <t>https://geonature.arb-idf.fr/geonature/api//media/attachments/4/48288_photos_20210923171104_1.jpg</t>
-  </si>
-  <si>
-    <t>https://geonature.arb-idf.fr/geonature/api//media/attachments/4/45608_P1638799.jpg</t>
-  </si>
-  <si>
-    <t>https://geonature.arb-idf.fr/geonature/api//media/attachments/4/86338_P1709185.jpg</t>
-  </si>
-  <si>
-    <t>https://geonature.arb-idf.fr/geonature/api//media/attachments/4/47486_photos_20220618092245.jpg</t>
-  </si>
-  <si>
-    <t>https://inaturalist-open-data.s3.amazonaws.com/photos/388322363/original.jpg</t>
-  </si>
-  <si>
-    <t>https://geonature.arb-idf.fr/geonature/api//media/attachments/4/49293_P1647058.jpg</t>
-  </si>
-  <si>
-    <t>https://geonature.arb-idf.fr/geonature/api//media/attachments/4/45348_image10.jpg</t>
-  </si>
-  <si>
-    <t>https://cardobs.mnhn.fr/cardObs/photos/download/15369_26112023104942_3153_1.jpg</t>
-  </si>
-  <si>
-    <t>https://geonature.arb-idf.fr/geonature/api//media/attachments/4/91720_P1638658.jpg</t>
-  </si>
-  <si>
     <t>Thyreosthenius parasiticus</t>
   </si>
   <si>
-    <t>https://geonature.arb-idf.fr/geonature/api//media/attachments/4/82906_P1662798.jpg</t>
-  </si>
-  <si>
-    <t>https://geonature.arb-idf.fr/geonature/api//media/attachments/4/46135_P1640880.jpg</t>
-  </si>
-  <si>
-    <t>https://geonature.arb-idf.fr/geonature/api//media/attachments/4/45250_P1629428_02.jpg</t>
-  </si>
-  <si>
-    <t>https://geonature.arb-idf.fr/geonature/api//media/attachments/4/92496_P1766843.jpg</t>
-  </si>
-  <si>
-    <t>https://inaturalist-open-data.s3.amazonaws.com/photos/384431070/original.jpg</t>
-  </si>
-  <si>
-    <t>https://geonature.arb-idf.fr/geonature/api//media/attachments/4/46295_P1641513.jpg</t>
-  </si>
-  <si>
-    <t>https://inaturalist-open-data.s3.amazonaws.com/photos/329962329/original.jpg</t>
-  </si>
-  <si>
-    <t>https://geonature.arb-idf.fr/geonature/api//media/attachments/4/45246_P1630438_03.jpg</t>
-  </si>
-  <si>
-    <t>https://geonature.arb-idf.fr/geonature/api//media/attachments/4/45267_rect82_03.jpg</t>
-  </si>
-  <si>
-    <t>https://geonature.arb-idf.fr/geonature/api//media/attachments/4/91588_P1766768.jpg</t>
-  </si>
-  <si>
-    <t>https://geonature.arb-idf.fr/geonature/api//media/attachments/4/92619_P1801918.jpg</t>
-  </si>
-  <si>
-    <t>https://geonature.arb-idf.fr/geonature/api//media/attachments/4/92310_P1801153.jpg</t>
-  </si>
-  <si>
-    <t>https://inaturalist-open-data.s3.amazonaws.com/photos/75324667/original.png</t>
-  </si>
-  <si>
-    <t>https://geonature.arb-idf.fr/geonature/api//media/attachments/4/57388_P1660307_cr.jpg</t>
-  </si>
-  <si>
     <t>male</t>
   </si>
   <si>
     <t>femelle</t>
   </si>
   <si>
-    <t>https://inaturalist-open-data.s3.amazonaws.com/photos/225178519/original.jpg</t>
-  </si>
-  <si>
-    <t>https://geonature.arb-idf.fr/geonature/api//media/attachments/4/46557_g959.jpg</t>
-  </si>
-  <si>
-    <t>https://geonature.arb-idf.fr/geonature/api//media/attachments/4/92385_IMG_20240707_123854.jpg</t>
-  </si>
-  <si>
-    <t>https://geonature.arb-idf.fr/geonature/api//media/attachments/4/87684_P1721550.jpg</t>
-  </si>
-  <si>
-    <t>https://inaturalist-open-data.s3.amazonaws.com/photos/164071730/original.jpg</t>
-  </si>
-  <si>
-    <t>https://geonature.arb-idf.fr/geonature/api//media/attachments/4/49530_P1639224.jpg</t>
-  </si>
-  <si>
-    <t>https://geonature.arb-idf.fr/geonature/api//media/attachments/4/90459_P1711003.jpg</t>
-  </si>
-  <si>
-    <t>https://inaturalist-open-data.s3.amazonaws.com/photos/328569562/original.jpg</t>
-  </si>
-  <si>
-    <t>https://inaturalist-open-data.s3.amazonaws.com/photos/388670964/original.jpg</t>
-  </si>
-  <si>
-    <t>https://geonature.arb-idf.fr/geonature/api//media/attachments/4/83002_P1662757.jpg</t>
-  </si>
-  <si>
-    <t>https://geonature.arb-idf.fr/geonature/api//media/attachments/4/46120_P1640650.jpg</t>
-  </si>
-  <si>
-    <t>https://geonature.arb-idf.fr/geonature/api//media/attachments/4/46122_P1640713.jpg</t>
-  </si>
-  <si>
-    <t>https://inaturalist-open-data.s3.amazonaws.com/photos/313178149/original.jpg</t>
-  </si>
-  <si>
-    <t>https://geonature.arb-idf.fr/geonature/api//media/attachments/4/49083_P1647003.jpg</t>
-  </si>
-  <si>
-    <t>https://geonature.arb-idf.fr/geonature/api//media/attachments/4/83674_P1676689.jpg</t>
-  </si>
-  <si>
-    <t>https://geonature.arb-idf.fr/geonature/api//media/attachments/4/83820_P1676776.jpg</t>
-  </si>
-  <si>
-    <t>https://inaturalist-open-data.s3.amazonaws.com/photos/224272635/original.jpg</t>
-  </si>
-  <si>
-    <t>https://geonature.arb-idf.fr/geonature/api//media/attachments/4/57840_P1661525.jpg</t>
-  </si>
-  <si>
-    <t>https://inaturalist-open-data.s3.amazonaws.com/photos/128087625/original.jpg</t>
-  </si>
-  <si>
-    <t>https://inaturalist-open-data.s3.amazonaws.com/photos/130929112/original.jpg</t>
-  </si>
-  <si>
-    <t>https://geonature.arb-idf.fr/geonature/api//media/attachments/4/94297_IMG_20240909_084830.jpg</t>
-  </si>
-  <si>
-    <t>https://geonature.arb-idf.fr/geonature/api//media/attachments/4/95175_2024-10-06-22-45-17.jpg</t>
-  </si>
-  <si>
-    <t>https://inaturalist-open-data.s3.amazonaws.com/photos/384437007/original.jpg</t>
-  </si>
-  <si>
-    <t>https://inaturalist-open-data.s3.amazonaws.com/photos/96665150/original.jpg</t>
-  </si>
-  <si>
-    <t>https://geonature.arb-idf.fr/geonature/api//media/attachments/4/95040_P1824880.jpg</t>
-  </si>
-  <si>
-    <t>https://inaturalist-open-data.s3.amazonaws.com/photos/225083974/original.jpg</t>
-  </si>
-  <si>
-    <t>https://inaturalist-open-data.s3.amazonaws.com/photos/225088849/original.jpg</t>
-  </si>
-  <si>
-    <t>https://inaturalist-open-data.s3.amazonaws.com/photos/76530568/original.png</t>
-  </si>
-  <si>
-    <t>https://inaturalist-open-data.s3.amazonaws.com/photos/76546564/original.png</t>
-  </si>
-  <si>
-    <t>https://inaturalist-open-data.s3.amazonaws.com/photos/392410024/original.jpg</t>
-  </si>
-  <si>
-    <t>https://geonature.arb-idf.fr/geonature/api//media/attachments/4/88755_P1732638.jpg</t>
-  </si>
-  <si>
-    <t>https://geonature.arb-idf.fr/geonature/api//media/attachments/4/47752_photos_20220623175101.jpg</t>
-  </si>
-  <si>
-    <t>https://geonature.arb-idf.fr/geonature/api//media/attachments/4/89750_P1755535.jpg</t>
-  </si>
-  <si>
-    <t>https://inaturalist-open-data.s3.amazonaws.com/photos/118387627/original.jpg</t>
-  </si>
-  <si>
-    <t>https://geonature.arb-idf.fr/geonature/api//media/attachments/4/58871_P1662214.jpg</t>
-  </si>
-  <si>
-    <t>https://geonature.arb-idf.fr/geonature/api//media/attachments/4/45690_P1500375.jpg</t>
-  </si>
-  <si>
-    <t>https://inaturalist-open-data.s3.amazonaws.com/photos/101381114/original.jpg</t>
-  </si>
-  <si>
-    <t>https://geonature.arb-idf.fr/geonature/api//media/attachments/4/45315_P1632248.jpg</t>
-  </si>
-  <si>
-    <t>https://geonature.arb-idf.fr/geonature/api//media/attachments/4/46022_P1640491.jpg</t>
-  </si>
-  <si>
-    <t>https://inaturalist-open-data.s3.amazonaws.com/photos/79368826/original.jpeg</t>
-  </si>
-  <si>
-    <t>https://geonature.arb-idf.fr/geonature/api//media/attachments/4/83030_P1663104.jpg</t>
-  </si>
-  <si>
-    <t>https://geonature.arb-idf.fr/geonature/api//media/attachments/4/85740_P1698731.jpg</t>
-  </si>
-  <si>
-    <t>https://geonature.arb-idf.fr/geonature/api//media/attachments/4/57834_P1661364.jpg</t>
-  </si>
-  <si>
-    <t>https://geonature.arb-idf.fr/geonature/api//media/attachments/4/57841_P1661489.jpg</t>
-  </si>
-  <si>
-    <t>https://inaturalist-open-data.s3.amazonaws.com/photos/75343149/original.jpg</t>
-  </si>
-  <si>
-    <t>https://inaturalist-open-data.s3.amazonaws.com/photos/37451658/original.jpg</t>
-  </si>
-  <si>
-    <t>https://geonature.arb-idf.fr/geonature/api//media/attachments/4/59047_P1662425.jpg</t>
-  </si>
-  <si>
-    <t>https://inaturalist-open-data.s3.amazonaws.com/photos/67675081/original.png</t>
-  </si>
-  <si>
-    <t>https://inaturalist-open-data.s3.amazonaws.com/photos/75367338/original.png</t>
-  </si>
-  <si>
-    <t>https://geonature.arb-idf.fr/geonature/api//media/attachments/4/91713_P1766633.jpg</t>
-  </si>
-  <si>
-    <t>https://geonature.arb-idf.fr/geonature/api//media/attachments/4/58879_P1662219.jpg</t>
-  </si>
-  <si>
-    <t>https://inaturalist-open-data.s3.amazonaws.com/photos/76430906/original.png</t>
-  </si>
-  <si>
-    <t>https://geonature.arb-idf.fr/geonature/api//media/attachments/4/46722_photos_20220510165510_1.jpg</t>
-  </si>
-  <si>
-    <t>https://inaturalist-open-data.s3.amazonaws.com/photos/33355256/original.jpg</t>
-  </si>
-  <si>
-    <t>https://inaturalist-open-data.s3.amazonaws.com/photos/71839773/original.jpg</t>
-  </si>
-  <si>
-    <t>https://geonature.arb-idf.fr/geonature/api//media/attachments/4/94079_P1824342.jpg</t>
-  </si>
-  <si>
-    <t>https://geonature.arb-idf.fr/geonature/api//media/attachments/4/45265_rect70_03.jpg</t>
-  </si>
-  <si>
-    <t>https://inaturalist-open-data.s3.amazonaws.com/photos/73564233/original.png</t>
-  </si>
-  <si>
-    <t>https://inaturalist-open-data.s3.amazonaws.com/photos/93726353/original.jpg</t>
-  </si>
-  <si>
-    <t>https://geonature.arb-idf.fr/geonature/api//media/attachments/4/88323_P1721755.jpg</t>
-  </si>
-  <si>
-    <t>https://inaturalist-open-data.s3.amazonaws.com/photos/79101896/original.jpeg</t>
-  </si>
-  <si>
-    <t>https://inaturalist-open-data.s3.amazonaws.com/photos/75540812/original.png</t>
-  </si>
-  <si>
-    <t>https://inaturalist-open-data.s3.amazonaws.com/photos/71035949/original.jpg</t>
-  </si>
-  <si>
-    <t>https://inaturalist-open-data.s3.amazonaws.com/photos/94735383/original.jpg</t>
-  </si>
-  <si>
-    <t>https://geonature.arb-idf.fr/geonature/api//media/attachments/4/45328_rect989.jpg</t>
-  </si>
-  <si>
-    <t>https://inaturalist-open-data.s3.amazonaws.com/photos/219997141/original.jpg</t>
-  </si>
-  <si>
-    <t>https://geonature.arb-idf.fr/geonature/api//media/attachments/4/58517_P1662006.jpg</t>
-  </si>
-  <si>
-    <t>https://inaturalist-open-data.s3.amazonaws.com/photos/76409637/original.png</t>
-  </si>
-  <si>
-    <t>https://geonature.arb-idf.fr/geonature/api//media/attachments/4/90364_P1755582.jpg</t>
-  </si>
-  <si>
-    <t>https://inaturalist-open-data.s3.amazonaws.com/photos/80227343/original.jpg</t>
-  </si>
-  <si>
-    <t>https://inaturalist-open-data.s3.amazonaws.com/photos/101235971/original.jpeg</t>
-  </si>
-  <si>
-    <t>https://geonature.arb-idf.fr/geonature/api//media/attachments/4/89753_P1755516.jpg</t>
-  </si>
-  <si>
-    <t>https://cardobs.mnhn.fr/cardObs/photos/download/15369_15072023152500_segestria_bavarica_dorsal.jpg</t>
-  </si>
-  <si>
-    <t>https://geonature.arb-idf.fr/geonature/api//media/attachments/4/46159_P1641073.jpg</t>
-  </si>
-  <si>
-    <t>https://inaturalist-open-data.s3.amazonaws.com/photos/386064694/original.jpg</t>
-  </si>
-  <si>
-    <t>https://inaturalist-open-data.s3.amazonaws.com/photos/437207501/original.jpg</t>
-  </si>
-  <si>
-    <t>https://geonature.arb-idf.fr/geonature/api//media/attachments/4/57980_P1661182.jpg</t>
-  </si>
-  <si>
-    <t>https://geonature.arb-idf.fr/geonature/api//media/attachments/4/91698_P1789606.jpg</t>
-  </si>
-  <si>
-    <t>https://inaturalist-open-data.s3.amazonaws.com/photos/435531484/original.jpg</t>
-  </si>
-  <si>
-    <t>https://geonature.arb-idf.fr/geonature/api//media/attachments/4/57831_P1661085.jpg</t>
-  </si>
-  <si>
-    <t>https://geonature.arb-idf.fr/geonature/api//media/attachments/4/91690_P1766621.jpg</t>
-  </si>
-  <si>
-    <t>https://geonature.arb-idf.fr/geonature/api//media/attachments/4/94740_P1824494.jpg</t>
-  </si>
-  <si>
-    <t>https://geonature.arb-idf.fr/geonature/api//media/attachments/4/92844_P1766922.jpg</t>
-  </si>
-  <si>
-    <t>https://geonature.arb-idf.fr/geonature/api//media/attachments/4/83176_P1676232.jpg</t>
-  </si>
-  <si>
-    <t>https://cardobs.mnhn.fr/cardObs/photos/download/15369_24112023213836_2823_1.jpg</t>
-  </si>
-  <si>
-    <t>https://geonature.arb-idf.fr/geonature/api//media/attachments/4/83183_P1676184.jpg</t>
-  </si>
-  <si>
-    <t>https://geonature.arb-idf.fr/geonature/api//media/attachments/4/88722_P1732535.jpg</t>
-  </si>
-  <si>
-    <t>https://geonature.arb-idf.fr/geonature/api//media/attachments/4/45316_P1632114.jpg</t>
-  </si>
-  <si>
-    <t>https://inaturalist-open-data.s3.amazonaws.com/photos/435576075/original.jpg</t>
-  </si>
-  <si>
-    <t>https://geonature.arb-idf.fr/geonature/api//media/attachments/4/83252_P1676045.jpg</t>
-  </si>
-  <si>
-    <t>https://geonature.arb-idf.fr/geonature/api//media/attachments/4/45446_rect1069.jpg</t>
-  </si>
-  <si>
-    <t>https://geonature.arb-idf.fr/geonature/api//media/attachments/4/45447_image44.jpg</t>
-  </si>
-  <si>
-    <t>https://inaturalist-open-data.s3.amazonaws.com/photos/79099952/original.jpeg</t>
-  </si>
-  <si>
-    <t>https://inaturalist-open-data.s3.amazonaws.com/photos/119152183/original.jpg</t>
-  </si>
-  <si>
-    <t>https://geonature.arb-idf.fr/geonature/api//media/attachments/4/88326_P1721746.jpg</t>
-  </si>
-  <si>
-    <t>https://inaturalist-open-data.s3.amazonaws.com/photos/75357757/original.jpg</t>
-  </si>
-  <si>
-    <t>https://geonature.arb-idf.fr/geonature/api//media/attachments/4/45347_rect1045.jpg</t>
-  </si>
-  <si>
-    <t>https://geonature.arb-idf.fr/geonature/api//media/attachments/4/92388_IMG_20240707_130838.jpg</t>
-  </si>
-  <si>
-    <t>https://geonature.arb-idf.fr/geonature/api//media/attachments/4/94652_P1824522.jpg</t>
-  </si>
-  <si>
-    <t>https://inaturalist-open-data.s3.amazonaws.com/photos/79100486/original.jpeg</t>
-  </si>
-  <si>
-    <t>https://geonature.arb-idf.fr/geonature/api//media/attachments/4/85757_P1698779.jpg</t>
-  </si>
-  <si>
-    <t>https://inaturalist-open-data.s3.amazonaws.com/photos/100809677/original.jpg</t>
-  </si>
-  <si>
-    <t>https://inaturalist-open-data.s3.amazonaws.com/photos/79171443/original.jpeg</t>
-  </si>
-  <si>
-    <t>https://geonature.arb-idf.fr/geonature/api//media/attachments/4/91247_IMG_20240617_184117.jpg</t>
-  </si>
-  <si>
-    <t>https://geonature.arb-idf.fr/geonature/api//media/attachments/4/47764_photos_20220629135438.jpg</t>
-  </si>
-  <si>
-    <t>https://inaturalist-open-data.s3.amazonaws.com/photos/79458175/original.jpeg</t>
-  </si>
-  <si>
-    <t>https://inaturalist-open-data.s3.amazonaws.com/photos/118973964/original.jpg</t>
-  </si>
-  <si>
-    <t>https://geonature.arb-idf.fr/geonature/api//media/attachments/4/80593_P1662397.jpg</t>
-  </si>
-  <si>
-    <t>https://inaturalist-open-data.s3.amazonaws.com/photos/28696403/original.jpg</t>
-  </si>
-  <si>
-    <t>https://geonature.arb-idf.fr/geonature/api//media/attachments/4/49963_P1647766.jpg</t>
-  </si>
-  <si>
-    <t>https://geonature.arb-idf.fr/geonature/api//media/attachments/4/57977_P1661428.jpg</t>
-  </si>
-  <si>
-    <t>https://inaturalist-open-data.s3.amazonaws.com/photos/313425661/original.jpg</t>
-  </si>
-  <si>
-    <t>https://geonature.arb-idf.fr/geonature/api//media/attachments/4/82971_P1662881.jpg</t>
-  </si>
-  <si>
-    <t>https://geonature.arb-idf.fr/geonature/api//media/attachments/4/91063_P1767092.jpg</t>
-  </si>
-  <si>
-    <t>https://geonature.arb-idf.fr/geonature/api//media/attachments/4/45226_P1557949.jpg</t>
-  </si>
-  <si>
-    <t>https://geonature.arb-idf.fr/geonature/api//media/attachments/4/45319_P1632043.jpg</t>
-  </si>
-  <si>
-    <t>https://geonature.arb-idf.fr/geonature/api//media/attachments/4/46619_P1643636.jpg</t>
-  </si>
-  <si>
-    <t>https://geonature.arb-idf.fr/geonature/api//media/attachments/4/59005_P1662503.jpg</t>
-  </si>
-  <si>
-    <t>https://geonature.arb-idf.fr/geonature/api//media/attachments/4/92996_P1802262.jpg</t>
-  </si>
-  <si>
-    <t>https://geonature.arb-idf.fr/geonature/api//media/attachments/4/46020_P1640295.jpg</t>
-  </si>
-  <si>
-    <t>https://geonature.arb-idf.fr/geonature/api//media/attachments/4/49194_P1647080.jpg</t>
-  </si>
-  <si>
-    <t>https://geonature.arb-idf.fr/geonature/api//media/attachments/4/46609_P1642384.jpg</t>
-  </si>
-  <si>
-    <t>https://geonature.arb-idf.fr/geonature/api//media/attachments/4/58638_P1662135.jpg</t>
-  </si>
-  <si>
-    <t>https://geonature.arb-idf.fr/geonature/api//media/attachments/4/59002_P1662594.jpg</t>
-  </si>
-  <si>
-    <t>https://inaturalist-open-data.s3.amazonaws.com/photos/386090556/original.jpg</t>
-  </si>
-  <si>
-    <t>https://geonature.arb-idf.fr/geonature/api//media/attachments/4/58641_P1661888.jpg</t>
-  </si>
-  <si>
-    <t>https://geonature.arb-idf.fr/geonature/api//media/attachments/4/91054_P1766672.jpg</t>
-  </si>
-  <si>
-    <t>https://geonature.arb-idf.fr/geonature/api//media/attachments/4/46721_photos_20220510172519.jpg</t>
-  </si>
-  <si>
-    <t>https://geonature.arb-idf.fr/geonature/api//media/attachments/4/57407_P1660322_cr.jpg</t>
-  </si>
-  <si>
-    <t>https://inaturalist-open-data.s3.amazonaws.com/photos/381172122/original.jpg</t>
-  </si>
-  <si>
-    <t>https://inaturalist-open-data.s3.amazonaws.com/photos/436496224/original.jpg</t>
-  </si>
-  <si>
-    <t>https://geonature.arb-idf.fr/geonature/api//media/attachments/4/95344_P1835369.jpg</t>
-  </si>
-  <si>
-    <t>https://geonature.arb-idf.fr/geonature/api//media/attachments/4/45234_image24_03.jpg</t>
-  </si>
-  <si>
-    <t>https://geonature.arb-idf.fr/geonature/api//media/attachments/4/45260_rect82.jpg</t>
-  </si>
-  <si>
-    <t>https://geonature.arb-idf.fr/geonature/api//media/attachments/4/56820_IMG_20230221_091826.jpg</t>
-  </si>
-  <si>
-    <t>https://inaturalist-open-data.s3.amazonaws.com/photos/44094008/original.jpg</t>
-  </si>
-  <si>
-    <t>https://inaturalist-open-data.s3.amazonaws.com/photos/164944987/original.jpg</t>
-  </si>
-  <si>
     <t>www/media/araneus_diadematus.webp</t>
   </si>
   <si>
@@ -2552,6 +1991,12 @@
   </si>
   <si>
     <t>www/media/anyphaena_accentuata.webp</t>
+  </si>
+  <si>
+    <t>www/media/argiope_bruennichi.webp</t>
+  </si>
+  <si>
+    <t>www/media/cercidia_prominens.webp</t>
   </si>
 </sst>
 </file>
@@ -2615,6 +2060,18 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{5221C8D7-EF93-417B-B8B8-217FC377064B}" name="Tableau1" displayName="Tableau1" ref="A1:C656" totalsRowShown="0">
+  <autoFilter ref="A1:C656" xr:uid="{5221C8D7-EF93-417B-B8B8-217FC377064B}"/>
+  <tableColumns count="3">
+    <tableColumn id="1" xr3:uid="{8CF3FEBE-EC73-416E-8610-F705B8D6D336}" name="taxon"/>
+    <tableColumn id="2" xr3:uid="{DBDA5D0E-A4B2-4E10-A6AF-85502F963E80}" name="male"/>
+    <tableColumn id="3" xr3:uid="{84160676-7B2A-4A0C-94B1-2901F12B1A91}" name="femelle"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2936,13 +2393,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C656"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C24" sqref="C24"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="B40" sqref="B40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="21.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="40.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="43" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
@@ -2950,10 +2409,10 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>698</v>
+        <v>648</v>
       </c>
       <c r="C1" t="s">
-        <v>699</v>
+        <v>649</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
@@ -2961,16 +2420,13 @@
         <v>1</v>
       </c>
       <c r="C2" t="s">
-        <v>841</v>
+        <v>654</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>2</v>
       </c>
-      <c r="C3" t="s">
-        <v>647</v>
-      </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
@@ -3062,7 +2518,7 @@
         <v>19</v>
       </c>
       <c r="C21" t="s">
-        <v>842</v>
+        <v>655</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
@@ -3075,7 +2531,7 @@
         <v>22</v>
       </c>
       <c r="C23" t="s">
-        <v>843</v>
+        <v>656</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
@@ -3087,9 +2543,6 @@
       <c r="A25" t="s">
         <v>24</v>
       </c>
-      <c r="C25" t="s">
-        <v>648</v>
-      </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
@@ -3110,19 +2563,13 @@
       <c r="A29" t="s">
         <v>29</v>
       </c>
-      <c r="C29" t="s">
-        <v>649</v>
-      </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>30</v>
       </c>
-      <c r="B30" t="s">
-        <v>700</v>
-      </c>
       <c r="C30" t="s">
-        <v>837</v>
+        <v>650</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
@@ -3130,7 +2577,7 @@
         <v>31</v>
       </c>
       <c r="C31" t="s">
-        <v>838</v>
+        <v>651</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
@@ -3138,10 +2585,10 @@
         <v>32</v>
       </c>
       <c r="B32" t="s">
-        <v>839</v>
+        <v>652</v>
       </c>
       <c r="C32" t="s">
-        <v>840</v>
+        <v>653</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
@@ -3158,12 +2605,6 @@
       <c r="A35" t="s">
         <v>35</v>
       </c>
-      <c r="B35" t="s">
-        <v>702</v>
-      </c>
-      <c r="C35" t="s">
-        <v>701</v>
-      </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
@@ -3174,19 +2615,13 @@
       <c r="A37" t="s">
         <v>37</v>
       </c>
-      <c r="B37" t="s">
-        <v>650</v>
-      </c>
-      <c r="C37" t="s">
-        <v>703</v>
-      </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>38</v>
       </c>
       <c r="C38" t="s">
-        <v>704</v>
+        <v>657</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
@@ -3194,16 +2629,13 @@
         <v>39</v>
       </c>
       <c r="B39" t="s">
-        <v>651</v>
+        <v>658</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>40</v>
       </c>
-      <c r="C40" t="s">
-        <v>705</v>
-      </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
@@ -3219,12 +2651,6 @@
       <c r="A43" t="s">
         <v>43</v>
       </c>
-      <c r="B43" t="s">
-        <v>706</v>
-      </c>
-      <c r="C43" t="s">
-        <v>707</v>
-      </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
@@ -3251,655 +2677,563 @@
         <v>48</v>
       </c>
     </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>49</v>
       </c>
-      <c r="B49" t="s">
-        <v>708</v>
-      </c>
-      <c r="C49" t="s">
-        <v>709</v>
-      </c>
-    </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="50" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>51</v>
       </c>
-      <c r="C51" t="s">
-        <v>652</v>
-      </c>
-    </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="52" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>55</v>
       </c>
-      <c r="B55" t="s">
-        <v>710</v>
-      </c>
-      <c r="C55" t="s">
-        <v>836</v>
-      </c>
-    </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="56" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>56</v>
       </c>
-      <c r="C57" t="s">
-        <v>653</v>
-      </c>
-    </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="58" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>59</v>
       </c>
-      <c r="B60" t="s">
-        <v>711</v>
-      </c>
-      <c r="C60" t="s">
-        <v>712</v>
-      </c>
-    </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="61" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>61</v>
       </c>
-      <c r="B62" t="s">
-        <v>714</v>
-      </c>
-      <c r="C62" t="s">
-        <v>713</v>
-      </c>
-    </row>
-    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="63" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>66</v>
       </c>
-      <c r="C67" t="s">
-        <v>654</v>
-      </c>
-    </row>
-    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="68" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="69" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="70" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="71" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="72" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="73" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
         <v>70</v>
       </c>
-      <c r="C73" t="s">
-        <v>659</v>
-      </c>
-    </row>
-    <row r="74" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="74" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="75" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="76" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="77" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="78" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="79" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="80" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="81" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="82" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
         <v>79</v>
       </c>
-      <c r="B82" s="1" t="s">
-        <v>656</v>
-      </c>
-    </row>
-    <row r="83" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B82" s="1"/>
+    </row>
+    <row r="83" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
         <v>80</v>
       </c>
-      <c r="C83" t="s">
-        <v>658</v>
-      </c>
-    </row>
-    <row r="84" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="84" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="85" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="86" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="87" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="88" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="89" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
         <v>86</v>
       </c>
-      <c r="B89" t="s">
-        <v>657</v>
-      </c>
-    </row>
-    <row r="90" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="90" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="91" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="92" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
         <v>89</v>
       </c>
-      <c r="C92" t="s">
-        <v>655</v>
-      </c>
-    </row>
-    <row r="93" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="93" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="94" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="95" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="96" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="97" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="98" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
         <v>95</v>
       </c>
-      <c r="B98" t="s">
-        <v>660</v>
-      </c>
-    </row>
-    <row r="99" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="99" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="100" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="101" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
         <v>98</v>
       </c>
-      <c r="B101" t="s">
-        <v>715</v>
-      </c>
-      <c r="C101" t="s">
-        <v>661</v>
-      </c>
-    </row>
-    <row r="102" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="102" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="103" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
         <v>100</v>
       </c>
-      <c r="B103" t="s">
-        <v>662</v>
-      </c>
-    </row>
-    <row r="104" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="104" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="105" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
         <v>102</v>
       </c>
-      <c r="B105" t="s">
-        <v>664</v>
-      </c>
-      <c r="C105" t="s">
-        <v>717</v>
-      </c>
-    </row>
-    <row r="106" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="106" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="107" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
         <v>104</v>
       </c>
-      <c r="B107" t="s">
-        <v>716</v>
-      </c>
-      <c r="C107" t="s">
-        <v>663</v>
-      </c>
-    </row>
-    <row r="108" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="108" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
         <v>105</v>
       </c>
-      <c r="B108" t="s">
-        <v>719</v>
-      </c>
-      <c r="C108" t="s">
-        <v>718</v>
-      </c>
-    </row>
-    <row r="109" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="109" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="110" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="111" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
         <v>108</v>
       </c>
-      <c r="C111" t="s">
-        <v>665</v>
-      </c>
-    </row>
-    <row r="112" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="112" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="113" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
         <v>110</v>
       </c>
-      <c r="B113" t="s">
-        <v>666</v>
-      </c>
-    </row>
-    <row r="114" spans="1:2" x14ac:dyDescent="0.25">
+    </row>
+    <row r="114" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="115" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="116" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="117" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="118" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="119" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="120" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="121" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="122" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
         <v>120</v>
       </c>
     </row>
-    <row r="123" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="124" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="125" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="126" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
         <v>124</v>
       </c>
     </row>
-    <row r="127" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="128" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
         <v>126</v>
       </c>
     </row>
-    <row r="129" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
         <v>127</v>
       </c>
     </row>
-    <row r="130" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="131" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="132" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A132" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="133" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A133" t="s">
         <v>131</v>
       </c>
-      <c r="C133" t="s">
-        <v>667</v>
-      </c>
-    </row>
-    <row r="134" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="134" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A134" t="s">
         <v>132</v>
       </c>
     </row>
-    <row r="135" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A135" t="s">
         <v>133</v>
       </c>
-      <c r="C135" t="s">
-        <v>668</v>
-      </c>
-    </row>
-    <row r="136" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="136" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A136" t="s">
         <v>134</v>
       </c>
     </row>
-    <row r="137" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A137" t="s">
         <v>135</v>
       </c>
     </row>
-    <row r="138" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A138" t="s">
         <v>136</v>
       </c>
     </row>
-    <row r="139" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A139" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="140" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A140" t="s">
         <v>138</v>
       </c>
     </row>
-    <row r="141" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A141" t="s">
         <v>139</v>
       </c>
     </row>
-    <row r="142" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A142" t="s">
         <v>140</v>
       </c>
     </row>
-    <row r="143" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A143" t="s">
         <v>141</v>
       </c>
     </row>
-    <row r="144" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A144" t="s">
         <v>142</v>
       </c>
     </row>
-    <row r="145" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A145" t="s">
         <v>143</v>
       </c>
     </row>
-    <row r="146" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A146" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="147" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A147" t="s">
         <v>144</v>
       </c>
     </row>
-    <row r="148" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A148" t="s">
         <v>145</v>
       </c>
     </row>
-    <row r="149" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A149" t="s">
         <v>146</v>
       </c>
     </row>
-    <row r="150" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A150" t="s">
         <v>147</v>
       </c>
     </row>
-    <row r="151" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A151" t="s">
         <v>148</v>
       </c>
     </row>
-    <row r="152" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A152" t="s">
         <v>149</v>
       </c>
-      <c r="C152" t="s">
-        <v>669</v>
-      </c>
-    </row>
-    <row r="153" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="153" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A153" t="s">
         <v>150</v>
       </c>
     </row>
-    <row r="154" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A154" t="s">
         <v>151</v>
       </c>
     </row>
-    <row r="155" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A155" t="s">
         <v>152</v>
       </c>
     </row>
-    <row r="156" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A156" t="s">
         <v>153</v>
       </c>
     </row>
-    <row r="157" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A157" t="s">
         <v>154</v>
       </c>
     </row>
-    <row r="158" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A158" t="s">
         <v>155</v>
       </c>
     </row>
-    <row r="159" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A159" t="s">
         <v>156</v>
       </c>
     </row>
-    <row r="160" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A160" t="s">
         <v>157</v>
       </c>
@@ -4064,542 +3398,482 @@
         <v>189</v>
       </c>
     </row>
-    <row r="193" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="193" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A193" t="s">
         <v>190</v>
       </c>
     </row>
-    <row r="194" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="194" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A194" t="s">
         <v>191</v>
       </c>
     </row>
-    <row r="195" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="195" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A195" t="s">
         <v>192</v>
       </c>
     </row>
-    <row r="196" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="196" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A196" t="s">
         <v>193</v>
       </c>
     </row>
-    <row r="197" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="197" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A197" t="s">
         <v>194</v>
       </c>
     </row>
-    <row r="198" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="198" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A198" t="s">
         <v>195</v>
       </c>
     </row>
-    <row r="199" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="199" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A199" t="s">
         <v>196</v>
       </c>
-      <c r="B199" t="s">
-        <v>670</v>
-      </c>
-    </row>
-    <row r="200" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="200" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A200" t="s">
         <v>197</v>
       </c>
     </row>
-    <row r="201" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="201" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A201" t="s">
         <v>198</v>
       </c>
     </row>
-    <row r="202" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="202" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A202" t="s">
         <v>199</v>
       </c>
     </row>
-    <row r="203" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="203" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A203" t="s">
         <v>200</v>
       </c>
     </row>
-    <row r="204" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="204" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A204" t="s">
         <v>201</v>
       </c>
     </row>
-    <row r="205" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="205" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A205" t="s">
         <v>202</v>
       </c>
     </row>
-    <row r="206" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="206" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A206" t="s">
         <v>203</v>
       </c>
-      <c r="C206" t="s">
-        <v>671</v>
-      </c>
-    </row>
-    <row r="207" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="207" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A207" t="s">
         <v>204</v>
       </c>
     </row>
-    <row r="208" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="208" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A208" t="s">
         <v>205</v>
       </c>
     </row>
-    <row r="209" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="209" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A209" t="s">
         <v>206</v>
       </c>
     </row>
-    <row r="210" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="210" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A210" t="s">
         <v>207</v>
       </c>
     </row>
-    <row r="211" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="211" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A211" t="s">
         <v>208</v>
       </c>
     </row>
-    <row r="212" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="212" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A212" t="s">
         <v>209</v>
       </c>
     </row>
-    <row r="213" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="213" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A213" t="s">
         <v>210</v>
       </c>
     </row>
-    <row r="214" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="214" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A214" t="s">
         <v>211</v>
       </c>
     </row>
-    <row r="215" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="215" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A215" t="s">
         <v>212</v>
       </c>
     </row>
-    <row r="216" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="216" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A216" t="s">
         <v>213</v>
       </c>
     </row>
-    <row r="217" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="217" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A217" t="s">
         <v>214</v>
       </c>
-      <c r="B217" t="s">
-        <v>672</v>
-      </c>
-    </row>
-    <row r="218" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="218" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A218" t="s">
         <v>215</v>
       </c>
     </row>
-    <row r="219" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="219" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A219" t="s">
         <v>216</v>
       </c>
     </row>
-    <row r="220" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="220" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A220" t="s">
         <v>217</v>
       </c>
     </row>
-    <row r="221" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="221" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A221" t="s">
         <v>218</v>
       </c>
-      <c r="B221" t="s">
-        <v>673</v>
-      </c>
-      <c r="C221" t="s">
-        <v>721</v>
-      </c>
-    </row>
-    <row r="222" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="222" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A222" t="s">
         <v>219</v>
       </c>
-      <c r="B222" t="s">
-        <v>720</v>
-      </c>
-      <c r="C222" t="s">
-        <v>722</v>
-      </c>
-    </row>
-    <row r="223" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="223" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A223" t="s">
         <v>220</v>
       </c>
     </row>
-    <row r="224" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="224" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A224" t="s">
         <v>221</v>
       </c>
     </row>
-    <row r="225" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="225" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A225" t="s">
         <v>222</v>
       </c>
     </row>
-    <row r="226" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="226" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A226" t="s">
         <v>223</v>
       </c>
-      <c r="B226" t="s">
-        <v>674</v>
-      </c>
-    </row>
-    <row r="227" spans="1:2" x14ac:dyDescent="0.25">
+    </row>
+    <row r="227" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A227" t="s">
         <v>224</v>
       </c>
     </row>
-    <row r="228" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="228" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A228" t="s">
         <v>225</v>
       </c>
     </row>
-    <row r="229" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="229" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A229" t="s">
         <v>226</v>
       </c>
     </row>
-    <row r="230" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="230" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A230" t="s">
         <v>227</v>
       </c>
     </row>
-    <row r="231" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="231" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A231" t="s">
         <v>228</v>
       </c>
     </row>
-    <row r="232" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="232" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A232" t="s">
         <v>229</v>
       </c>
     </row>
-    <row r="233" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="233" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A233" t="s">
         <v>229</v>
       </c>
     </row>
-    <row r="234" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="234" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A234" t="s">
         <v>230</v>
       </c>
     </row>
-    <row r="235" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="235" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A235" t="s">
         <v>231</v>
       </c>
     </row>
-    <row r="236" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="236" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A236" t="s">
         <v>232</v>
       </c>
     </row>
-    <row r="237" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="237" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A237" t="s">
         <v>233</v>
       </c>
     </row>
-    <row r="238" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="238" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A238" t="s">
         <v>234</v>
       </c>
     </row>
-    <row r="239" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="239" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A239" t="s">
         <v>235</v>
       </c>
     </row>
-    <row r="240" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="240" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A240" t="s">
         <v>236</v>
       </c>
     </row>
-    <row r="241" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="241" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A241" t="s">
         <v>237</v>
       </c>
     </row>
-    <row r="242" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="242" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A242" t="s">
         <v>238</v>
       </c>
     </row>
-    <row r="243" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="243" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A243" t="s">
         <v>239</v>
       </c>
     </row>
-    <row r="244" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="244" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A244" t="s">
         <v>240</v>
       </c>
     </row>
-    <row r="245" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="245" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A245" t="s">
         <v>241</v>
       </c>
     </row>
-    <row r="246" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="246" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A246" t="s">
         <v>242</v>
       </c>
-      <c r="C246" t="s">
-        <v>723</v>
-      </c>
-    </row>
-    <row r="247" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="247" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A247" t="s">
         <v>243</v>
       </c>
-      <c r="B247" t="s">
-        <v>675</v>
-      </c>
-      <c r="C247" t="s">
-        <v>724</v>
-      </c>
-    </row>
-    <row r="248" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="248" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A248" t="s">
         <v>244</v>
       </c>
-      <c r="B248" t="s">
-        <v>676</v>
-      </c>
-    </row>
-    <row r="249" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="249" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A249" t="s">
         <v>245</v>
       </c>
     </row>
-    <row r="250" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="250" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A250" t="s">
         <v>246</v>
       </c>
-      <c r="B250" t="s">
-        <v>725</v>
-      </c>
-      <c r="C250" t="s">
-        <v>726</v>
-      </c>
-    </row>
-    <row r="251" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="251" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A251" t="s">
         <v>247</v>
       </c>
     </row>
-    <row r="252" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="252" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A252" t="s">
         <v>248</v>
       </c>
     </row>
-    <row r="253" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="253" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A253" t="s">
         <v>249</v>
       </c>
     </row>
-    <row r="254" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="254" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A254" t="s">
         <v>250</v>
       </c>
     </row>
-    <row r="255" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="255" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A255" t="s">
         <v>251</v>
       </c>
     </row>
-    <row r="256" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="256" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A256" t="s">
         <v>252</v>
       </c>
     </row>
-    <row r="257" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="257" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A257" t="s">
         <v>253</v>
       </c>
     </row>
-    <row r="258" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="258" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A258" t="s">
         <v>254</v>
       </c>
     </row>
-    <row r="259" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="259" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A259" t="s">
         <v>255</v>
       </c>
     </row>
-    <row r="260" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="260" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A260" t="s">
         <v>256</v>
       </c>
     </row>
-    <row r="261" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="261" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A261" t="s">
         <v>257</v>
       </c>
     </row>
-    <row r="262" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="262" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A262" t="s">
         <v>258</v>
       </c>
     </row>
-    <row r="263" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="263" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A263" t="s">
         <v>259</v>
       </c>
     </row>
-    <row r="264" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="264" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A264" t="s">
         <v>260</v>
       </c>
-      <c r="B264" t="s">
-        <v>677</v>
-      </c>
-    </row>
-    <row r="265" spans="1:2" x14ac:dyDescent="0.25">
+    </row>
+    <row r="265" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A265" t="s">
         <v>261</v>
       </c>
     </row>
-    <row r="266" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="266" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A266" t="s">
         <v>262</v>
       </c>
     </row>
-    <row r="267" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="267" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A267" t="s">
         <v>263</v>
       </c>
     </row>
-    <row r="268" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="268" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A268" t="s">
         <v>264</v>
       </c>
     </row>
-    <row r="269" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="269" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A269" t="s">
         <v>265</v>
       </c>
     </row>
-    <row r="270" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="270" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A270" t="s">
         <v>266</v>
       </c>
     </row>
-    <row r="271" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="271" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A271" t="s">
         <v>267</v>
       </c>
     </row>
-    <row r="272" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="272" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A272" t="s">
         <v>268</v>
       </c>
     </row>
-    <row r="273" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="273" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A273" t="s">
         <v>269</v>
       </c>
     </row>
-    <row r="274" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="274" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A274" t="s">
         <v>270</v>
       </c>
     </row>
-    <row r="275" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="275" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A275" t="s">
         <v>271</v>
       </c>
     </row>
-    <row r="276" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="276" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A276" t="s">
         <v>272</v>
       </c>
     </row>
-    <row r="277" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="277" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A277" t="s">
         <v>273</v>
       </c>
     </row>
-    <row r="278" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="278" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A278" t="s">
         <v>274</v>
       </c>
-      <c r="B278" t="s">
-        <v>678</v>
-      </c>
-    </row>
-    <row r="279" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="279" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A279" t="s">
         <v>275</v>
       </c>
-      <c r="C279" t="s">
-        <v>679</v>
-      </c>
-    </row>
-    <row r="280" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="280" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A280" t="s">
         <v>276</v>
       </c>
-      <c r="B280" t="s">
-        <v>728</v>
-      </c>
-      <c r="C280" t="s">
-        <v>727</v>
-      </c>
-    </row>
-    <row r="281" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="281" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A281" t="s">
         <v>277</v>
       </c>
     </row>
-    <row r="282" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="282" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A282" t="s">
         <v>278</v>
       </c>
     </row>
-    <row r="283" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="283" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A283" t="s">
         <v>279</v>
       </c>
     </row>
-    <row r="284" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="284" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A284" t="s">
         <v>280</v>
       </c>
     </row>
-    <row r="285" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="285" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A285" t="s">
         <v>281</v>
       </c>
     </row>
-    <row r="286" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="286" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A286" t="s">
         <v>282</v>
       </c>
     </row>
-    <row r="287" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="287" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A287" t="s">
         <v>283</v>
       </c>
-      <c r="C287" t="s">
-        <v>680</v>
-      </c>
-    </row>
-    <row r="288" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="288" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A288" t="s">
         <v>284</v>
       </c>
@@ -4764,91 +4038,82 @@
         <v>316</v>
       </c>
     </row>
-    <row r="321" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="321" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A321" t="s">
         <v>317</v>
       </c>
     </row>
-    <row r="322" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="322" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A322" t="s">
         <v>318</v>
       </c>
     </row>
-    <row r="323" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="323" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A323" t="s">
         <v>319</v>
       </c>
     </row>
-    <row r="324" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="324" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A324" t="s">
         <v>320</v>
       </c>
     </row>
-    <row r="325" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="325" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A325" t="s">
         <v>321</v>
       </c>
     </row>
-    <row r="326" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="326" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A326" t="s">
         <v>322</v>
       </c>
     </row>
-    <row r="327" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="327" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A327" t="s">
         <v>323</v>
       </c>
     </row>
-    <row r="328" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="328" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A328" t="s">
         <v>324</v>
       </c>
     </row>
-    <row r="329" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="329" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A329" t="s">
         <v>325</v>
       </c>
     </row>
-    <row r="330" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="330" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A330" t="s">
         <v>326</v>
       </c>
     </row>
-    <row r="331" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="331" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A331" t="s">
         <v>327</v>
       </c>
     </row>
-    <row r="332" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="332" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A332" t="s">
         <v>328</v>
       </c>
-      <c r="B332" t="s">
-        <v>729</v>
-      </c>
-      <c r="C332" t="s">
-        <v>681</v>
-      </c>
-    </row>
-    <row r="333" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="333" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A333" t="s">
         <v>327</v>
       </c>
     </row>
-    <row r="334" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="334" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A334" t="s">
         <v>329</v>
       </c>
     </row>
-    <row r="335" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="335" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A335" t="s">
-        <v>683</v>
-      </c>
-      <c r="C335" t="s">
-        <v>682</v>
-      </c>
-    </row>
-    <row r="336" spans="1:3" x14ac:dyDescent="0.25">
+        <v>647</v>
+      </c>
+    </row>
+    <row r="336" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A336" t="s">
         <v>330</v>
       </c>
@@ -5013,1588 +4278,1282 @@
         <v>360</v>
       </c>
     </row>
-    <row r="369" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="369" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A369" t="s">
         <v>361</v>
       </c>
     </row>
-    <row r="370" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="370" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A370" t="s">
         <v>362</v>
       </c>
     </row>
-    <row r="371" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="371" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A371" t="s">
         <v>363</v>
       </c>
     </row>
-    <row r="372" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="372" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A372" t="s">
         <v>364</v>
       </c>
     </row>
-    <row r="373" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="373" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A373" t="s">
         <v>365</v>
       </c>
     </row>
-    <row r="374" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="374" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A374" t="s">
         <v>366</v>
       </c>
     </row>
-    <row r="375" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="375" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A375" t="s">
         <v>367</v>
       </c>
     </row>
-    <row r="376" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="376" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A376" t="s">
         <v>368</v>
       </c>
     </row>
-    <row r="377" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="377" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A377" t="s">
         <v>369</v>
       </c>
     </row>
-    <row r="378" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="378" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A378" t="s">
         <v>370</v>
       </c>
     </row>
-    <row r="379" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="379" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A379" t="s">
         <v>371</v>
       </c>
     </row>
-    <row r="380" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="380" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A380" t="s">
         <v>372</v>
       </c>
-      <c r="B380" t="s">
-        <v>684</v>
-      </c>
-    </row>
-    <row r="381" spans="1:2" x14ac:dyDescent="0.25">
+    </row>
+    <row r="381" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A381" t="s">
         <v>373</v>
       </c>
     </row>
-    <row r="382" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="382" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A382" t="s">
         <v>374</v>
       </c>
     </row>
-    <row r="383" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="383" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A383" t="s">
         <v>375</v>
       </c>
     </row>
-    <row r="384" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="384" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A384" t="s">
         <v>376</v>
       </c>
     </row>
-    <row r="385" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="385" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A385" t="s">
         <v>377</v>
       </c>
-      <c r="B385" t="s">
-        <v>685</v>
-      </c>
-    </row>
-    <row r="386" spans="1:2" x14ac:dyDescent="0.25">
+    </row>
+    <row r="386" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A386" t="s">
         <v>378</v>
       </c>
     </row>
-    <row r="387" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="387" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A387" t="s">
         <v>379</v>
       </c>
     </row>
-    <row r="388" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="388" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A388" t="s">
         <v>380</v>
       </c>
     </row>
-    <row r="389" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="389" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A389" t="s">
         <v>381</v>
       </c>
     </row>
-    <row r="390" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="390" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A390" t="s">
         <v>382</v>
       </c>
-      <c r="B390" t="s">
-        <v>688</v>
-      </c>
-    </row>
-    <row r="391" spans="1:2" x14ac:dyDescent="0.25">
+    </row>
+    <row r="391" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A391" t="s">
         <v>383</v>
       </c>
     </row>
-    <row r="392" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="392" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A392" t="s">
         <v>384</v>
       </c>
-      <c r="B392" t="s">
-        <v>686</v>
-      </c>
-    </row>
-    <row r="393" spans="1:2" x14ac:dyDescent="0.25">
+    </row>
+    <row r="393" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A393" t="s">
         <v>385</v>
       </c>
     </row>
-    <row r="394" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="394" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A394" t="s">
         <v>386</v>
       </c>
     </row>
-    <row r="395" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="395" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A395" t="s">
         <v>387</v>
       </c>
     </row>
-    <row r="396" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="396" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A396" t="s">
         <v>388</v>
       </c>
     </row>
-    <row r="397" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="397" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A397" t="s">
         <v>389</v>
       </c>
     </row>
-    <row r="398" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="398" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A398" t="s">
         <v>390</v>
       </c>
     </row>
-    <row r="399" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="399" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A399" t="s">
         <v>391</v>
       </c>
     </row>
-    <row r="400" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="400" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A400" t="s">
         <v>392</v>
       </c>
     </row>
-    <row r="401" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="401" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A401" t="s">
         <v>393</v>
       </c>
-      <c r="B401" t="s">
-        <v>687</v>
-      </c>
-    </row>
-    <row r="402" spans="1:2" x14ac:dyDescent="0.25">
+    </row>
+    <row r="402" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A402" t="s">
         <v>394</v>
       </c>
     </row>
-    <row r="403" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="403" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A403" t="s">
         <v>395</v>
       </c>
     </row>
-    <row r="404" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="404" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A404" t="s">
         <v>396</v>
       </c>
     </row>
-    <row r="405" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="405" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A405" t="s">
         <v>397</v>
       </c>
     </row>
-    <row r="406" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="406" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A406" t="s">
         <v>398</v>
       </c>
     </row>
-    <row r="407" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="407" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A407" t="s">
         <v>399</v>
       </c>
     </row>
-    <row r="408" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="408" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A408" t="s">
         <v>400</v>
       </c>
     </row>
-    <row r="409" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="409" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A409" t="s">
         <v>401</v>
       </c>
     </row>
-    <row r="410" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="410" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A410" t="s">
         <v>402</v>
       </c>
-      <c r="B410" t="s">
-        <v>689</v>
-      </c>
-    </row>
-    <row r="411" spans="1:2" x14ac:dyDescent="0.25">
+    </row>
+    <row r="411" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A411" t="s">
         <v>403</v>
       </c>
     </row>
-    <row r="412" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="412" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A412" t="s">
         <v>404</v>
       </c>
     </row>
-    <row r="413" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="413" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A413" t="s">
         <v>405</v>
       </c>
     </row>
-    <row r="414" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="414" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A414" t="s">
         <v>406</v>
       </c>
     </row>
-    <row r="415" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="415" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A415" t="s">
         <v>407</v>
       </c>
     </row>
-    <row r="416" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="416" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A416" t="s">
         <v>408</v>
       </c>
     </row>
-    <row r="417" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="417" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A417" t="s">
         <v>409</v>
       </c>
-      <c r="C417" t="s">
-        <v>690</v>
-      </c>
-    </row>
-    <row r="418" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="418" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A418" t="s">
         <v>410</v>
       </c>
     </row>
-    <row r="419" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="419" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A419" t="s">
         <v>411</v>
       </c>
     </row>
-    <row r="420" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="420" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A420" t="s">
         <v>412</v>
       </c>
     </row>
-    <row r="421" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="421" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A421" t="s">
         <v>413</v>
       </c>
     </row>
-    <row r="422" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="422" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A422" t="s">
         <v>414</v>
       </c>
     </row>
-    <row r="423" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="423" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A423" t="s">
         <v>415</v>
       </c>
     </row>
-    <row r="424" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="424" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A424" t="s">
         <v>416</v>
       </c>
     </row>
-    <row r="425" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="425" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A425" t="s">
         <v>417</v>
       </c>
     </row>
-    <row r="426" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="426" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A426" t="s">
         <v>418</v>
       </c>
-      <c r="C426" t="s">
-        <v>691</v>
-      </c>
-    </row>
-    <row r="427" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="427" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A427" t="s">
         <v>419</v>
       </c>
     </row>
-    <row r="428" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="428" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A428" t="s">
         <v>420</v>
       </c>
     </row>
-    <row r="429" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="429" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A429" t="s">
         <v>421</v>
       </c>
     </row>
-    <row r="430" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="430" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A430" t="s">
         <v>422</v>
       </c>
     </row>
-    <row r="431" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="431" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A431" t="s">
         <v>423</v>
       </c>
     </row>
-    <row r="432" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="432" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A432" t="s">
         <v>424</v>
       </c>
     </row>
-    <row r="433" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="433" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A433" t="s">
         <v>425</v>
       </c>
     </row>
-    <row r="434" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="434" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A434" t="s">
         <v>426</v>
       </c>
-      <c r="B434" t="s">
-        <v>730</v>
-      </c>
-      <c r="C434" t="s">
-        <v>693</v>
-      </c>
-    </row>
-    <row r="435" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="435" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A435" t="s">
         <v>427</v>
       </c>
-      <c r="C435" t="s">
-        <v>731</v>
-      </c>
-    </row>
-    <row r="436" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="436" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A436" t="s">
         <v>428</v>
       </c>
-      <c r="B436" t="s">
-        <v>692</v>
-      </c>
-      <c r="C436" t="s">
-        <v>732</v>
-      </c>
-    </row>
-    <row r="437" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="437" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A437" t="s">
         <v>429</v>
       </c>
     </row>
-    <row r="438" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="438" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A438" t="s">
         <v>430</v>
       </c>
-      <c r="B438" t="s">
-        <v>734</v>
-      </c>
-      <c r="C438" t="s">
-        <v>733</v>
-      </c>
-    </row>
-    <row r="439" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="439" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A439" t="s">
         <v>431</v>
       </c>
     </row>
-    <row r="440" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="440" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A440" t="s">
         <v>432</v>
       </c>
     </row>
-    <row r="441" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="441" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A441" t="s">
         <v>431</v>
       </c>
     </row>
-    <row r="442" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="442" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A442" t="s">
         <v>433</v>
       </c>
     </row>
-    <row r="443" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="443" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A443" t="s">
         <v>434</v>
       </c>
     </row>
-    <row r="444" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="444" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A444" t="s">
         <v>435</v>
       </c>
-      <c r="B444" t="s">
-        <v>694</v>
-      </c>
-    </row>
-    <row r="445" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="445" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A445" t="s">
         <v>436</v>
       </c>
     </row>
-    <row r="446" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="446" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A446" t="s">
         <v>437</v>
       </c>
     </row>
-    <row r="447" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="447" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A447" t="s">
         <v>437</v>
       </c>
     </row>
-    <row r="448" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="448" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A448" t="s">
         <v>438</v>
       </c>
     </row>
-    <row r="449" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="449" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A449" t="s">
         <v>439</v>
       </c>
     </row>
-    <row r="450" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="450" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A450" t="s">
         <v>440</v>
       </c>
     </row>
-    <row r="451" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="451" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A451" t="s">
         <v>441</v>
       </c>
     </row>
-    <row r="452" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="452" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A452" t="s">
         <v>442</v>
       </c>
     </row>
-    <row r="453" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="453" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A453" t="s">
         <v>443</v>
       </c>
     </row>
-    <row r="454" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="454" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A454" t="s">
         <v>444</v>
       </c>
-      <c r="B454" t="s">
-        <v>695</v>
-      </c>
-    </row>
-    <row r="455" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="455" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A455" t="s">
         <v>445</v>
       </c>
-      <c r="C455" t="s">
-        <v>696</v>
-      </c>
-    </row>
-    <row r="456" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="456" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A456" t="s">
         <v>446</v>
       </c>
     </row>
-    <row r="457" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="457" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A457" t="s">
         <v>447</v>
       </c>
-      <c r="B457" t="s">
-        <v>735</v>
-      </c>
-      <c r="C457" t="s">
-        <v>736</v>
-      </c>
-    </row>
-    <row r="458" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="458" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A458" t="s">
         <v>448</v>
       </c>
-      <c r="C458" t="s">
-        <v>737</v>
-      </c>
-    </row>
-    <row r="459" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="459" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A459" t="s">
         <v>449</v>
       </c>
     </row>
-    <row r="460" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="460" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A460" t="s">
         <v>450</v>
       </c>
     </row>
-    <row r="461" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="461" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A461" t="s">
         <v>451</v>
       </c>
     </row>
-    <row r="462" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="462" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A462" t="s">
         <v>452</v>
       </c>
     </row>
-    <row r="463" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="463" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A463" t="s">
         <v>453</v>
       </c>
     </row>
-    <row r="464" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="464" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A464" t="s">
         <v>454</v>
       </c>
-      <c r="B464" t="s">
-        <v>738</v>
-      </c>
-      <c r="C464" t="s">
-        <v>697</v>
-      </c>
-    </row>
-    <row r="465" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="465" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A465" t="s">
         <v>455</v>
       </c>
     </row>
-    <row r="466" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="466" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A466" t="s">
         <v>456</v>
       </c>
     </row>
-    <row r="467" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="467" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A467" t="s">
         <v>457</v>
       </c>
     </row>
-    <row r="468" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="468" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A468" t="s">
         <v>458</v>
       </c>
     </row>
-    <row r="469" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="469" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A469" t="s">
         <v>459</v>
       </c>
-      <c r="B469" t="s">
-        <v>739</v>
-      </c>
-    </row>
-    <row r="470" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="470" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A470" t="s">
         <v>460</v>
       </c>
     </row>
-    <row r="471" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="471" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A471" t="s">
         <v>461</v>
       </c>
-      <c r="B471" t="s">
-        <v>740</v>
-      </c>
-      <c r="C471" t="s">
-        <v>741</v>
-      </c>
-    </row>
-    <row r="472" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="472" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A472" t="s">
         <v>462</v>
       </c>
     </row>
-    <row r="473" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="473" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A473" t="s">
         <v>463</v>
       </c>
-      <c r="B473" t="s">
-        <v>742</v>
-      </c>
-      <c r="C473" t="s">
-        <v>743</v>
-      </c>
-    </row>
-    <row r="474" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="474" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A474" t="s">
         <v>464</v>
       </c>
     </row>
-    <row r="475" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="475" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A475" t="s">
         <v>465</v>
       </c>
     </row>
-    <row r="476" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="476" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A476" t="s">
         <v>467</v>
       </c>
-      <c r="B476" t="s">
-        <v>744</v>
-      </c>
-    </row>
-    <row r="477" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="477" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A477" t="s">
         <v>468</v>
       </c>
-      <c r="C477" t="s">
-        <v>745</v>
-      </c>
-    </row>
-    <row r="478" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="478" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A478" t="s">
         <v>469</v>
       </c>
-      <c r="B478" t="s">
-        <v>746</v>
-      </c>
-    </row>
-    <row r="479" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="479" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A479" t="s">
         <v>470</v>
       </c>
     </row>
-    <row r="480" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="480" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A480" t="s">
         <v>471</v>
       </c>
     </row>
-    <row r="481" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="481" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A481" t="s">
         <v>472</v>
       </c>
     </row>
-    <row r="482" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="482" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A482" t="s">
         <v>473</v>
       </c>
     </row>
-    <row r="483" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="483" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A483" t="s">
         <v>474</v>
       </c>
-      <c r="C483" t="s">
-        <v>749</v>
-      </c>
-    </row>
-    <row r="484" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="484" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A484" t="s">
         <v>475</v>
       </c>
     </row>
-    <row r="485" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="485" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A485" t="s">
         <v>476</v>
       </c>
     </row>
-    <row r="486" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="486" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A486" t="s">
         <v>477</v>
       </c>
-      <c r="B486" t="s">
-        <v>747</v>
-      </c>
-      <c r="C486" t="s">
-        <v>748</v>
-      </c>
-    </row>
-    <row r="487" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="487" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A487" t="s">
         <v>478</v>
       </c>
-      <c r="B487" t="s">
-        <v>751</v>
-      </c>
-      <c r="C487" t="s">
-        <v>750</v>
-      </c>
-    </row>
-    <row r="488" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="488" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A488" t="s">
         <v>479</v>
       </c>
     </row>
-    <row r="489" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="489" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A489" t="s">
         <v>466</v>
       </c>
-      <c r="B489" t="s">
-        <v>752</v>
-      </c>
-      <c r="C489" t="s">
-        <v>753</v>
-      </c>
-    </row>
-    <row r="490" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="490" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A490" t="s">
         <v>480</v>
       </c>
-      <c r="B490" t="s">
-        <v>755</v>
-      </c>
-      <c r="C490" t="s">
-        <v>754</v>
-      </c>
-    </row>
-    <row r="491" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="491" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A491" t="s">
         <v>481</v>
       </c>
     </row>
-    <row r="492" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="492" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A492" t="s">
         <v>482</v>
       </c>
     </row>
-    <row r="493" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="493" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A493" t="s">
         <v>483</v>
       </c>
     </row>
-    <row r="494" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="494" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A494" t="s">
         <v>484</v>
       </c>
     </row>
-    <row r="495" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="495" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A495" t="s">
         <v>485</v>
       </c>
     </row>
-    <row r="496" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="496" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A496" t="s">
         <v>486</v>
       </c>
     </row>
-    <row r="497" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="497" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A497" t="s">
         <v>487</v>
       </c>
     </row>
-    <row r="498" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="498" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A498" t="s">
         <v>488</v>
       </c>
     </row>
-    <row r="499" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="499" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A499" t="s">
         <v>489</v>
       </c>
     </row>
-    <row r="500" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="500" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A500" t="s">
         <v>490</v>
       </c>
     </row>
-    <row r="501" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="501" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A501" t="s">
         <v>491</v>
       </c>
     </row>
-    <row r="502" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="502" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A502" t="s">
         <v>492</v>
       </c>
     </row>
-    <row r="503" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="503" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A503" t="s">
         <v>493</v>
       </c>
     </row>
-    <row r="504" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="504" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A504" t="s">
         <v>494</v>
       </c>
-      <c r="C504" t="s">
-        <v>756</v>
-      </c>
-    </row>
-    <row r="505" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="505" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A505" t="s">
         <v>495</v>
       </c>
     </row>
-    <row r="506" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="506" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A506" t="s">
         <v>496</v>
       </c>
-      <c r="B506" t="s">
-        <v>760</v>
-      </c>
-      <c r="C506" t="s">
-        <v>759</v>
-      </c>
-    </row>
-    <row r="507" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="507" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A507" t="s">
         <v>497</v>
       </c>
-      <c r="B507" t="s">
-        <v>757</v>
-      </c>
-      <c r="C507" t="s">
-        <v>758</v>
-      </c>
-    </row>
-    <row r="508" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="508" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A508" t="s">
         <v>498</v>
       </c>
     </row>
-    <row r="509" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="509" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A509" t="s">
         <v>499</v>
       </c>
-      <c r="B509" t="s">
-        <v>761</v>
-      </c>
-      <c r="C509" t="s">
-        <v>762</v>
-      </c>
-    </row>
-    <row r="510" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="510" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A510" t="s">
         <v>500</v>
       </c>
-      <c r="C510" t="s">
-        <v>763</v>
-      </c>
-    </row>
-    <row r="511" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="511" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A511" t="s">
         <v>501</v>
       </c>
     </row>
-    <row r="512" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="512" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A512" t="s">
         <v>502</v>
       </c>
-      <c r="C512" t="s">
-        <v>764</v>
-      </c>
-    </row>
-    <row r="513" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="513" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A513" t="s">
         <v>503</v>
       </c>
-      <c r="B513" t="s">
-        <v>766</v>
-      </c>
-      <c r="C513" t="s">
-        <v>765</v>
-      </c>
-    </row>
-    <row r="514" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="514" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A514" t="s">
         <v>504</v>
       </c>
-      <c r="B514" t="s">
-        <v>768</v>
-      </c>
-      <c r="C514" t="s">
-        <v>767</v>
-      </c>
-    </row>
-    <row r="515" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="515" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A515" t="s">
         <v>505</v>
       </c>
     </row>
-    <row r="516" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="516" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A516" t="s">
         <v>506</v>
       </c>
     </row>
-    <row r="517" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="517" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A517" t="s">
         <v>507</v>
       </c>
     </row>
-    <row r="518" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="518" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A518" t="s">
         <v>508</v>
       </c>
     </row>
-    <row r="519" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="519" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A519" t="s">
         <v>509</v>
       </c>
     </row>
-    <row r="520" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="520" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A520" t="s">
         <v>510</v>
       </c>
     </row>
-    <row r="521" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="521" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A521" t="s">
         <v>511</v>
       </c>
     </row>
-    <row r="522" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="522" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A522" t="s">
         <v>512</v>
       </c>
     </row>
-    <row r="523" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="523" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A523" t="s">
         <v>513</v>
       </c>
-      <c r="C523" t="s">
-        <v>769</v>
-      </c>
-    </row>
-    <row r="524" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="524" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A524" t="s">
         <v>514</v>
       </c>
-      <c r="C524" t="s">
-        <v>772</v>
-      </c>
-    </row>
-    <row r="525" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="525" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A525" t="s">
         <v>516</v>
       </c>
-      <c r="B525" t="s">
-        <v>770</v>
-      </c>
-      <c r="C525" t="s">
-        <v>771</v>
-      </c>
-    </row>
-    <row r="526" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="526" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A526" t="s">
         <v>515</v>
       </c>
     </row>
-    <row r="527" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="527" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A527" t="s">
         <v>517</v>
       </c>
     </row>
-    <row r="528" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="528" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A528" t="s">
         <v>518</v>
       </c>
     </row>
-    <row r="529" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="529" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A529" t="s">
         <v>519</v>
       </c>
     </row>
-    <row r="530" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="530" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A530" t="s">
         <v>520</v>
       </c>
     </row>
-    <row r="531" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="531" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A531" t="s">
         <v>521</v>
       </c>
     </row>
-    <row r="532" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="532" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A532" t="s">
         <v>522</v>
       </c>
-      <c r="B532" t="s">
-        <v>773</v>
-      </c>
-      <c r="C532" t="s">
-        <v>774</v>
-      </c>
-    </row>
-    <row r="533" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="533" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A533" t="s">
         <v>524</v>
       </c>
-      <c r="C533" t="s">
-        <v>775</v>
-      </c>
-    </row>
-    <row r="534" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="534" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A534" t="s">
         <v>523</v>
       </c>
     </row>
-    <row r="535" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="535" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A535" t="s">
         <v>525</v>
       </c>
     </row>
-    <row r="536" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="536" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A536" t="s">
         <v>526</v>
       </c>
-      <c r="B536" t="s">
-        <v>776</v>
-      </c>
-    </row>
-    <row r="537" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="537" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A537" t="s">
         <v>527</v>
       </c>
     </row>
-    <row r="538" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="538" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A538" t="s">
         <v>528</v>
       </c>
-      <c r="C538" t="s">
-        <v>781</v>
-      </c>
-    </row>
-    <row r="539" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="539" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A539" t="s">
         <v>529</v>
       </c>
-      <c r="B539" t="s">
-        <v>778</v>
-      </c>
-      <c r="C539" t="s">
-        <v>779</v>
-      </c>
-    </row>
-    <row r="540" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="540" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A540" t="s">
         <v>530</v>
       </c>
-      <c r="B540" t="s">
-        <v>777</v>
-      </c>
-      <c r="C540" t="s">
-        <v>780</v>
-      </c>
-    </row>
-    <row r="541" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="541" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A541" t="s">
         <v>531</v>
       </c>
     </row>
-    <row r="542" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="542" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A542" t="s">
         <v>532</v>
       </c>
     </row>
-    <row r="543" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="543" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A543" t="s">
         <v>533</v>
       </c>
     </row>
-    <row r="544" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="544" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A544" t="s">
         <v>534</v>
       </c>
     </row>
-    <row r="545" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="545" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A545" t="s">
         <v>535</v>
       </c>
     </row>
-    <row r="546" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="546" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A546" t="s">
         <v>536</v>
       </c>
     </row>
-    <row r="547" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="547" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A547" t="s">
         <v>537</v>
       </c>
     </row>
-    <row r="548" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="548" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A548" t="s">
         <v>538</v>
       </c>
     </row>
-    <row r="549" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="549" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A549" t="s">
         <v>539</v>
       </c>
     </row>
-    <row r="550" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="550" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A550" t="s">
         <v>540</v>
       </c>
     </row>
-    <row r="551" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="551" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A551" t="s">
         <v>541</v>
       </c>
     </row>
-    <row r="552" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="552" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A552" t="s">
         <v>542</v>
       </c>
-      <c r="C552" t="s">
-        <v>782</v>
-      </c>
-    </row>
-    <row r="553" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="553" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A553" t="s">
         <v>543</v>
       </c>
     </row>
-    <row r="554" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="554" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A554" t="s">
         <v>544</v>
       </c>
     </row>
-    <row r="555" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="555" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A555" t="s">
         <v>545</v>
       </c>
     </row>
-    <row r="556" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="556" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A556" t="s">
         <v>546</v>
       </c>
-      <c r="C556" t="s">
-        <v>784</v>
-      </c>
-    </row>
-    <row r="557" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="557" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A557" t="s">
         <v>548</v>
       </c>
     </row>
-    <row r="558" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="558" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A558" t="s">
         <v>549</v>
       </c>
     </row>
-    <row r="559" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="559" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A559" t="s">
         <v>547</v>
       </c>
-      <c r="B559" t="s">
-        <v>783</v>
-      </c>
-      <c r="C559" t="s">
-        <v>785</v>
-      </c>
-    </row>
-    <row r="560" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="560" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A560" t="s">
         <v>550</v>
       </c>
     </row>
-    <row r="561" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="561" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A561" t="s">
         <v>551</v>
       </c>
     </row>
-    <row r="562" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="562" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A562" t="s">
         <v>552</v>
       </c>
     </row>
-    <row r="563" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="563" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A563" t="s">
         <v>553</v>
       </c>
-      <c r="B563" t="s">
-        <v>787</v>
-      </c>
-      <c r="C563" t="s">
-        <v>786</v>
-      </c>
-    </row>
-    <row r="564" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="564" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A564" t="s">
         <v>554</v>
       </c>
-      <c r="B564" t="s">
-        <v>788</v>
-      </c>
-    </row>
-    <row r="565" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="565" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A565" t="s">
         <v>555</v>
       </c>
-      <c r="B565" t="s">
-        <v>789</v>
-      </c>
-    </row>
-    <row r="566" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="566" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A566" t="s">
         <v>556</v>
       </c>
     </row>
-    <row r="567" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="567" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A567" t="s">
         <v>557</v>
       </c>
     </row>
-    <row r="568" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="568" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A568" t="s">
         <v>558</v>
       </c>
-      <c r="B568" t="s">
-        <v>791</v>
-      </c>
-      <c r="C568" t="s">
-        <v>790</v>
-      </c>
-    </row>
-    <row r="569" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="569" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A569" t="s">
         <v>559</v>
       </c>
     </row>
-    <row r="570" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="570" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A570" t="s">
         <v>560</v>
       </c>
     </row>
-    <row r="571" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="571" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A571" t="s">
         <v>561</v>
       </c>
-      <c r="B571" t="s">
-        <v>792</v>
-      </c>
-      <c r="C571" t="s">
-        <v>793</v>
-      </c>
-    </row>
-    <row r="572" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="572" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A572" t="s">
         <v>562</v>
       </c>
     </row>
-    <row r="573" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="573" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A573" t="s">
         <v>563</v>
       </c>
     </row>
-    <row r="574" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="574" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A574" t="s">
         <v>564</v>
       </c>
     </row>
-    <row r="575" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="575" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A575" t="s">
         <v>565</v>
       </c>
-      <c r="B575" t="s">
-        <v>794</v>
-      </c>
-      <c r="C575" t="s">
-        <v>795</v>
-      </c>
-    </row>
-    <row r="576" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="576" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A576" t="s">
         <v>566</v>
       </c>
     </row>
-    <row r="577" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="577" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A577" t="s">
         <v>567</v>
       </c>
-      <c r="C577" t="s">
-        <v>796</v>
-      </c>
-    </row>
-    <row r="578" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="578" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A578" t="s">
         <v>568</v>
       </c>
     </row>
-    <row r="579" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="579" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A579" t="s">
         <v>569</v>
       </c>
     </row>
-    <row r="580" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="580" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A580" t="s">
         <v>570</v>
       </c>
     </row>
-    <row r="581" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="581" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A581" t="s">
         <v>571</v>
       </c>
-      <c r="C581" t="s">
-        <v>797</v>
-      </c>
-    </row>
-    <row r="582" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="582" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A582" t="s">
         <v>572</v>
       </c>
     </row>
-    <row r="583" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="583" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A583" t="s">
         <v>573</v>
       </c>
-      <c r="C583" t="s">
-        <v>798</v>
-      </c>
-    </row>
-    <row r="584" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="584" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A584" t="s">
         <v>574</v>
       </c>
     </row>
-    <row r="585" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="585" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A585" t="s">
         <v>575</v>
       </c>
     </row>
-    <row r="586" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="586" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A586" t="s">
         <v>576</v>
       </c>
     </row>
-    <row r="587" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="587" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A587" t="s">
         <v>577</v>
       </c>
     </row>
-    <row r="588" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="588" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A588" t="s">
         <v>578</v>
       </c>
     </row>
-    <row r="589" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="589" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A589" t="s">
         <v>579</v>
       </c>
-      <c r="B589" t="s">
-        <v>800</v>
-      </c>
-      <c r="C589" t="s">
-        <v>799</v>
-      </c>
-    </row>
-    <row r="590" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="590" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A590" t="s">
         <v>580</v>
       </c>
     </row>
-    <row r="591" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="591" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A591" t="s">
         <v>581</v>
       </c>
     </row>
-    <row r="592" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="592" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A592" t="s">
         <v>582</v>
       </c>
     </row>
-    <row r="593" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="593" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A593" t="s">
         <v>583</v>
       </c>
-      <c r="B593" t="s">
-        <v>802</v>
-      </c>
-      <c r="C593" t="s">
-        <v>804</v>
-      </c>
-    </row>
-    <row r="594" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="594" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A594" t="s">
         <v>584</v>
       </c>
-      <c r="B594" t="s">
-        <v>801</v>
-      </c>
-      <c r="C594" t="s">
-        <v>803</v>
-      </c>
-    </row>
-    <row r="595" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="595" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A595" t="s">
         <v>585</v>
       </c>
     </row>
-    <row r="596" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="596" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A596" t="s">
         <v>586</v>
       </c>
-      <c r="C596" t="s">
-        <v>805</v>
-      </c>
-    </row>
-    <row r="597" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="597" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A597" t="s">
         <v>587</v>
       </c>
     </row>
-    <row r="598" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="598" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A598" t="s">
         <v>588</v>
       </c>
     </row>
-    <row r="599" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="599" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A599" t="s">
         <v>589</v>
       </c>
     </row>
-    <row r="600" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="600" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A600" t="s">
         <v>590</v>
       </c>
     </row>
-    <row r="601" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="601" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A601" t="s">
         <v>591</v>
       </c>
-      <c r="C601" t="s">
-        <v>806</v>
-      </c>
-    </row>
-    <row r="602" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="602" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A602" t="s">
         <v>592</v>
       </c>
-      <c r="B602" t="s">
-        <v>807</v>
-      </c>
-    </row>
-    <row r="603" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="603" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A603" t="s">
         <v>593</v>
       </c>
     </row>
-    <row r="604" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="604" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A604" t="s">
         <v>594</v>
       </c>
     </row>
-    <row r="605" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="605" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A605" t="s">
         <v>595</v>
       </c>
     </row>
-    <row r="606" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="606" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A606" t="s">
         <v>596</v>
       </c>
     </row>
-    <row r="607" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="607" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A607" t="s">
         <v>597</v>
       </c>
     </row>
-    <row r="608" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="608" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A608" t="s">
         <v>598</v>
       </c>
     </row>
-    <row r="609" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="609" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A609" t="s">
         <v>599</v>
       </c>
     </row>
-    <row r="610" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="610" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A610" t="s">
         <v>600</v>
       </c>
-      <c r="B610" t="s">
-        <v>808</v>
-      </c>
-      <c r="C610" t="s">
-        <v>809</v>
-      </c>
-    </row>
-    <row r="611" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="611" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A611" t="s">
         <v>601</v>
       </c>
     </row>
-    <row r="612" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="612" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A612" t="s">
         <v>602</v>
       </c>
-      <c r="B612" t="s">
-        <v>810</v>
-      </c>
-      <c r="C612" t="s">
-        <v>811</v>
-      </c>
-    </row>
-    <row r="613" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="613" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A613" t="s">
         <v>603</v>
       </c>
     </row>
-    <row r="614" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="614" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A614" t="s">
         <v>604</v>
       </c>
     </row>
-    <row r="615" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="615" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A615" t="s">
         <v>605</v>
       </c>
-      <c r="B615" t="s">
-        <v>812</v>
-      </c>
-      <c r="C615" t="s">
-        <v>813</v>
-      </c>
-    </row>
-    <row r="616" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="616" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A616" t="s">
         <v>606</v>
       </c>
     </row>
-    <row r="617" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="617" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A617" t="s">
         <v>607</v>
       </c>
     </row>
-    <row r="618" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="618" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A618" t="s">
         <v>608</v>
       </c>
-      <c r="B618" t="s">
-        <v>816</v>
-      </c>
-    </row>
-    <row r="619" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="619" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A619" t="s">
         <v>609</v>
       </c>
-      <c r="B619" t="s">
-        <v>815</v>
-      </c>
-      <c r="C619" t="s">
-        <v>814</v>
-      </c>
-    </row>
-    <row r="620" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="620" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A620" t="s">
         <v>610</v>
       </c>
     </row>
-    <row r="621" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="621" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A621" t="s">
         <v>611</v>
       </c>
     </row>
-    <row r="622" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="622" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A622" t="s">
         <v>612</v>
       </c>
     </row>
-    <row r="623" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="623" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A623" t="s">
         <v>613</v>
       </c>
-      <c r="B623" t="s">
-        <v>817</v>
-      </c>
-    </row>
-    <row r="624" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="624" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A624" t="s">
         <v>614</v>
       </c>
@@ -6608,20 +5567,11 @@
       <c r="A626" t="s">
         <v>616</v>
       </c>
-      <c r="C626" t="s">
-        <v>818</v>
-      </c>
     </row>
     <row r="627" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A627" t="s">
         <v>617</v>
       </c>
-      <c r="B627" t="s">
-        <v>819</v>
-      </c>
-      <c r="C627" t="s">
-        <v>820</v>
-      </c>
     </row>
     <row r="628" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A628" t="s">
@@ -6632,9 +5582,6 @@
       <c r="A629" t="s">
         <v>619</v>
       </c>
-      <c r="B629" t="s">
-        <v>821</v>
-      </c>
     </row>
     <row r="630" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A630" t="s">
@@ -6645,12 +5592,6 @@
       <c r="A631" t="s">
         <v>621</v>
       </c>
-      <c r="B631" t="s">
-        <v>824</v>
-      </c>
-      <c r="C631" t="s">
-        <v>829</v>
-      </c>
     </row>
     <row r="632" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A632" t="s">
@@ -6676,9 +5617,6 @@
       <c r="A636" t="s">
         <v>626</v>
       </c>
-      <c r="C636" t="s">
-        <v>830</v>
-      </c>
     </row>
     <row r="637" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A637" t="s">
@@ -6694,132 +5632,99 @@
       <c r="A639" t="s">
         <v>629</v>
       </c>
-      <c r="B639" t="s">
-        <v>825</v>
-      </c>
     </row>
     <row r="640" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A640" t="s">
         <v>630</v>
       </c>
-      <c r="B640" t="s">
-        <v>822</v>
-      </c>
-      <c r="C640" s="1" t="s">
-        <v>827</v>
-      </c>
-    </row>
-    <row r="641" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C640" s="1"/>
+    </row>
+    <row r="641" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A641" t="s">
         <v>631</v>
       </c>
-      <c r="C641" t="s">
-        <v>828</v>
-      </c>
-    </row>
-    <row r="642" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="642" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A642" t="s">
         <v>632</v>
       </c>
     </row>
-    <row r="643" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="643" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A643" t="s">
         <v>633</v>
       </c>
-      <c r="B643" t="s">
-        <v>823</v>
-      </c>
-    </row>
-    <row r="644" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="644" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A644" t="s">
         <v>634</v>
       </c>
     </row>
-    <row r="645" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="645" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A645" t="s">
         <v>635</v>
       </c>
     </row>
-    <row r="646" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="646" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A646" t="s">
         <v>636</v>
       </c>
-      <c r="C646" t="s">
-        <v>826</v>
-      </c>
-    </row>
-    <row r="647" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="647" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A647" t="s">
         <v>637</v>
       </c>
     </row>
-    <row r="648" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="648" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A648" t="s">
         <v>638</v>
       </c>
     </row>
-    <row r="649" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="649" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A649" t="s">
         <v>639</v>
       </c>
     </row>
-    <row r="650" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="650" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A650" t="s">
         <v>640</v>
       </c>
-      <c r="C650" t="s">
-        <v>831</v>
-      </c>
-    </row>
-    <row r="651" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="651" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A651" t="s">
         <v>641</v>
       </c>
     </row>
-    <row r="652" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="652" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A652" t="s">
         <v>642</v>
       </c>
     </row>
-    <row r="653" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="653" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A653" t="s">
         <v>643</v>
       </c>
     </row>
-    <row r="654" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="654" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A654" t="s">
         <v>644</v>
       </c>
-      <c r="B654" t="s">
-        <v>833</v>
-      </c>
-      <c r="C654" t="s">
-        <v>832</v>
-      </c>
-    </row>
-    <row r="655" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="655" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A655" t="s">
         <v>645</v>
       </c>
     </row>
-    <row r="656" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="656" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A656" t="s">
         <v>646</v>
       </c>
-      <c r="B656" t="s">
-        <v>834</v>
-      </c>
-      <c r="C656" t="s">
-        <v>835</v>
-      </c>
     </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="B82" r:id="rId1" xr:uid="{90A7AB64-9086-49EB-9ED9-D71B18321B6C}"/>
-    <hyperlink ref="C640" r:id="rId2" xr:uid="{47C200D2-424A-47F6-9C2D-7CB05DF18E8F}"/>
-  </hyperlinks>
   <printOptions gridLines="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+  <tableParts count="1">
+    <tablePart r:id="rId2"/>
+  </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
add 5 species with commented pictures
</commit_message>
<xml_diff>
--- a/photos.xlsx
+++ b/photos.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cedri\Documents\web\araignees_idf\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{145E0451-82A3-42C8-B961-9E743842C836}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C585311E-7B67-4A91-84AE-5B9E34BE0A09}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-105" yWindow="0" windowWidth="19410" windowHeight="15585" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="667" uniqueCount="659">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="672" uniqueCount="664">
   <si>
     <t>taxon</t>
   </si>
@@ -1997,6 +1997,21 @@
   </si>
   <si>
     <t>www/media/cercidia_prominens.webp</t>
+  </si>
+  <si>
+    <t>www/media/cyclosa_conica.webp</t>
+  </si>
+  <si>
+    <t>www/media/gibbaranea_gibbosa.webp</t>
+  </si>
+  <si>
+    <t>www/media/larinioides_cornutus.webp</t>
+  </si>
+  <si>
+    <t>www/media/larinioides_sclopetarius.webp</t>
+  </si>
+  <si>
+    <t>www/media/mangora_acalypha.webp</t>
   </si>
 </sst>
 </file>
@@ -2393,8 +2408,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C656"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="B40" sqref="B40"/>
+    <sheetView tabSelected="1" topLeftCell="A24" workbookViewId="0">
+      <selection activeCell="C55" sqref="C55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2636,6 +2651,9 @@
       <c r="A40" t="s">
         <v>40</v>
       </c>
+      <c r="C40" t="s">
+        <v>659</v>
+      </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
@@ -2651,6 +2669,9 @@
       <c r="A43" t="s">
         <v>43</v>
       </c>
+      <c r="C43" t="s">
+        <v>660</v>
+      </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
@@ -2677,82 +2698,91 @@
         <v>48</v>
       </c>
     </row>
-    <row r="49" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="50" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="C49" t="s">
+        <v>661</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="51" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="52" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="C51" t="s">
+        <v>662</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="53" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="54" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="55" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="56" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="C55" t="s">
+        <v>663</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="57" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="58" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="59" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="60" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="61" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="62" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="63" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="64" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>63</v>
       </c>

</xml_diff>

<commit_message>
remove pictures from INPN
</commit_message>
<xml_diff>
--- a/photos.xlsx
+++ b/photos.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cedri\Documents\web\araignees_idf\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E631A780-6D95-4F64-8369-C1AAFEADF7DE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{82293FEC-2514-439B-91F0-29DF54609B8C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1391" uniqueCount="739">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1361" uniqueCount="709">
   <si>
     <t>taxon</t>
   </si>
@@ -2148,96 +2148,6 @@
   </si>
   <si>
     <t>www/media/fiches/ballus_chalybeius_male.webp</t>
-  </si>
-  <si>
-    <t>https://inpn.mnhn.fr/photos/uploads/webtofs/inpn/8/122548.jpg</t>
-  </si>
-  <si>
-    <t>https://inpn.mnhn.fr/photos/uploads/webtofs/inpn/7/322667.jpg</t>
-  </si>
-  <si>
-    <t>https://inpn.mnhn.fr/photos/uploads/webtofs/inpn/7/378147.jpg</t>
-  </si>
-  <si>
-    <t>https://inpn.mnhn.fr/photos/uploads/webtofs/inpn/6/431746.jpg</t>
-  </si>
-  <si>
-    <t>https://inpn.mnhn.fr/photos/uploads/webtofs/inpn/9/210319.jpg</t>
-  </si>
-  <si>
-    <t>https://inpn.mnhn.fr/photos/uploads/webtofs/inpn/9/322729.jpg</t>
-  </si>
-  <si>
-    <t>https://inpn.mnhn.fr/photos/uploads/webtofs/inpn/5/334975.jpg</t>
-  </si>
-  <si>
-    <t>https://inpn.mnhn.fr/photos/uploads/webtofs/inpn/5/443635.jpg</t>
-  </si>
-  <si>
-    <t>https://inpn.mnhn.fr/photos/uploads/webtofs/inpn/2/169872.jpg</t>
-  </si>
-  <si>
-    <t>https://inpn.mnhn.fr/photos/uploads/webtofs/inpn/6/423276.jpg</t>
-  </si>
-  <si>
-    <t>https://inpn.mnhn.fr/photos/uploads/webtofs/inpn/ant/96649.jpg</t>
-  </si>
-  <si>
-    <t>https://inpn.mnhn.fr/photos/uploads/webtofs/inpn/ant/96651.jpg</t>
-  </si>
-  <si>
-    <t>https://inpn.mnhn.fr/photos/uploads/webtofs/inpn/0/212190.jpg</t>
-  </si>
-  <si>
-    <t>https://inpn.mnhn.fr/photos/uploads/webtofs/inpn/1/212191.jpg</t>
-  </si>
-  <si>
-    <t>https://inpn.mnhn.fr/photos/uploads/webtofs/inpn/6/122546.jpg</t>
-  </si>
-  <si>
-    <t>https://inpn.mnhn.fr/photos/uploads/webtofs/inpn/ant/96748.jpg</t>
-  </si>
-  <si>
-    <t>https://inpn.mnhn.fr/photos/uploads/webtofs/inpn/7/170187.jpg</t>
-  </si>
-  <si>
-    <t>https://inpn.mnhn.fr/photos/uploads/webtofs/inpn/3/122613.jpg</t>
-  </si>
-  <si>
-    <t>https://inpn.mnhn.fr/photos/uploads/webtofs/inpn/6/122526.jpg</t>
-  </si>
-  <si>
-    <t>https://inpn.mnhn.fr/photos/uploads/webtofs/inpn/1/423291.jpg</t>
-  </si>
-  <si>
-    <t>https://inpn.mnhn.fr/photos/uploads/webtofs/inpn/ant/96865.jpg</t>
-  </si>
-  <si>
-    <t>https://inpn.mnhn.fr/photos/uploads/webtofs/inpn/ant/96870.jpg</t>
-  </si>
-  <si>
-    <t>https://inpn.mnhn.fr/photos/uploads/webtofs/inpn/4/322774.jpg</t>
-  </si>
-  <si>
-    <t>https://inpn.mnhn.fr/photos/uploads/webtofs/inpn/0/415110.jpg</t>
-  </si>
-  <si>
-    <t>https://inpn.mnhn.fr/photos/uploads/webtofs/inpn/1/378201.jpg</t>
-  </si>
-  <si>
-    <t>https://inpn.mnhn.fr/photos/uploads/webtofs/inpn/2/378202.jpg</t>
-  </si>
-  <si>
-    <t>https://inpn.mnhn.fr/photos/uploads/webtofs/inpn/4/122584.jpg</t>
-  </si>
-  <si>
-    <t>https://inpn.mnhn.fr/photos/uploads/webtofs/inpn/1/378221.jpg</t>
-  </si>
-  <si>
-    <t>https://inpn.mnhn.fr/photos/uploads/webtofs/inpn/8/400418.jpg</t>
-  </si>
-  <si>
-    <t>https://inpn.mnhn.fr/photos/uploads/webtofs/inpn/0/322690.jpg</t>
   </si>
 </sst>
 </file>
@@ -2649,8 +2559,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D656"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
-      <selection activeCell="C64" sqref="C64"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D28" sqref="D28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2685,9 +2595,6 @@
       <c r="C2" t="s">
         <v>678</v>
       </c>
-      <c r="D2" t="s">
-        <v>709</v>
-      </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
@@ -2696,12 +2603,6 @@
       <c r="B3" t="s">
         <v>659</v>
       </c>
-      <c r="C3" t="s">
-        <v>711</v>
-      </c>
-      <c r="D3" t="s">
-        <v>710</v>
-      </c>
     </row>
     <row r="4" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
@@ -2798,9 +2699,6 @@
       <c r="B15" t="s">
         <v>659</v>
       </c>
-      <c r="C15" t="s">
-        <v>712</v>
-      </c>
     </row>
     <row r="16" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
@@ -2825,12 +2723,6 @@
       <c r="B18" t="s">
         <v>659</v>
       </c>
-      <c r="C18" t="s">
-        <v>713</v>
-      </c>
-      <c r="D18" t="s">
-        <v>714</v>
-      </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
@@ -2839,9 +2731,6 @@
       <c r="B19" t="s">
         <v>661</v>
       </c>
-      <c r="C19" t="s">
-        <v>715</v>
-      </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
@@ -2850,12 +2739,6 @@
       <c r="B20" t="s">
         <v>659</v>
       </c>
-      <c r="C20" t="s">
-        <v>716</v>
-      </c>
-      <c r="D20" t="s">
-        <v>717</v>
-      </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
@@ -2867,9 +2750,6 @@
       <c r="C21" t="s">
         <v>679</v>
       </c>
-      <c r="D21" t="s">
-        <v>718</v>
-      </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
@@ -2878,9 +2758,6 @@
       <c r="B22" t="s">
         <v>659</v>
       </c>
-      <c r="C22" t="s">
-        <v>719</v>
-      </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
@@ -2892,9 +2769,6 @@
       <c r="C23" t="s">
         <v>680</v>
       </c>
-      <c r="D23" t="s">
-        <v>720</v>
-      </c>
     </row>
     <row r="24" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
@@ -2919,12 +2793,6 @@
       <c r="B26" t="s">
         <v>659</v>
       </c>
-      <c r="C26" t="s">
-        <v>721</v>
-      </c>
-      <c r="D26" t="s">
-        <v>722</v>
-      </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
@@ -2933,9 +2801,6 @@
       <c r="B27" t="s">
         <v>659</v>
       </c>
-      <c r="C27" t="s">
-        <v>723</v>
-      </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
@@ -2944,9 +2809,6 @@
       <c r="B28" t="s">
         <v>659</v>
       </c>
-      <c r="C28" t="s">
-        <v>724</v>
-      </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
@@ -2955,12 +2817,6 @@
       <c r="B29" t="s">
         <v>659</v>
       </c>
-      <c r="C29" t="s">
-        <v>725</v>
-      </c>
-      <c r="D29" t="s">
-        <v>726</v>
-      </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
@@ -2972,9 +2828,6 @@
       <c r="C30" t="s">
         <v>681</v>
       </c>
-      <c r="D30" t="s">
-        <v>727</v>
-      </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
@@ -3051,9 +2904,6 @@
       <c r="C38" t="s">
         <v>683</v>
       </c>
-      <c r="D38" t="s">
-        <v>728</v>
-      </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
@@ -3062,9 +2912,6 @@
       <c r="B39" t="s">
         <v>659</v>
       </c>
-      <c r="C39" t="s">
-        <v>729</v>
-      </c>
       <c r="D39" t="s">
         <v>684</v>
       </c>
@@ -3087,9 +2934,6 @@
       <c r="B41" t="s">
         <v>659</v>
       </c>
-      <c r="C41" t="s">
-        <v>730</v>
-      </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
@@ -3098,12 +2942,6 @@
       <c r="B42" t="s">
         <v>659</v>
       </c>
-      <c r="C42" t="s">
-        <v>731</v>
-      </c>
-      <c r="D42" t="s">
-        <v>732</v>
-      </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
@@ -3131,12 +2969,6 @@
       <c r="B45" t="s">
         <v>659</v>
       </c>
-      <c r="C45" t="s">
-        <v>733</v>
-      </c>
-      <c r="D45" t="s">
-        <v>734</v>
-      </c>
     </row>
     <row r="46" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
@@ -3172,9 +3004,6 @@
       <c r="C49" t="s">
         <v>687</v>
       </c>
-      <c r="D49" t="s">
-        <v>735</v>
-      </c>
     </row>
     <row r="50" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
@@ -3237,9 +3066,6 @@
       <c r="B56" t="s">
         <v>659</v>
       </c>
-      <c r="C56" t="s">
-        <v>736</v>
-      </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
@@ -3259,9 +3085,7 @@
       <c r="B58" t="s">
         <v>659</v>
       </c>
-      <c r="C58" s="1" t="s">
-        <v>737</v>
-      </c>
+      <c r="C58" s="1"/>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
@@ -3311,9 +3135,6 @@
       <c r="B63" t="s">
         <v>659</v>
       </c>
-      <c r="C63" t="s">
-        <v>738</v>
-      </c>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
@@ -8149,14 +7970,11 @@
       </c>
     </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="C58" r:id="rId1" xr:uid="{EA88CC23-8DEB-439F-9636-E00F8F2C36E7}"/>
-  </hyperlinks>
   <printOptions gridLines="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
   <tableParts count="1">
-    <tablePart r:id="rId3"/>
+    <tablePart r:id="rId2"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
add A. ferox male
</commit_message>
<xml_diff>
--- a/photos.xlsx
+++ b/photos.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cedri\Documents\web\araignees_idf\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3FE4ED6A-F0C1-4664-9266-08B59CE8F8F7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F96D43EF-FBFB-4EE7-8633-DE23702396A5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1404" uniqueCount="752">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1405" uniqueCount="753">
   <si>
     <t>taxon</t>
   </si>
@@ -2276,6 +2276,9 @@
   </si>
   <si>
     <t>www/media/fiches/diaea_dorsata_male.webp</t>
+  </si>
+  <si>
+    <t>www/media/fiches/amaurobius_ferox_male.webp</t>
   </si>
 </sst>
 </file>
@@ -2354,7 +2357,14 @@
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{5221C8D7-EF93-417B-B8B8-217FC377064B}" name="Tableau1" displayName="Tableau1" ref="A1:E656" totalsRowShown="0">
-  <autoFilter ref="A1:E656" xr:uid="{5221C8D7-EF93-417B-B8B8-217FC377064B}"/>
+  <autoFilter ref="A1:E656" xr:uid="{5221C8D7-EF93-417B-B8B8-217FC377064B}">
+    <filterColumn colId="1">
+      <filters>
+        <filter val="?"/>
+        <filter val="oui"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <tableColumns count="5">
     <tableColumn id="1" xr3:uid="{8CF3FEBE-EC73-416E-8610-F705B8D6D336}" name="taxon"/>
     <tableColumn id="4" xr3:uid="{666FCC22-DD53-4830-B712-02B264DDA363}" name="id à vue"/>
@@ -2687,8 +2697,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E656"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A591" workbookViewId="0">
-      <selection activeCell="D611" sqref="D611"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D22" sqref="D22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2743,7 +2753,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -2755,7 +2765,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -2767,7 +2777,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>5</v>
       </c>
@@ -2779,7 +2789,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>6</v>
       </c>
@@ -2791,7 +2801,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>7</v>
       </c>
@@ -2803,7 +2813,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>8</v>
       </c>
@@ -2815,7 +2825,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>9</v>
       </c>
@@ -2827,7 +2837,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>10</v>
       </c>
@@ -2839,7 +2849,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>11</v>
       </c>
@@ -2851,7 +2861,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>12</v>
       </c>
@@ -2863,7 +2873,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>13</v>
       </c>
@@ -2887,7 +2897,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>15</v>
       </c>
@@ -2899,7 +2909,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>16</v>
       </c>
@@ -2957,6 +2967,9 @@
       <c r="C21" t="s">
         <v>679</v>
       </c>
+      <c r="D21" t="s">
+        <v>752</v>
+      </c>
       <c r="E21" t="b">
         <f>OR(Tableau1[[#This Row],[femelle]]&lt;&gt;"", Tableau1[[#This Row],[male]]&lt;&gt;"")</f>
         <v>1</v>
@@ -2989,7 +3002,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>23</v>
       </c>
@@ -3001,7 +3014,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>24</v>
       </c>
@@ -3109,7 +3122,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>33</v>
       </c>
@@ -3121,7 +3134,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>34</v>
       </c>
@@ -3133,7 +3146,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>35</v>
       </c>
@@ -3145,7 +3158,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>36</v>
       </c>
@@ -3157,7 +3170,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>37</v>
       </c>
@@ -3253,7 +3266,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
         <v>43</v>
       </c>
@@ -3277,7 +3290,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
         <v>45</v>
       </c>
@@ -3289,7 +3302,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
         <v>46</v>
       </c>
@@ -3301,7 +3314,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
         <v>47</v>
       </c>
@@ -3328,7 +3341,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
         <v>49</v>
       </c>
@@ -3355,7 +3368,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
         <v>51</v>
       </c>
@@ -3367,7 +3380,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
         <v>52</v>
       </c>
@@ -3379,7 +3392,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
         <v>53</v>
       </c>
@@ -3539,7 +3552,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
         <v>618</v>
       </c>
@@ -3569,7 +3582,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
         <v>65</v>
       </c>
@@ -3593,7 +3606,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="70" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
         <v>620</v>
       </c>
@@ -3605,7 +3618,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="71" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
         <v>66</v>
       </c>
@@ -3617,7 +3630,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="72" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
         <v>67</v>
       </c>
@@ -3656,7 +3669,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="75" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A75" t="s">
         <v>70</v>
       </c>
@@ -3668,7 +3681,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="76" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A76" t="s">
         <v>71</v>
       </c>
@@ -3680,7 +3693,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="77" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A77" t="s">
         <v>72</v>
       </c>
@@ -3692,7 +3705,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="78" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A78" t="s">
         <v>73</v>
       </c>
@@ -3704,7 +3717,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="79" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A79" t="s">
         <v>74</v>
       </c>
@@ -3716,7 +3729,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="80" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A80" t="s">
         <v>75</v>
       </c>
@@ -3728,7 +3741,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="81" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A81" t="s">
         <v>76</v>
       </c>
@@ -3740,7 +3753,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="82" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A82" t="s">
         <v>77</v>
       </c>
@@ -3753,7 +3766,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="83" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A83" t="s">
         <v>78</v>
       </c>
@@ -3765,7 +3778,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="84" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A84" t="s">
         <v>79</v>
       </c>
@@ -3777,7 +3790,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="85" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A85" t="s">
         <v>80</v>
       </c>
@@ -3789,7 +3802,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="86" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A86" t="s">
         <v>81</v>
       </c>
@@ -3801,7 +3814,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="87" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A87" t="s">
         <v>82</v>
       </c>
@@ -3813,7 +3826,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="88" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A88" t="s">
         <v>83</v>
       </c>
@@ -3825,7 +3838,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="89" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A89" t="s">
         <v>84</v>
       </c>
@@ -3837,7 +3850,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="90" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A90" t="s">
         <v>85</v>
       </c>
@@ -3849,7 +3862,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="91" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A91" t="s">
         <v>621</v>
       </c>
@@ -3876,7 +3889,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="93" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A93" t="s">
         <v>87</v>
       </c>
@@ -3888,7 +3901,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="94" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A94" t="s">
         <v>622</v>
       </c>
@@ -3900,7 +3913,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="95" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A95" t="s">
         <v>88</v>
       </c>
@@ -3912,7 +3925,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="96" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A96" t="s">
         <v>89</v>
       </c>
@@ -3951,7 +3964,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="99" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A99" t="s">
         <v>92</v>
       </c>
@@ -3963,7 +3976,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="100" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A100" t="s">
         <v>93</v>
       </c>
@@ -3975,7 +3988,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="101" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A101" t="s">
         <v>94</v>
       </c>
@@ -3987,7 +4000,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="102" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A102" t="s">
         <v>95</v>
       </c>
@@ -3999,7 +4012,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="103" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A103" t="s">
         <v>96</v>
       </c>
@@ -4011,7 +4024,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="104" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A104" t="s">
         <v>97</v>
       </c>
@@ -4095,7 +4108,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="110" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A110" t="s">
         <v>103</v>
       </c>
@@ -4173,7 +4186,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="116" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A116" t="s">
         <v>110</v>
       </c>
@@ -4185,7 +4198,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="117" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="117" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A117" t="s">
         <v>111</v>
       </c>
@@ -4197,7 +4210,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="118" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="118" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A118" t="s">
         <v>112</v>
       </c>
@@ -4209,7 +4222,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="119" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="119" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A119" t="s">
         <v>113</v>
       </c>
@@ -4221,7 +4234,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="120" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="120" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A120" t="s">
         <v>114</v>
       </c>
@@ -4233,7 +4246,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="121" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="121" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A121" t="s">
         <v>115</v>
       </c>
@@ -4245,7 +4258,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="122" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="122" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A122" t="s">
         <v>116</v>
       </c>
@@ -4257,7 +4270,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="123" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="123" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A123" t="s">
         <v>117</v>
       </c>
@@ -4269,7 +4282,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="124" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="124" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A124" t="s">
         <v>118</v>
       </c>
@@ -4281,7 +4294,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="125" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="125" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A125" t="s">
         <v>119</v>
       </c>
@@ -4293,7 +4306,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="126" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="126" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A126" t="s">
         <v>120</v>
       </c>
@@ -4305,7 +4318,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="127" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="127" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A127" t="s">
         <v>121</v>
       </c>
@@ -4317,7 +4330,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="128" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="128" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A128" t="s">
         <v>122</v>
       </c>
@@ -4329,7 +4342,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="129" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="129" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A129" t="s">
         <v>123</v>
       </c>
@@ -4341,7 +4354,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="130" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="130" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A130" t="s">
         <v>623</v>
       </c>
@@ -4353,7 +4366,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="131" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="131" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A131" t="s">
         <v>124</v>
       </c>
@@ -4365,7 +4378,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="132" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="132" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A132" t="s">
         <v>125</v>
       </c>
@@ -4377,7 +4390,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="133" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="133" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A133" t="s">
         <v>126</v>
       </c>
@@ -4389,7 +4402,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="134" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="134" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A134" t="s">
         <v>127</v>
       </c>
@@ -4401,7 +4414,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="135" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="135" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A135" t="s">
         <v>128</v>
       </c>
@@ -4425,7 +4438,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="137" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="137" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A137" t="s">
         <v>130</v>
       </c>
@@ -4449,7 +4462,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="139" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="139" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A139" t="s">
         <v>132</v>
       </c>
@@ -4485,7 +4498,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="142" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="142" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A142" t="s">
         <v>135</v>
       </c>
@@ -4497,7 +4510,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="143" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="143" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A143" t="s">
         <v>136</v>
       </c>
@@ -4509,7 +4522,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="144" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="144" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A144" t="s">
         <v>137</v>
       </c>
@@ -4521,7 +4534,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="145" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="145" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A145" t="s">
         <v>138</v>
       </c>
@@ -4593,7 +4606,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="151" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="151" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A151" t="s">
         <v>142</v>
       </c>
@@ -4617,7 +4630,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="153" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="153" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A153" t="s">
         <v>144</v>
       </c>
@@ -4629,7 +4642,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="154" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="154" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A154" t="s">
         <v>145</v>
       </c>
@@ -4641,7 +4654,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="155" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="155" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A155" t="s">
         <v>146</v>
       </c>
@@ -4653,7 +4666,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="156" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="156" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A156" t="s">
         <v>147</v>
       </c>
@@ -4665,7 +4678,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="157" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="157" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A157" t="s">
         <v>148</v>
       </c>
@@ -4677,7 +4690,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="158" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="158" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A158" t="s">
         <v>149</v>
       </c>
@@ -4689,7 +4702,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="159" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="159" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A159" t="s">
         <v>150</v>
       </c>
@@ -4701,7 +4714,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="160" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="160" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A160" t="s">
         <v>151</v>
       </c>
@@ -4713,7 +4726,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="161" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="161" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A161" t="s">
         <v>152</v>
       </c>
@@ -4737,7 +4750,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="163" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="163" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A163" t="s">
         <v>154</v>
       </c>
@@ -4749,7 +4762,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="164" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="164" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A164" t="s">
         <v>155</v>
       </c>
@@ -4761,7 +4774,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="165" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="165" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A165" t="s">
         <v>156</v>
       </c>
@@ -4773,7 +4786,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="166" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="166" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A166" t="s">
         <v>157</v>
       </c>
@@ -4785,7 +4798,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="167" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="167" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A167" t="s">
         <v>158</v>
       </c>
@@ -4797,7 +4810,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="168" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="168" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A168" t="s">
         <v>159</v>
       </c>
@@ -4809,7 +4822,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="169" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="169" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A169" t="s">
         <v>160</v>
       </c>
@@ -4821,7 +4834,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="170" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="170" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A170" t="s">
         <v>161</v>
       </c>
@@ -4833,7 +4846,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="171" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="171" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A171" t="s">
         <v>162</v>
       </c>
@@ -4845,7 +4858,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="172" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="172" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A172" t="s">
         <v>163</v>
       </c>
@@ -4857,7 +4870,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="173" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="173" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A173" t="s">
         <v>164</v>
       </c>
@@ -4869,7 +4882,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="174" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="174" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A174" t="s">
         <v>165</v>
       </c>
@@ -4881,7 +4894,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="175" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="175" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A175" t="s">
         <v>166</v>
       </c>
@@ -4893,7 +4906,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="176" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="176" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A176" t="s">
         <v>167</v>
       </c>
@@ -4905,7 +4918,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="177" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="177" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A177" t="s">
         <v>168</v>
       </c>
@@ -4917,7 +4930,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="178" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="178" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A178" t="s">
         <v>169</v>
       </c>
@@ -4929,7 +4942,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="179" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="179" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A179" t="s">
         <v>170</v>
       </c>
@@ -4941,7 +4954,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="180" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="180" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A180" t="s">
         <v>171</v>
       </c>
@@ -4953,7 +4966,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="181" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="181" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A181" t="s">
         <v>172</v>
       </c>
@@ -4965,7 +4978,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="182" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="182" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A182" t="s">
         <v>173</v>
       </c>
@@ -4977,7 +4990,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="183" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="183" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A183" t="s">
         <v>174</v>
       </c>
@@ -4989,7 +5002,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="184" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="184" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A184" t="s">
         <v>175</v>
       </c>
@@ -5001,7 +5014,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="185" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="185" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A185" t="s">
         <v>176</v>
       </c>
@@ -5013,7 +5026,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="186" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="186" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A186" t="s">
         <v>177</v>
       </c>
@@ -5025,7 +5038,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="187" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="187" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A187" t="s">
         <v>625</v>
       </c>
@@ -5037,7 +5050,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="188" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="188" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A188" t="s">
         <v>178</v>
       </c>
@@ -5049,7 +5062,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="189" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="189" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A189" t="s">
         <v>179</v>
       </c>
@@ -5061,7 +5074,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="190" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="190" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A190" t="s">
         <v>180</v>
       </c>
@@ -5073,7 +5086,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="191" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="191" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A191" t="s">
         <v>181</v>
       </c>
@@ -5085,7 +5098,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="192" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="192" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A192" t="s">
         <v>182</v>
       </c>
@@ -5097,7 +5110,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="193" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="193" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A193" t="s">
         <v>183</v>
       </c>
@@ -5109,7 +5122,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="194" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="194" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A194" t="s">
         <v>184</v>
       </c>
@@ -5121,7 +5134,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="195" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="195" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A195" t="s">
         <v>185</v>
       </c>
@@ -5133,7 +5146,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="196" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="196" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A196" t="s">
         <v>186</v>
       </c>
@@ -5145,7 +5158,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="197" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="197" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A197" t="s">
         <v>187</v>
       </c>
@@ -5157,7 +5170,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="198" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="198" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A198" t="s">
         <v>188</v>
       </c>
@@ -5169,7 +5182,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="199" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="199" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A199" t="s">
         <v>189</v>
       </c>
@@ -5181,7 +5194,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="200" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="200" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A200" t="s">
         <v>190</v>
       </c>
@@ -5193,7 +5206,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="201" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="201" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A201" t="s">
         <v>191</v>
       </c>
@@ -5205,7 +5218,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="202" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="202" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A202" t="s">
         <v>192</v>
       </c>
@@ -5217,7 +5230,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="203" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="203" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A203" t="s">
         <v>193</v>
       </c>
@@ -5229,7 +5242,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="204" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="204" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A204" t="s">
         <v>194</v>
       </c>
@@ -5241,7 +5254,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="205" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="205" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A205" t="s">
         <v>195</v>
       </c>
@@ -5253,7 +5266,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="206" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="206" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A206" t="s">
         <v>196</v>
       </c>
@@ -5265,7 +5278,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="207" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="207" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A207" t="s">
         <v>197</v>
       </c>
@@ -5277,7 +5290,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="208" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="208" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A208" t="s">
         <v>198</v>
       </c>
@@ -5289,7 +5302,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="209" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="209" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A209" t="s">
         <v>199</v>
       </c>
@@ -5301,7 +5314,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="210" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="210" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A210" t="s">
         <v>200</v>
       </c>
@@ -5313,7 +5326,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="211" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="211" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A211" t="s">
         <v>201</v>
       </c>
@@ -5325,7 +5338,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="212" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="212" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A212" t="s">
         <v>202</v>
       </c>
@@ -5337,7 +5350,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="213" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="213" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A213" t="s">
         <v>203</v>
       </c>
@@ -5349,7 +5362,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="214" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="214" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A214" t="s">
         <v>204</v>
       </c>
@@ -5361,7 +5374,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="215" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="215" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A215" t="s">
         <v>205</v>
       </c>
@@ -5373,7 +5386,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="216" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="216" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A216" t="s">
         <v>206</v>
       </c>
@@ -5385,7 +5398,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="217" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="217" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A217" t="s">
         <v>207</v>
       </c>
@@ -5397,7 +5410,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="218" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="218" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A218" t="s">
         <v>208</v>
       </c>
@@ -5409,7 +5422,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="219" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="219" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A219" t="s">
         <v>209</v>
       </c>
@@ -5421,7 +5434,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="220" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="220" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A220" t="s">
         <v>210</v>
       </c>
@@ -5433,7 +5446,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="221" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="221" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A221" t="s">
         <v>211</v>
       </c>
@@ -5445,7 +5458,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="222" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="222" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A222" t="s">
         <v>212</v>
       </c>
@@ -5457,7 +5470,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="223" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="223" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A223" t="s">
         <v>213</v>
       </c>
@@ -5469,7 +5482,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="224" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="224" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A224" t="s">
         <v>214</v>
       </c>
@@ -5508,7 +5521,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="227" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="227" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A227" t="s">
         <v>217</v>
       </c>
@@ -5520,7 +5533,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="228" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="228" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A228" t="s">
         <v>218</v>
       </c>
@@ -5532,7 +5545,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="229" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="229" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A229" t="s">
         <v>219</v>
       </c>
@@ -5544,7 +5557,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="230" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="230" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A230" t="s">
         <v>220</v>
       </c>
@@ -5556,7 +5569,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="231" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="231" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A231" t="s">
         <v>221</v>
       </c>
@@ -5568,7 +5581,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="232" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="232" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A232" t="s">
         <v>626</v>
       </c>
@@ -5580,7 +5593,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="233" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="233" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A233" t="s">
         <v>627</v>
       </c>
@@ -5592,7 +5605,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="234" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="234" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A234" t="s">
         <v>222</v>
       </c>
@@ -5604,7 +5617,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="235" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="235" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A235" t="s">
         <v>223</v>
       </c>
@@ -5616,7 +5629,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="236" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="236" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A236" t="s">
         <v>224</v>
       </c>
@@ -5628,7 +5641,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="237" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="237" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A237" t="s">
         <v>225</v>
       </c>
@@ -5640,7 +5653,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="238" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="238" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A238" t="s">
         <v>628</v>
       </c>
@@ -5652,7 +5665,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="239" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="239" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A239" t="s">
         <v>226</v>
       </c>
@@ -5664,7 +5677,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="240" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="240" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A240" t="s">
         <v>227</v>
       </c>
@@ -5676,7 +5689,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="241" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="241" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A241" t="s">
         <v>228</v>
       </c>
@@ -5688,7 +5701,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="242" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="242" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A242" t="s">
         <v>229</v>
       </c>
@@ -5700,7 +5713,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="243" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="243" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A243" t="s">
         <v>230</v>
       </c>
@@ -5712,7 +5725,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="244" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="244" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A244" t="s">
         <v>231</v>
       </c>
@@ -5724,7 +5737,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="245" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="245" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A245" t="s">
         <v>232</v>
       </c>
@@ -5736,7 +5749,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="246" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="246" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A246" t="s">
         <v>233</v>
       </c>
@@ -5748,7 +5761,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="247" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="247" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A247" t="s">
         <v>234</v>
       </c>
@@ -5760,7 +5773,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="248" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="248" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A248" t="s">
         <v>235</v>
       </c>
@@ -5772,7 +5785,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="249" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="249" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A249" t="s">
         <v>236</v>
       </c>
@@ -5802,7 +5815,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="251" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="251" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A251" t="s">
         <v>238</v>
       </c>
@@ -5814,7 +5827,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="252" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="252" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A252" t="s">
         <v>239</v>
       </c>
@@ -5826,7 +5839,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="253" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="253" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A253" t="s">
         <v>629</v>
       </c>
@@ -5838,7 +5851,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="254" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="254" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A254" t="s">
         <v>240</v>
       </c>
@@ -5850,7 +5863,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="255" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="255" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A255" t="s">
         <v>241</v>
       </c>
@@ -5862,7 +5875,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="256" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="256" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A256" t="s">
         <v>242</v>
       </c>
@@ -5874,7 +5887,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="257" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="257" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A257" t="s">
         <v>630</v>
       </c>
@@ -5886,7 +5899,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="258" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="258" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A258" t="s">
         <v>243</v>
       </c>
@@ -5898,7 +5911,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="259" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="259" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A259" t="s">
         <v>631</v>
       </c>
@@ -5910,7 +5923,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="260" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="260" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A260" t="s">
         <v>244</v>
       </c>
@@ -5922,7 +5935,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="261" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="261" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A261" t="s">
         <v>245</v>
       </c>
@@ -5934,7 +5947,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="262" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="262" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A262" t="s">
         <v>632</v>
       </c>
@@ -5946,7 +5959,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="263" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="263" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A263" t="s">
         <v>246</v>
       </c>
@@ -5958,7 +5971,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="264" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="264" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A264" t="s">
         <v>247</v>
       </c>
@@ -5970,7 +5983,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="265" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="265" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A265" t="s">
         <v>248</v>
       </c>
@@ -5982,7 +5995,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="266" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="266" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A266" t="s">
         <v>249</v>
       </c>
@@ -5994,7 +6007,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="267" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="267" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A267" t="s">
         <v>250</v>
       </c>
@@ -6006,7 +6019,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="268" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="268" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A268" t="s">
         <v>251</v>
       </c>
@@ -6018,7 +6031,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="269" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="269" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A269" t="s">
         <v>252</v>
       </c>
@@ -6030,7 +6043,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="270" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="270" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A270" t="s">
         <v>253</v>
       </c>
@@ -6042,7 +6055,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="271" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="271" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A271" t="s">
         <v>633</v>
       </c>
@@ -6054,7 +6067,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="272" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="272" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A272" t="s">
         <v>254</v>
       </c>
@@ -6066,7 +6079,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="273" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="273" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A273" t="s">
         <v>634</v>
       </c>
@@ -6078,7 +6091,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="274" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="274" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A274" t="s">
         <v>255</v>
       </c>
@@ -6102,7 +6115,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="276" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="276" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A276" t="s">
         <v>257</v>
       </c>
@@ -6114,7 +6127,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="277" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="277" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A277" t="s">
         <v>258</v>
       </c>
@@ -6141,7 +6154,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="279" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="279" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A279" t="s">
         <v>260</v>
       </c>
@@ -6171,7 +6184,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="281" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="281" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A281" t="s">
         <v>262</v>
       </c>
@@ -6183,7 +6196,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="282" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="282" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A282" t="s">
         <v>263</v>
       </c>
@@ -6195,7 +6208,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="283" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="283" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A283" t="s">
         <v>264</v>
       </c>
@@ -6207,7 +6220,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="284" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="284" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A284" t="s">
         <v>265</v>
       </c>
@@ -6219,7 +6232,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="285" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="285" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A285" t="s">
         <v>266</v>
       </c>
@@ -6231,7 +6244,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="286" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="286" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A286" t="s">
         <v>267</v>
       </c>
@@ -6258,7 +6271,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="288" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="288" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A288" t="s">
         <v>269</v>
       </c>
@@ -6270,7 +6283,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="289" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="289" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A289" t="s">
         <v>270</v>
       </c>
@@ -6282,7 +6295,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="290" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="290" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A290" t="s">
         <v>271</v>
       </c>
@@ -6294,7 +6307,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="291" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="291" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A291" t="s">
         <v>272</v>
       </c>
@@ -6306,7 +6319,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="292" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="292" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A292" t="s">
         <v>273</v>
       </c>
@@ -6318,7 +6331,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="293" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="293" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A293" t="s">
         <v>274</v>
       </c>
@@ -6330,7 +6343,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="294" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="294" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A294" t="s">
         <v>275</v>
       </c>
@@ -6342,7 +6355,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="295" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="295" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A295" t="s">
         <v>635</v>
       </c>
@@ -6354,7 +6367,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="296" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="296" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A296" t="s">
         <v>276</v>
       </c>
@@ -6366,7 +6379,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="297" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="297" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A297" t="s">
         <v>277</v>
       </c>
@@ -6378,7 +6391,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="298" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="298" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A298" t="s">
         <v>278</v>
       </c>
@@ -6390,7 +6403,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="299" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="299" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A299" t="s">
         <v>279</v>
       </c>
@@ -6402,7 +6415,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="300" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="300" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A300" t="s">
         <v>280</v>
       </c>
@@ -6414,7 +6427,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="301" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="301" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A301" t="s">
         <v>281</v>
       </c>
@@ -6426,7 +6439,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="302" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="302" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A302" t="s">
         <v>282</v>
       </c>
@@ -6438,7 +6451,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="303" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="303" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A303" t="s">
         <v>283</v>
       </c>
@@ -6450,7 +6463,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="304" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="304" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A304" t="s">
         <v>284</v>
       </c>
@@ -6462,7 +6475,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="305" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="305" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A305" t="s">
         <v>636</v>
       </c>
@@ -6474,7 +6487,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="306" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="306" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A306" t="s">
         <v>285</v>
       </c>
@@ -6486,7 +6499,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="307" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="307" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A307" t="s">
         <v>286</v>
       </c>
@@ -6498,7 +6511,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="308" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="308" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A308" t="s">
         <v>287</v>
       </c>
@@ -6510,7 +6523,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="309" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="309" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A309" t="s">
         <v>637</v>
       </c>
@@ -6522,7 +6535,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="310" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="310" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A310" t="s">
         <v>288</v>
       </c>
@@ -6534,7 +6547,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="311" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="311" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A311" t="s">
         <v>289</v>
       </c>
@@ -6546,7 +6559,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="312" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="312" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A312" t="s">
         <v>290</v>
       </c>
@@ -6558,7 +6571,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="313" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="313" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A313" t="s">
         <v>291</v>
       </c>
@@ -6570,7 +6583,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="314" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="314" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A314" t="s">
         <v>292</v>
       </c>
@@ -6582,7 +6595,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="315" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="315" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A315" t="s">
         <v>293</v>
       </c>
@@ -6594,7 +6607,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="316" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="316" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A316" t="s">
         <v>294</v>
       </c>
@@ -6606,7 +6619,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="317" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="317" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A317" t="s">
         <v>295</v>
       </c>
@@ -6618,7 +6631,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="318" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="318" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A318" t="s">
         <v>296</v>
       </c>
@@ -6630,7 +6643,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="319" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="319" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A319" t="s">
         <v>297</v>
       </c>
@@ -6642,7 +6655,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="320" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="320" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A320" t="s">
         <v>298</v>
       </c>
@@ -6654,7 +6667,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="321" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="321" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A321" t="s">
         <v>299</v>
       </c>
@@ -6666,7 +6679,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="322" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="322" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A322" t="s">
         <v>300</v>
       </c>
@@ -6678,7 +6691,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="323" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="323" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A323" t="s">
         <v>301</v>
       </c>
@@ -6690,7 +6703,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="324" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="324" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A324" t="s">
         <v>302</v>
       </c>
@@ -6702,7 +6715,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="325" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="325" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A325" t="s">
         <v>303</v>
       </c>
@@ -6714,7 +6727,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="326" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="326" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A326" t="s">
         <v>304</v>
       </c>
@@ -6726,7 +6739,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="327" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="327" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A327" t="s">
         <v>305</v>
       </c>
@@ -6738,7 +6751,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="328" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="328" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A328" t="s">
         <v>306</v>
       </c>
@@ -6750,7 +6763,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="329" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="329" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A329" t="s">
         <v>307</v>
       </c>
@@ -6762,7 +6775,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="330" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="330" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A330" t="s">
         <v>308</v>
       </c>
@@ -6774,7 +6787,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="331" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="331" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A331" t="s">
         <v>638</v>
       </c>
@@ -6786,7 +6799,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="332" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="332" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A332" t="s">
         <v>309</v>
       </c>
@@ -6798,7 +6811,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="333" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="333" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A333" t="s">
         <v>639</v>
       </c>
@@ -6810,7 +6823,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="334" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="334" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A334" t="s">
         <v>310</v>
       </c>
@@ -6822,7 +6835,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="335" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="335" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A335" t="s">
         <v>614</v>
       </c>
@@ -6834,7 +6847,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="336" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="336" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A336" t="s">
         <v>311</v>
       </c>
@@ -6846,7 +6859,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="337" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="337" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A337" t="s">
         <v>640</v>
       </c>
@@ -6858,7 +6871,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="338" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="338" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A338" t="s">
         <v>312</v>
       </c>
@@ -6870,7 +6883,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="339" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="339" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A339" t="s">
         <v>313</v>
       </c>
@@ -6882,7 +6895,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="340" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="340" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A340" t="s">
         <v>314</v>
       </c>
@@ -6894,7 +6907,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="341" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="341" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A341" t="s">
         <v>315</v>
       </c>
@@ -6906,7 +6919,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="342" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="342" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A342" t="s">
         <v>316</v>
       </c>
@@ -6918,7 +6931,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="343" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="343" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A343" t="s">
         <v>641</v>
       </c>
@@ -6930,7 +6943,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="344" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="344" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A344" t="s">
         <v>317</v>
       </c>
@@ -6954,7 +6967,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="346" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="346" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A346" t="s">
         <v>319</v>
       </c>
@@ -6966,7 +6979,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="347" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="347" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A347" t="s">
         <v>320</v>
       </c>
@@ -6978,7 +6991,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="348" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="348" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A348" t="s">
         <v>321</v>
       </c>
@@ -6990,7 +7003,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="349" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="349" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A349" t="s">
         <v>322</v>
       </c>
@@ -7002,7 +7015,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="350" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="350" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A350" t="s">
         <v>642</v>
       </c>
@@ -7014,7 +7027,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="351" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="351" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A351" t="s">
         <v>323</v>
       </c>
@@ -7026,7 +7039,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="352" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="352" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A352" t="s">
         <v>324</v>
       </c>
@@ -7038,7 +7051,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="353" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="353" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A353" t="s">
         <v>643</v>
       </c>
@@ -7050,7 +7063,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="354" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="354" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A354" t="s">
         <v>325</v>
       </c>
@@ -7062,7 +7075,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="355" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="355" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A355" t="s">
         <v>326</v>
       </c>
@@ -7074,7 +7087,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="356" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="356" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A356" t="s">
         <v>327</v>
       </c>
@@ -7086,7 +7099,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="357" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="357" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A357" t="s">
         <v>644</v>
       </c>
@@ -7098,7 +7111,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="358" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="358" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A358" t="s">
         <v>328</v>
       </c>
@@ -7110,7 +7123,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="359" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="359" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A359" t="s">
         <v>329</v>
       </c>
@@ -7122,7 +7135,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="360" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="360" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A360" t="s">
         <v>330</v>
       </c>
@@ -7134,7 +7147,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="361" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="361" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A361" t="s">
         <v>331</v>
       </c>
@@ -7146,7 +7159,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="362" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="362" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A362" t="s">
         <v>332</v>
       </c>
@@ -7158,7 +7171,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="363" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="363" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A363" t="s">
         <v>333</v>
       </c>
@@ -7170,7 +7183,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="364" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="364" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A364" t="s">
         <v>334</v>
       </c>
@@ -7182,7 +7195,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="365" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="365" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A365" t="s">
         <v>335</v>
       </c>
@@ -7194,7 +7207,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="366" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="366" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A366" t="s">
         <v>336</v>
       </c>
@@ -7206,7 +7219,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="367" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="367" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A367" t="s">
         <v>337</v>
       </c>
@@ -7218,7 +7231,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="368" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="368" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A368" t="s">
         <v>338</v>
       </c>
@@ -7266,7 +7279,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="372" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="372" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A372" t="s">
         <v>342</v>
       </c>
@@ -7302,7 +7315,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="375" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="375" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A375" t="s">
         <v>345</v>
       </c>
@@ -7326,7 +7339,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="377" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="377" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A377" t="s">
         <v>347</v>
       </c>
@@ -7338,7 +7351,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="378" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="378" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A378" t="s">
         <v>348</v>
       </c>
@@ -7350,7 +7363,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="379" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="379" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A379" t="s">
         <v>349</v>
       </c>
@@ -7362,7 +7375,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="380" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="380" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A380" t="s">
         <v>350</v>
       </c>
@@ -7374,7 +7387,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="381" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="381" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A381" t="s">
         <v>351</v>
       </c>
@@ -7386,7 +7399,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="382" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="382" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A382" t="s">
         <v>352</v>
       </c>
@@ -7410,7 +7423,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="384" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="384" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A384" t="s">
         <v>354</v>
       </c>
@@ -7461,7 +7474,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="388" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="388" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A388" t="s">
         <v>357</v>
       </c>
@@ -7473,7 +7486,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="389" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="389" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A389" t="s">
         <v>358</v>
       </c>
@@ -7485,7 +7498,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="390" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="390" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A390" t="s">
         <v>359</v>
       </c>
@@ -7509,7 +7522,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="392" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="392" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A392" t="s">
         <v>361</v>
       </c>
@@ -7521,7 +7534,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="393" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="393" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A393" t="s">
         <v>362</v>
       </c>
@@ -7533,7 +7546,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="394" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="394" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A394" t="s">
         <v>363</v>
       </c>
@@ -7557,7 +7570,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="396" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="396" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A396" t="s">
         <v>365</v>
       </c>
@@ -7569,7 +7582,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="397" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="397" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A397" t="s">
         <v>366</v>
       </c>
@@ -7581,7 +7594,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="398" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="398" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A398" t="s">
         <v>367</v>
       </c>
@@ -7593,7 +7606,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="399" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="399" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A399" t="s">
         <v>368</v>
       </c>
@@ -7605,7 +7618,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="400" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="400" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A400" t="s">
         <v>369</v>
       </c>
@@ -7617,7 +7630,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="401" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="401" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A401" t="s">
         <v>370</v>
       </c>
@@ -7629,7 +7642,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="402" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="402" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A402" t="s">
         <v>371</v>
       </c>
@@ -7653,7 +7666,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="404" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="404" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A404" t="s">
         <v>373</v>
       </c>
@@ -7665,7 +7678,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="405" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="405" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A405" t="s">
         <v>374</v>
       </c>
@@ -7677,7 +7690,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="406" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="406" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A406" t="s">
         <v>375</v>
       </c>
@@ -7689,7 +7702,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="407" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="407" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A407" t="s">
         <v>376</v>
       </c>
@@ -7701,7 +7714,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="408" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="408" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A408" t="s">
         <v>377</v>
       </c>
@@ -7713,7 +7726,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="409" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="409" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A409" t="s">
         <v>378</v>
       </c>
@@ -7725,7 +7738,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="410" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="410" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A410" t="s">
         <v>379</v>
       </c>
@@ -7737,7 +7750,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="411" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="411" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A411" t="s">
         <v>380</v>
       </c>
@@ -7749,7 +7762,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="412" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="412" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A412" t="s">
         <v>381</v>
       </c>
@@ -7773,7 +7786,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="414" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="414" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A414" t="s">
         <v>383</v>
       </c>
@@ -7785,7 +7798,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="415" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="415" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A415" t="s">
         <v>384</v>
       </c>
@@ -7797,7 +7810,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="416" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="416" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A416" t="s">
         <v>385</v>
       </c>
@@ -7809,7 +7822,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="417" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="417" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A417" t="s">
         <v>386</v>
       </c>
@@ -7821,7 +7834,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="418" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="418" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A418" t="s">
         <v>387</v>
       </c>
@@ -7833,7 +7846,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="419" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="419" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A419" t="s">
         <v>388</v>
       </c>
@@ -7857,7 +7870,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="421" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="421" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A421" t="s">
         <v>390</v>
       </c>
@@ -7869,7 +7882,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="422" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="422" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A422" t="s">
         <v>391</v>
       </c>
@@ -7905,7 +7918,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="425" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="425" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A425" t="s">
         <v>646</v>
       </c>
@@ -7917,7 +7930,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="426" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="426" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A426" t="s">
         <v>394</v>
       </c>
@@ -7929,7 +7942,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="427" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="427" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A427" t="s">
         <v>395</v>
       </c>
@@ -7941,7 +7954,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="428" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="428" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A428" t="s">
         <v>396</v>
       </c>
@@ -7953,7 +7966,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="429" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="429" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A429" t="s">
         <v>397</v>
       </c>
@@ -7977,7 +7990,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="431" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="431" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A431" t="s">
         <v>398</v>
       </c>
@@ -7989,7 +8002,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="432" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="432" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A432" t="s">
         <v>399</v>
       </c>
@@ -8013,7 +8026,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="434" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="434" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A434" t="s">
         <v>401</v>
       </c>
@@ -8025,7 +8038,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="435" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="435" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A435" t="s">
         <v>402</v>
       </c>
@@ -8037,7 +8050,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="436" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="436" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A436" t="s">
         <v>403</v>
       </c>
@@ -8049,7 +8062,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="437" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="437" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A437" t="s">
         <v>404</v>
       </c>
@@ -8079,7 +8092,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="439" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="439" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A439" t="s">
         <v>648</v>
       </c>
@@ -8091,7 +8104,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="440" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="440" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A440" t="s">
         <v>406</v>
       </c>
@@ -8115,7 +8128,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="442" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="442" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A442" t="s">
         <v>407</v>
       </c>
@@ -8127,7 +8140,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="443" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="443" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A443" t="s">
         <v>408</v>
       </c>
@@ -8139,7 +8152,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="444" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="444" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A444" t="s">
         <v>409</v>
       </c>
@@ -8151,7 +8164,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="445" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="445" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A445" t="s">
         <v>410</v>
       </c>
@@ -8163,7 +8176,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="446" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="446" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A446" t="s">
         <v>650</v>
       </c>
@@ -8175,7 +8188,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="447" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="447" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A447" t="s">
         <v>651</v>
       </c>
@@ -8199,7 +8212,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="449" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="449" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A449" t="s">
         <v>412</v>
       </c>
@@ -8211,7 +8224,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="450" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="450" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A450" t="s">
         <v>413</v>
       </c>
@@ -8223,7 +8236,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="451" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="451" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A451" t="s">
         <v>414</v>
       </c>
@@ -8247,7 +8260,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="453" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="453" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A453" t="s">
         <v>416</v>
       </c>
@@ -8259,7 +8272,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="454" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="454" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A454" t="s">
         <v>417</v>
       </c>
@@ -8331,7 +8344,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="459" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="459" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A459" t="s">
         <v>422</v>
       </c>
@@ -8343,7 +8356,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="460" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="460" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A460" t="s">
         <v>423</v>
       </c>
@@ -8355,7 +8368,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="461" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="461" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A461" t="s">
         <v>424</v>
       </c>
@@ -8367,7 +8380,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="462" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="462" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A462" t="s">
         <v>425</v>
       </c>
@@ -8379,7 +8392,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="463" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="463" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A463" t="s">
         <v>426</v>
       </c>
@@ -8433,7 +8446,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="467" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="467" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A467" t="s">
         <v>430</v>
       </c>
@@ -8445,7 +8458,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="468" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="468" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A468" t="s">
         <v>431</v>
       </c>
@@ -8598,7 +8611,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="479" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="479" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A479" t="s">
         <v>442</v>
       </c>
@@ -8610,7 +8623,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="480" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="480" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A480" t="s">
         <v>443</v>
       </c>
@@ -8634,7 +8647,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="482" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="482" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A482" t="s">
         <v>445</v>
       </c>
@@ -8661,7 +8674,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="484" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="484" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A484" t="s">
         <v>447</v>
       </c>
@@ -8781,7 +8794,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="492" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="492" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A492" t="s">
         <v>453</v>
       </c>
@@ -8793,7 +8806,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="493" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="493" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A493" t="s">
         <v>454</v>
       </c>
@@ -8829,7 +8842,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="496" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="496" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A496" t="s">
         <v>457</v>
       </c>
@@ -8841,7 +8854,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="497" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="497" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A497" t="s">
         <v>458</v>
       </c>
@@ -8853,7 +8866,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="498" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="498" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A498" t="s">
         <v>459</v>
       </c>
@@ -8865,7 +8878,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="499" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="499" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A499" t="s">
         <v>460</v>
       </c>
@@ -8877,7 +8890,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="500" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="500" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A500" t="s">
         <v>461</v>
       </c>
@@ -8952,7 +8965,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="506" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="506" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A506" t="s">
         <v>467</v>
       </c>
@@ -8964,7 +8977,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="507" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="507" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A507" t="s">
         <v>468</v>
       </c>
@@ -9006,7 +9019,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="510" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="510" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A510" t="s">
         <v>471</v>
       </c>
@@ -9018,7 +9031,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="511" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="511" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A511" t="s">
         <v>472</v>
       </c>
@@ -9060,7 +9073,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="514" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="514" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A514" t="s">
         <v>475</v>
       </c>
@@ -9072,7 +9085,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="515" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="515" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A515" t="s">
         <v>476</v>
       </c>
@@ -9084,7 +9097,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="516" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="516" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A516" t="s">
         <v>477</v>
       </c>
@@ -9096,7 +9109,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="517" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="517" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A517" t="s">
         <v>478</v>
       </c>
@@ -9108,7 +9121,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="518" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="518" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A518" t="s">
         <v>479</v>
       </c>
@@ -9132,7 +9145,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="520" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="520" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A520" t="s">
         <v>481</v>
       </c>
@@ -9144,7 +9157,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="521" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="521" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A521" t="s">
         <v>482</v>
       </c>
@@ -9372,7 +9385,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="538" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="538" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A538" t="s">
         <v>499</v>
       </c>
@@ -9384,7 +9397,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="539" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="539" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A539" t="s">
         <v>500</v>
       </c>
@@ -9396,7 +9409,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="540" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="540" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A540" t="s">
         <v>501</v>
       </c>
@@ -9408,7 +9421,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="541" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="541" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A541" t="s">
         <v>502</v>
       </c>
@@ -9420,7 +9433,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="542" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="542" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A542" t="s">
         <v>503</v>
       </c>
@@ -9432,7 +9445,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="543" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="543" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A543" t="s">
         <v>504</v>
       </c>
@@ -9444,7 +9457,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="544" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="544" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A544" t="s">
         <v>505</v>
       </c>
@@ -9456,7 +9469,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="545" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="545" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A545" t="s">
         <v>506</v>
       </c>
@@ -9468,7 +9481,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="546" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="546" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A546" t="s">
         <v>507</v>
       </c>
@@ -9504,7 +9517,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="549" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="549" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A549" t="s">
         <v>510</v>
       </c>
@@ -9516,7 +9529,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="550" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="550" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A550" t="s">
         <v>511</v>
       </c>
@@ -9528,7 +9541,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="551" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="551" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A551" t="s">
         <v>512</v>
       </c>
@@ -9555,7 +9568,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="553" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="553" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A553" t="s">
         <v>514</v>
       </c>
@@ -9567,7 +9580,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="554" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="554" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A554" t="s">
         <v>515</v>
       </c>
@@ -9579,7 +9592,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="555" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="555" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A555" t="s">
         <v>516</v>
       </c>
@@ -9591,7 +9604,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="556" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="556" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A556" t="s">
         <v>517</v>
       </c>
@@ -9603,7 +9616,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="557" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="557" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A557" t="s">
         <v>654</v>
       </c>
@@ -9615,7 +9628,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="558" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="558" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A558" t="s">
         <v>519</v>
       </c>
@@ -9627,7 +9640,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="559" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="559" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A559" t="s">
         <v>518</v>
       </c>
@@ -9639,7 +9652,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="560" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="560" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A560" t="s">
         <v>520</v>
       </c>
@@ -9651,7 +9664,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="561" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="561" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A561" t="s">
         <v>521</v>
       </c>
@@ -9723,7 +9736,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="566" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="566" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A566" t="s">
         <v>526</v>
       </c>
@@ -9735,7 +9748,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="567" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="567" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A567" t="s">
         <v>527</v>
       </c>
@@ -9747,7 +9760,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="568" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="568" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A568" t="s">
         <v>655</v>
       </c>
@@ -9771,7 +9784,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="570" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="570" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A570" t="s">
         <v>529</v>
       </c>
@@ -9810,7 +9823,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="573" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="573" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A573" t="s">
         <v>532</v>
       </c>
@@ -9822,7 +9835,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="574" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="574" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A574" t="s">
         <v>533</v>
       </c>
@@ -9876,7 +9889,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="578" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="578" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A578" t="s">
         <v>536</v>
       </c>
@@ -9900,7 +9913,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="580" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="580" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A580" t="s">
         <v>538</v>
       </c>
@@ -9912,7 +9925,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="581" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="581" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A581" t="s">
         <v>539</v>
       </c>
@@ -9924,7 +9937,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="582" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="582" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A582" t="s">
         <v>540</v>
       </c>
@@ -9951,7 +9964,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="584" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="584" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A584" t="s">
         <v>542</v>
       </c>
@@ -9963,7 +9976,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="585" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="585" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A585" t="s">
         <v>543</v>
       </c>
@@ -9975,7 +9988,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="586" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="586" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A586" t="s">
         <v>544</v>
       </c>
@@ -9987,7 +10000,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="587" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="587" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A587" t="s">
         <v>545</v>
       </c>
@@ -9999,7 +10012,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="588" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="588" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A588" t="s">
         <v>546</v>
       </c>
@@ -10011,7 +10024,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="589" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="589" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A589" t="s">
         <v>547</v>
       </c>
@@ -10119,7 +10132,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="597" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="597" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A597" t="s">
         <v>555</v>
       </c>
@@ -10131,7 +10144,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="598" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="598" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A598" t="s">
         <v>556</v>
       </c>
@@ -10143,7 +10156,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="599" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="599" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A599" t="s">
         <v>557</v>
       </c>
@@ -10155,7 +10168,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="600" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="600" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A600" t="s">
         <v>558</v>
       </c>
@@ -10167,7 +10180,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="601" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="601" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A601" t="s">
         <v>559</v>
       </c>
@@ -10179,7 +10192,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="602" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="602" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A602" t="s">
         <v>560</v>
       </c>
@@ -10191,7 +10204,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="603" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="603" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A603" t="s">
         <v>561</v>
       </c>
@@ -10203,7 +10216,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="604" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="604" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A604" t="s">
         <v>562</v>
       </c>
@@ -10215,7 +10228,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="605" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="605" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A605" t="s">
         <v>563</v>
       </c>
@@ -10239,7 +10252,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="607" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="607" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A607" t="s">
         <v>564</v>
       </c>
@@ -10263,7 +10276,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="609" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="609" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A609" t="s">
         <v>566</v>
       </c>
@@ -10329,7 +10342,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="614" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="614" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A614" t="s">
         <v>571</v>
       </c>
@@ -10353,7 +10366,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="616" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="616" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A616" t="s">
         <v>573</v>
       </c>
@@ -10365,7 +10378,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="617" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="617" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A617" t="s">
         <v>574</v>
       </c>
@@ -10377,7 +10390,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="618" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="618" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A618" t="s">
         <v>575</v>
       </c>
@@ -10389,7 +10402,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="619" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="619" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A619" t="s">
         <v>576</v>
       </c>
@@ -10401,7 +10414,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="620" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="620" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A620" t="s">
         <v>577</v>
       </c>
@@ -10413,7 +10426,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="621" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="621" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A621" t="s">
         <v>578</v>
       </c>
@@ -10425,7 +10438,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="622" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="622" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A622" t="s">
         <v>579</v>
       </c>
@@ -10437,7 +10450,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="623" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="623" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A623" t="s">
         <v>580</v>
       </c>
@@ -10461,7 +10474,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="625" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="625" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A625" t="s">
         <v>582</v>
       </c>
@@ -10509,7 +10522,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="629" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="629" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A629" t="s">
         <v>586</v>
       </c>
@@ -10521,7 +10534,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="630" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="630" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A630" t="s">
         <v>587</v>
       </c>
@@ -10533,7 +10546,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="631" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="631" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A631" t="s">
         <v>588</v>
       </c>
@@ -10545,7 +10558,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="632" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="632" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A632" t="s">
         <v>589</v>
       </c>
@@ -10557,7 +10570,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="633" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="633" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A633" t="s">
         <v>590</v>
       </c>
@@ -10569,7 +10582,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="634" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="634" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A634" t="s">
         <v>591</v>
       </c>
@@ -10581,7 +10594,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="635" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="635" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A635" t="s">
         <v>592</v>
       </c>
@@ -10593,7 +10606,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="636" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="636" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A636" t="s">
         <v>593</v>
       </c>
@@ -10605,7 +10618,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="637" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="637" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A637" t="s">
         <v>594</v>
       </c>
@@ -10617,7 +10630,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="638" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="638" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A638" t="s">
         <v>595</v>
       </c>
@@ -10629,7 +10642,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="639" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="639" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A639" t="s">
         <v>596</v>
       </c>
@@ -10641,7 +10654,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="640" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="640" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A640" t="s">
         <v>597</v>
       </c>
@@ -10654,7 +10667,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="641" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="641" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A641" t="s">
         <v>598</v>
       </c>
@@ -10666,7 +10679,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="642" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="642" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A642" t="s">
         <v>599</v>
       </c>
@@ -10678,7 +10691,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="643" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="643" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A643" t="s">
         <v>600</v>
       </c>
@@ -10690,7 +10703,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="644" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="644" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A644" t="s">
         <v>601</v>
       </c>
@@ -10702,7 +10715,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="645" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="645" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A645" t="s">
         <v>602</v>
       </c>
@@ -10738,7 +10751,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="648" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="648" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A648" t="s">
         <v>605</v>
       </c>
@@ -10750,7 +10763,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="649" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="649" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A649" t="s">
         <v>606</v>
       </c>
@@ -10762,7 +10775,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="650" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="650" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A650" t="s">
         <v>607</v>
       </c>
@@ -10798,7 +10811,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="653" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="653" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A653" t="s">
         <v>610</v>
       </c>
@@ -10810,7 +10823,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="654" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="654" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A654" t="s">
         <v>611</v>
       </c>
@@ -10822,7 +10835,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="655" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="655" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A655" t="s">
         <v>612</v>
       </c>

</xml_diff>

<commit_message>
add Neriene montana female
</commit_message>
<xml_diff>
--- a/photos.xlsx
+++ b/photos.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cedri\Documents\web\araignees_idf\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A5BCA8FC-ED4F-474C-9174-570D6549506D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{43CE82C5-169B-4307-809F-C1D6C6C4ADBF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1496" uniqueCount="844">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1497" uniqueCount="845">
   <si>
     <t>taxon</t>
   </si>
@@ -2552,6 +2552,9 @@
   </si>
   <si>
     <t>www/media/fiches/scotophaeus_scutulatus_femelle.webp</t>
+  </si>
+  <si>
+    <t>www/media/fiches/neriene_montana_femelle.webp</t>
   </si>
 </sst>
 </file>
@@ -2963,8 +2966,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E656"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A132" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="D151" sqref="D151"/>
+    <sheetView tabSelected="1" topLeftCell="A256" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="D279" sqref="D279"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -6509,6 +6512,9 @@
         <f>OR(Tableau1[[#This Row],[femelle]]&lt;&gt;"", Tableau1[[#This Row],[male]]&lt;&gt;"")</f>
         <v>1</v>
       </c>
+      <c r="D278" t="s">
+        <v>844</v>
+      </c>
       <c r="E278" t="s">
         <v>675</v>
       </c>

</xml_diff>

<commit_message>
add female Enoplognatha mandibularis
</commit_message>
<xml_diff>
--- a/photos.xlsx
+++ b/photos.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cedri\Documents\web\araignees_idf\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A1E3065A-3DF3-4B59-AEE9-D0BB87F3FD1E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B20F6A8E-9312-4F01-B811-F1877683D16E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1498" uniqueCount="846">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1499" uniqueCount="847">
   <si>
     <t>taxon</t>
   </si>
@@ -2558,6 +2558,9 @@
   </si>
   <si>
     <t>www/media/fiches/araneus_triguttatus_femelle.webp</t>
+  </si>
+  <si>
+    <t>www/media/fiches/enoplognatha_mandibularis_femelle.webp</t>
   </si>
 </sst>
 </file>
@@ -2969,8 +2972,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E656"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="D35" sqref="D35"/>
+    <sheetView tabSelected="1" topLeftCell="A539" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="D558" sqref="D558"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -10076,6 +10079,9 @@
         <f>OR(Tableau1[[#This Row],[femelle]]&lt;&gt;"", Tableau1[[#This Row],[male]]&lt;&gt;"")</f>
         <v>1</v>
       </c>
+      <c r="D557" t="s">
+        <v>846</v>
+      </c>
       <c r="E557" t="s">
         <v>826</v>
       </c>

</xml_diff>

<commit_message>
add pictures of three species
</commit_message>
<xml_diff>
--- a/photos.xlsx
+++ b/photos.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28730"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cedri\Documents\web\araignees_idf\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B20F6A8E-9312-4F01-B811-F1877683D16E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BAC17C8D-80BF-4EFF-ABFE-EFD422E75F31}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1499" uniqueCount="847">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1502" uniqueCount="850">
   <si>
     <t>taxon</t>
   </si>
@@ -2561,6 +2561,15 @@
   </si>
   <si>
     <t>www/media/fiches/enoplognatha_mandibularis_femelle.webp</t>
+  </si>
+  <si>
+    <t>www/media/fiches/pardosa_hortensis_femelle.webp</t>
+  </si>
+  <si>
+    <t>www/media/fiches/pardosa_prativaga_male.webp</t>
+  </si>
+  <si>
+    <t>www/media/fiches/eratigena_saeva_femelle.webp</t>
   </si>
 </sst>
 </file>
@@ -2972,8 +2981,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E656"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A539" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="D558" sqref="D558"/>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3113,7 +3122,10 @@
       </c>
       <c r="C10" t="b">
         <f>OR(Tableau1[[#This Row],[femelle]]&lt;&gt;"", Tableau1[[#This Row],[male]]&lt;&gt;"")</f>
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="D10" t="s">
+        <v>849</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.3">
@@ -7919,6 +7931,9 @@
         <f>OR(Tableau1[[#This Row],[femelle]]&lt;&gt;"", Tableau1[[#This Row],[male]]&lt;&gt;"")</f>
         <v>1</v>
       </c>
+      <c r="D392" t="s">
+        <v>847</v>
+      </c>
       <c r="E392" t="s">
         <v>796</v>
       </c>
@@ -7992,7 +8007,10 @@
       </c>
       <c r="C398" t="b">
         <f>OR(Tableau1[[#This Row],[femelle]]&lt;&gt;"", Tableau1[[#This Row],[male]]&lt;&gt;"")</f>
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="E398" t="s">
+        <v>848</v>
       </c>
     </row>
     <row r="399" spans="1:5" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
add Clubiona terrestris female
</commit_message>
<xml_diff>
--- a/photos.xlsx
+++ b/photos.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cedri\Documents\web\araignees_idf\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BAC17C8D-80BF-4EFF-ABFE-EFD422E75F31}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C1A300E-A91E-4AE8-AB28-767F6BEA85F1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1502" uniqueCount="850">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1503" uniqueCount="851">
   <si>
     <t>taxon</t>
   </si>
@@ -2570,6 +2570,9 @@
   </si>
   <si>
     <t>www/media/fiches/eratigena_saeva_femelle.webp</t>
+  </si>
+  <si>
+    <t>www/media/fiches/clubiona_terrestris_femelle.webp</t>
   </si>
 </sst>
 </file>
@@ -2981,8 +2984,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E656"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+    <sheetView tabSelected="1" topLeftCell="A56" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="D90" sqref="D90"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4166,6 +4169,9 @@
         <f>OR(Tableau1[[#This Row],[femelle]]&lt;&gt;"", Tableau1[[#This Row],[male]]&lt;&gt;"")</f>
         <v>1</v>
       </c>
+      <c r="D89" t="s">
+        <v>850</v>
+      </c>
       <c r="E89" t="s">
         <v>771</v>
       </c>

</xml_diff>

<commit_message>
add Civizelotes civicus female
</commit_message>
<xml_diff>
--- a/photos.xlsx
+++ b/photos.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28827"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cedri\Documents\web\araignees_idf\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C1A300E-A91E-4AE8-AB28-767F6BEA85F1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84776515-2C4C-4D0C-B25E-25755FA9A315}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1503" uniqueCount="851">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1504" uniqueCount="852">
   <si>
     <t>taxon</t>
   </si>
@@ -2573,6 +2573,9 @@
   </si>
   <si>
     <t>www/media/fiches/clubiona_terrestris_femelle.webp</t>
+  </si>
+  <si>
+    <t>www/media/fiches/civizelotes_civicus_femelle.webp</t>
   </si>
 </sst>
 </file>
@@ -2984,8 +2987,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E656"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A56" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="D90" sqref="D90"/>
+    <sheetView tabSelected="1" topLeftCell="A105" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="D117" sqref="D117"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4527,7 +4530,10 @@
       </c>
       <c r="C116" t="b">
         <f>OR(Tableau1[[#This Row],[femelle]]&lt;&gt;"", Tableau1[[#This Row],[male]]&lt;&gt;"")</f>
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="D116" t="s">
+        <v>851</v>
       </c>
     </row>
     <row r="117" spans="1:5" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
add female Runcinia grammica
</commit_message>
<xml_diff>
--- a/photos.xlsx
+++ b/photos.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cedri\Documents\web\araignees_idf\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{73513C62-E174-4883-AFB5-A04032DD0853}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{70978014-950F-4C47-8BA1-B324D823138C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1508" uniqueCount="856">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1509" uniqueCount="857">
   <si>
     <t>taxon</t>
   </si>
@@ -2588,6 +2588,9 @@
   </si>
   <si>
     <t>www/media/fiches/zora_spinimana_femelle.webp</t>
+  </si>
+  <si>
+    <t>www/media/fiches/runcinia_grammica_femelle.webp</t>
   </si>
 </sst>
 </file>
@@ -2999,8 +3002,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E656"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A625" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="D533" sqref="D533"/>
+    <sheetView tabSelected="1" topLeftCell="A622" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="D627" sqref="D627"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -11057,6 +11060,9 @@
         <f>OR(Tableau1[[#This Row],[femelle]]&lt;&gt;"", Tableau1[[#This Row],[male]]&lt;&gt;"")</f>
         <v>1</v>
       </c>
+      <c r="D626" t="s">
+        <v>856</v>
+      </c>
       <c r="E626" t="s">
         <v>755</v>
       </c>

</xml_diff>

<commit_message>
add Piratula hygrophila female
</commit_message>
<xml_diff>
--- a/photos.xlsx
+++ b/photos.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29127"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cedri\Documents\web\araignees_idf\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{090DE7E1-01C4-4E21-86BF-26130009AD75}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7367FDB-06DB-48D5-A3D8-025E39B03A34}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1510" uniqueCount="858">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1511" uniqueCount="859">
   <si>
     <t>taxon</t>
   </si>
@@ -2594,6 +2594,9 @@
   </si>
   <si>
     <t>www/media/fiches/clubiona_lutescens_femelle.webp</t>
+  </si>
+  <si>
+    <t>www/media/fiches/piratula_hygrophila_femelle.webp</t>
   </si>
 </sst>
 </file>
@@ -3005,8 +3008,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E656"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A58" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="E79" sqref="E79"/>
+    <sheetView tabSelected="1" topLeftCell="A386" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="D405" sqref="D405"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -8124,7 +8127,10 @@
       </c>
       <c r="C404" t="b">
         <f>OR(Tableau1[[#This Row],[femelle]]&lt;&gt;"", Tableau1[[#This Row],[male]]&lt;&gt;"")</f>
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="D404" t="s">
+        <v>858</v>
       </c>
     </row>
     <row r="405" spans="1:5" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
add Pardosa saltans male
</commit_message>
<xml_diff>
--- a/photos.xlsx
+++ b/photos.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cedri\Documents\web\araignees_idf\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7367FDB-06DB-48D5-A3D8-025E39B03A34}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F6B31C2-1DFF-4748-A56D-8D2C7063875E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="11424" yWindow="0" windowWidth="11712" windowHeight="12336" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet 1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1511" uniqueCount="859">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1512" uniqueCount="860">
   <si>
     <t>taxon</t>
   </si>
@@ -2597,6 +2597,9 @@
   </si>
   <si>
     <t>www/media/fiches/piratula_hygrophila_femelle.webp</t>
+  </si>
+  <si>
+    <t>www/media/fiches/pardosa_saltans_male.webp</t>
   </si>
 </sst>
 </file>
@@ -2656,7 +2659,56 @@
     <cellStyle name="Lien hypertexte" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="1">
+  <dxfs count="8">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
@@ -2679,7 +2731,7 @@
   <tableColumns count="5">
     <tableColumn id="1" xr3:uid="{8CF3FEBE-EC73-416E-8610-F705B8D6D336}" name="taxon"/>
     <tableColumn id="4" xr3:uid="{666FCC22-DD53-4830-B712-02B264DDA363}" name="id à vue"/>
-    <tableColumn id="6" xr3:uid="{6FBFF4C7-96B5-4733-BA2F-DBB356BBCD3F}" name="fiche" dataDxfId="0">
+    <tableColumn id="6" xr3:uid="{6FBFF4C7-96B5-4733-BA2F-DBB356BBCD3F}" name="fiche" dataDxfId="7">
       <calculatedColumnFormula>OR(Tableau1[[#This Row],[femelle]]&lt;&gt;"", Tableau1[[#This Row],[male]]&lt;&gt;"")</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="3" xr3:uid="{84160676-7B2A-4A0C-94B1-2901F12B1A91}" name="femelle"/>
@@ -3008,8 +3060,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E656"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A386" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="D405" sqref="D405"/>
+    <sheetView tabSelected="1" topLeftCell="B369" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="E402" sqref="E402"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -8091,7 +8143,10 @@
       </c>
       <c r="C401" t="b">
         <f>OR(Tableau1[[#This Row],[femelle]]&lt;&gt;"", Tableau1[[#This Row],[male]]&lt;&gt;"")</f>
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="E401" t="s">
+        <v>859</v>
       </c>
     </row>
     <row r="402" spans="1:5" x14ac:dyDescent="0.3">
@@ -11488,6 +11543,20 @@
       </c>
     </row>
   </sheetData>
+  <conditionalFormatting sqref="B2:C656">
+    <cfRule type="cellIs" dxfId="3" priority="4" operator="equal">
+      <formula>"oui"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="4" priority="3" operator="equal">
+      <formula>TRUE</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="5" priority="2" operator="equal">
+      <formula>"non"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="2" priority="1" operator="equal">
+      <formula>FALSE</formula>
+    </cfRule>
+  </conditionalFormatting>
   <printOptions gridLines="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>

</xml_diff>

<commit_message>
add Oxyopes lineatus female
</commit_message>
<xml_diff>
--- a/photos.xlsx
+++ b/photos.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cedri\Documents\web\araignees_idf\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F6B31C2-1DFF-4748-A56D-8D2C7063875E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{58D498A5-BD1D-454D-B124-7C0E4CBE6DE3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="11424" yWindow="0" windowWidth="11712" windowHeight="12336" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1512" uniqueCount="860">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1513" uniqueCount="861">
   <si>
     <t>taxon</t>
   </si>
@@ -2600,6 +2600,9 @@
   </si>
   <si>
     <t>www/media/fiches/pardosa_saltans_male.webp</t>
+  </si>
+  <si>
+    <t>www/media/fiches/oxyopes_lineatus_femelle.webp</t>
   </si>
 </sst>
 </file>
@@ -3060,8 +3063,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E656"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B369" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="E402" sqref="E402"/>
+    <sheetView tabSelected="1" topLeftCell="A405" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="D432" sqref="D432"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -8521,7 +8524,10 @@
       </c>
       <c r="C431" t="b">
         <f>OR(Tableau1[[#This Row],[femelle]]&lt;&gt;"", Tableau1[[#This Row],[male]]&lt;&gt;"")</f>
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="D431" t="s">
+        <v>860</v>
       </c>
     </row>
     <row r="432" spans="1:4" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
add Steatoda triangulosa female
</commit_message>
<xml_diff>
--- a/photos.xlsx
+++ b/photos.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cedri\Documents\web\araignees_idf\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{58D498A5-BD1D-454D-B124-7C0E4CBE6DE3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53FEF936-48DC-402E-8F88-1C0E657032A3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="11424" yWindow="0" windowWidth="11712" windowHeight="12336" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1513" uniqueCount="861">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1514" uniqueCount="862">
   <si>
     <t>taxon</t>
   </si>
@@ -2603,6 +2603,9 @@
   </si>
   <si>
     <t>www/media/fiches/oxyopes_lineatus_femelle.webp</t>
+  </si>
+  <si>
+    <t>www/media/fiches/steatoda_triangulosa_femelle.webp</t>
   </si>
 </sst>
 </file>
@@ -3063,8 +3066,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E656"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A405" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="D432" sqref="D432"/>
+    <sheetView tabSelected="1" topLeftCell="A577" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="D597" sqref="D597"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -10738,7 +10741,10 @@
       </c>
       <c r="C596" t="b">
         <f>OR(Tableau1[[#This Row],[femelle]]&lt;&gt;"", Tableau1[[#This Row],[male]]&lt;&gt;"")</f>
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="D596" t="s">
+        <v>861</v>
       </c>
     </row>
     <row r="597" spans="1:5" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
add Trachyzelotes pedestris female
</commit_message>
<xml_diff>
--- a/photos.xlsx
+++ b/photos.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cedri\Documents\web\araignees_idf\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53FEF936-48DC-402E-8F88-1C0E657032A3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B54DF420-6C6A-48E5-AA5B-1EAF33C8A9A4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="11424" yWindow="0" windowWidth="11712" windowHeight="12336" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1514" uniqueCount="862">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1515" uniqueCount="863">
   <si>
     <t>taxon</t>
   </si>
@@ -2606,6 +2606,9 @@
   </si>
   <si>
     <t>www/media/fiches/steatoda_triangulosa_femelle.webp</t>
+  </si>
+  <si>
+    <t>www/media/fiches/trachyzelotes_pedestris_femelle.webp</t>
   </si>
 </sst>
 </file>
@@ -3066,8 +3069,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E656"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A577" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="D597" sqref="D597"/>
+    <sheetView tabSelected="1" topLeftCell="A134" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="D153" sqref="D153"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5065,7 +5068,10 @@
       </c>
       <c r="C152" t="b">
         <f>OR(Tableau1[[#This Row],[femelle]]&lt;&gt;"", Tableau1[[#This Row],[male]]&lt;&gt;"")</f>
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="D152" t="s">
+        <v>862</v>
       </c>
     </row>
     <row r="153" spans="1:5" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
add Synema globosum male
</commit_message>
<xml_diff>
--- a/photos.xlsx
+++ b/photos.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cedri\Documents\web\araignees_idf\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B54DF420-6C6A-48E5-AA5B-1EAF33C8A9A4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9974DE99-2DEF-4186-AF2C-8413A58A5947}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11424" yWindow="0" windowWidth="11712" windowHeight="12336" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet 1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1515" uniqueCount="863">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1516" uniqueCount="864">
   <si>
     <t>taxon</t>
   </si>
@@ -2609,6 +2609,9 @@
   </si>
   <si>
     <t>www/media/fiches/trachyzelotes_pedestris_femelle.webp</t>
+  </si>
+  <si>
+    <t>www/media/fiches/synema_globosum_male.webp</t>
   </si>
 </sst>
 </file>
@@ -2668,28 +2671,7 @@
     <cellStyle name="Lien hypertexte" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="8">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="5">
     <dxf>
       <fill>
         <patternFill>
@@ -2714,7 +2696,7 @@
     <dxf>
       <fill>
         <patternFill>
-          <bgColor theme="9"/>
+          <bgColor theme="5"/>
         </patternFill>
       </fill>
     </dxf>
@@ -2740,7 +2722,7 @@
   <tableColumns count="5">
     <tableColumn id="1" xr3:uid="{8CF3FEBE-EC73-416E-8610-F705B8D6D336}" name="taxon"/>
     <tableColumn id="4" xr3:uid="{666FCC22-DD53-4830-B712-02B264DDA363}" name="id à vue"/>
-    <tableColumn id="6" xr3:uid="{6FBFF4C7-96B5-4733-BA2F-DBB356BBCD3F}" name="fiche" dataDxfId="7">
+    <tableColumn id="6" xr3:uid="{6FBFF4C7-96B5-4733-BA2F-DBB356BBCD3F}" name="fiche" dataDxfId="4">
       <calculatedColumnFormula>OR(Tableau1[[#This Row],[femelle]]&lt;&gt;"", Tableau1[[#This Row],[male]]&lt;&gt;"")</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="3" xr3:uid="{84160676-7B2A-4A0C-94B1-2901F12B1A91}" name="femelle"/>
@@ -3069,8 +3051,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E656"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A134" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="D153" sqref="D153"/>
+    <sheetView tabSelected="1" topLeftCell="A609" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="E628" sqref="E628"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -11166,6 +11148,9 @@
       <c r="D627" t="s">
         <v>759</v>
       </c>
+      <c r="E627" t="s">
+        <v>863</v>
+      </c>
     </row>
     <row r="628" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A628" t="s">
@@ -11562,17 +11547,17 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="B2:C656">
-    <cfRule type="cellIs" dxfId="3" priority="4" operator="equal">
-      <formula>"oui"</formula>
+    <cfRule type="cellIs" dxfId="3" priority="1" operator="equal">
+      <formula>FALSE</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="4" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="2" priority="2" operator="equal">
+      <formula>"non"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="1" priority="3" operator="equal">
       <formula>TRUE</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="5" priority="2" operator="equal">
-      <formula>"non"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="1" operator="equal">
-      <formula>FALSE</formula>
+    <cfRule type="cellIs" dxfId="0" priority="4" operator="equal">
+      <formula>"oui"</formula>
     </cfRule>
   </conditionalFormatting>
   <printOptions gridLines="1"/>

</xml_diff>

<commit_message>
add Pardosa agrestis female
</commit_message>
<xml_diff>
--- a/photos.xlsx
+++ b/photos.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cedri\Documents\web\araignees_idf\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9974DE99-2DEF-4186-AF2C-8413A58A5947}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C94532A-A317-496F-96CD-05EC3C72BC59}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1516" uniqueCount="864">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1517" uniqueCount="865">
   <si>
     <t>taxon</t>
   </si>
@@ -2612,6 +2612,9 @@
   </si>
   <si>
     <t>www/media/fiches/synema_globosum_male.webp</t>
+  </si>
+  <si>
+    <t>www/media/fiches/pardosa_agrestis_femelle.webp</t>
   </si>
 </sst>
 </file>
@@ -3051,8 +3054,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E656"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A609" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="E628" sqref="E628"/>
+    <sheetView tabSelected="1" topLeftCell="A370" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="D389" sqref="D389"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -7972,7 +7975,10 @@
       </c>
       <c r="C388" t="b">
         <f>OR(Tableau1[[#This Row],[femelle]]&lt;&gt;"", Tableau1[[#This Row],[male]]&lt;&gt;"")</f>
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="D388" t="s">
+        <v>864</v>
       </c>
     </row>
     <row r="389" spans="1:5" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
add Lathys humilis female
</commit_message>
<xml_diff>
--- a/photos.xlsx
+++ b/photos.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cedri\Documents\web\araignees_idf\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C94532A-A317-496F-96CD-05EC3C72BC59}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{742C5D92-DCAF-4920-80BD-323990B5A325}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1517" uniqueCount="865">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1518" uniqueCount="866">
   <si>
     <t>taxon</t>
   </si>
@@ -2615,6 +2615,9 @@
   </si>
   <si>
     <t>www/media/fiches/pardosa_agrestis_femelle.webp</t>
+  </si>
+  <si>
+    <t>www/media/fiches/lathys_humilis_femelle.webp</t>
   </si>
 </sst>
 </file>
@@ -3054,8 +3057,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E656"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A370" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="D389" sqref="D389"/>
+    <sheetView tabSelected="1" topLeftCell="A85" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="D104" sqref="D104"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4430,6 +4433,9 @@
       <c r="C103" t="b">
         <f>OR(Tableau1[[#This Row],[femelle]]&lt;&gt;"", Tableau1[[#This Row],[male]]&lt;&gt;"")</f>
         <v>1</v>
+      </c>
+      <c r="D103" t="s">
+        <v>865</v>
       </c>
       <c r="E103" t="s">
         <v>773</v>

</xml_diff>

<commit_message>
add Ozyptila sanctuaria male
</commit_message>
<xml_diff>
--- a/photos.xlsx
+++ b/photos.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cedri\Documents\web\araignees_idf\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{742C5D92-DCAF-4920-80BD-323990B5A325}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED7EE921-2948-4F61-BCE8-7105D949F8EC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,11 +16,12 @@
     <sheet name="Sheet 1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
+  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1518" uniqueCount="866">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1519" uniqueCount="867">
   <si>
     <t>taxon</t>
   </si>
@@ -2618,6 +2619,9 @@
   </si>
   <si>
     <t>www/media/fiches/lathys_humilis_femelle.webp</t>
+  </si>
+  <si>
+    <t>www/media/fiches/ozyptila_sanctuaria_male.webp</t>
   </si>
 </sst>
 </file>
@@ -3057,8 +3061,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E656"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A85" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="D104" sqref="D104"/>
+    <sheetView tabSelected="1" topLeftCell="A603" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="E622" sqref="E622"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -11074,7 +11078,10 @@
       </c>
       <c r="C621" t="b">
         <f>OR(Tableau1[[#This Row],[femelle]]&lt;&gt;"", Tableau1[[#This Row],[male]]&lt;&gt;"")</f>
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="E621" t="s">
+        <v>866</v>
       </c>
     </row>
     <row r="622" spans="1:5" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
add two females (P. simoni an T. nigrita)
</commit_message>
<xml_diff>
--- a/photos.xlsx
+++ b/photos.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29231"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cedri\Documents\web\araignees_idf\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED7EE921-2948-4F61-BCE8-7105D949F8EC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{42E3A230-D770-47F2-A445-B75F7420AEB4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,12 +16,11 @@
     <sheet name="Sheet 1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
-  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1519" uniqueCount="867">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1521" uniqueCount="869">
   <si>
     <t>taxon</t>
   </si>
@@ -2622,6 +2621,12 @@
   </si>
   <si>
     <t>www/media/fiches/ozyptila_sanctuaria_male.webp</t>
+  </si>
+  <si>
+    <t>www/media/fiches/tetragnatha_nigrita_femelle.webp</t>
+  </si>
+  <si>
+    <t>www/media/fiches/psilochorus_simoni_femelle.webp</t>
   </si>
 </sst>
 </file>
@@ -3061,8 +3066,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E656"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A603" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="E622" sqref="E622"/>
+    <sheetView tabSelected="1" topLeftCell="A440" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="D459" sqref="D459"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -8896,6 +8901,9 @@
         <f>OR(Tableau1[[#This Row],[femelle]]&lt;&gt;"", Tableau1[[#This Row],[male]]&lt;&gt;"")</f>
         <v>1</v>
       </c>
+      <c r="D458" t="s">
+        <v>868</v>
+      </c>
       <c r="E458" t="s">
         <v>705</v>
       </c>
@@ -10016,7 +10024,10 @@
       </c>
       <c r="C541" t="b">
         <f>OR(Tableau1[[#This Row],[femelle]]&lt;&gt;"", Tableau1[[#This Row],[male]]&lt;&gt;"")</f>
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="D541" t="s">
+        <v>867</v>
       </c>
     </row>
     <row r="542" spans="1:5" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
add male Argiope bruennichi
</commit_message>
<xml_diff>
--- a/photos.xlsx
+++ b/photos.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29328"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cedri\Documents\web\araignees_idf\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{42E3A230-D770-47F2-A445-B75F7420AEB4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B8451F4-8C6E-4FCF-A521-8CD43B70CEFA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1521" uniqueCount="869">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1522" uniqueCount="870">
   <si>
     <t>taxon</t>
   </si>
@@ -2627,6 +2627,9 @@
   </si>
   <si>
     <t>www/media/fiches/psilochorus_simoni_femelle.webp</t>
+  </si>
+  <si>
+    <t>www/media/fiches/argiope_bruennichi_male.webp</t>
   </si>
 </sst>
 </file>
@@ -3066,8 +3069,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E656"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A440" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="D459" sqref="D459"/>
+    <sheetView tabSelected="1" topLeftCell="A20" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="E39" sqref="E39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3595,6 +3598,9 @@
       </c>
       <c r="D38" t="s">
         <v>683</v>
+      </c>
+      <c r="E38" t="s">
+        <v>869</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
add Salticus scenicus female
</commit_message>
<xml_diff>
--- a/photos.xlsx
+++ b/photos.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29426"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cedri\Documents\web\araignees_idf\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B8451F4-8C6E-4FCF-A521-8CD43B70CEFA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{32A6BCB8-D5C7-4383-9041-5124B7C4F269}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1522" uniqueCount="870">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1523" uniqueCount="871">
   <si>
     <t>taxon</t>
   </si>
@@ -2630,6 +2630,9 @@
   </si>
   <si>
     <t>www/media/fiches/argiope_bruennichi_male.webp</t>
+  </si>
+  <si>
+    <t>www/media/fiches/salticus_scenicus_femelle.webp</t>
   </si>
 </sst>
 </file>
@@ -3069,8 +3072,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E656"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A20" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="E39" sqref="E39"/>
+    <sheetView tabSelected="1" topLeftCell="A495" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="D514" sqref="D514"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -9650,6 +9653,9 @@
       <c r="C513" t="b">
         <f>OR(Tableau1[[#This Row],[femelle]]&lt;&gt;"", Tableau1[[#This Row],[male]]&lt;&gt;"")</f>
         <v>1</v>
+      </c>
+      <c r="D513" t="s">
+        <v>870</v>
       </c>
       <c r="E513" t="s">
         <v>731</v>

</xml_diff>

<commit_message>
add Philodromus aureolus male
</commit_message>
<xml_diff>
--- a/photos.xlsx
+++ b/photos.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cedri\Documents\web\araignees_idf\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{32A6BCB8-D5C7-4383-9041-5124B7C4F269}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7C14410-53FC-4A21-B3DD-AF01AB423E15}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,11 +16,12 @@
     <sheet name="Sheet 1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
+  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1523" uniqueCount="871">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1524" uniqueCount="872">
   <si>
     <t>taxon</t>
   </si>
@@ -2633,6 +2634,9 @@
   </si>
   <si>
     <t>www/media/fiches/salticus_scenicus_femelle.webp</t>
+  </si>
+  <si>
+    <t>www/media/fiches/philodromus_aureolus_male.webp</t>
   </si>
 </sst>
 </file>
@@ -3072,8 +3076,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E656"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A495" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="D514" sqref="D514"/>
+    <sheetView tabSelected="1" topLeftCell="A416" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="E436" sqref="E436"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -8606,6 +8610,9 @@
       </c>
       <c r="D435" t="s">
         <v>801</v>
+      </c>
+      <c r="E435" t="s">
+        <v>871</v>
       </c>
     </row>
     <row r="436" spans="1:5" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
ajoute Enoplognatha mordax mâle
</commit_message>
<xml_diff>
--- a/photos.xlsx
+++ b/photos.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cedri\Documents\web\araignees_idf\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7C14410-53FC-4A21-B3DD-AF01AB423E15}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{263ABDA9-CE19-4CBE-BEA4-B2D2016A8150}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12432" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet 1" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1524" uniqueCount="872">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1525" uniqueCount="873">
   <si>
     <t>taxon</t>
   </si>
@@ -2637,6 +2637,9 @@
   </si>
   <si>
     <t>www/media/fiches/philodromus_aureolus_male.webp</t>
+  </si>
+  <si>
+    <t>www/media/fiches/enoplognatha_mordax_male.webp</t>
   </si>
 </sst>
 </file>
@@ -3076,8 +3079,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E656"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A416" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="E436" sqref="E436"/>
+    <sheetView tabSelected="1" topLeftCell="A540" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="E559" sqref="E559"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -10262,7 +10265,10 @@
       </c>
       <c r="C558" t="b">
         <f>OR(Tableau1[[#This Row],[femelle]]&lt;&gt;"", Tableau1[[#This Row],[male]]&lt;&gt;"")</f>
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="E558" t="s">
+        <v>872</v>
       </c>
     </row>
     <row r="559" spans="1:5" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
ajoute Dictyna uncinata mâle
</commit_message>
<xml_diff>
--- a/photos.xlsx
+++ b/photos.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cedri\Documents\web\araignees_idf\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{263ABDA9-CE19-4CBE-BEA4-B2D2016A8150}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{931DB368-9636-4C09-99CD-98F4EDA9F422}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12432" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet 1" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1525" uniqueCount="873">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1526" uniqueCount="874">
   <si>
     <t>taxon</t>
   </si>
@@ -2640,6 +2640,9 @@
   </si>
   <si>
     <t>www/media/fiches/enoplognatha_mordax_male.webp</t>
+  </si>
+  <si>
+    <t>www/media/fiches/dictyna_uncinata_male.webp</t>
   </si>
 </sst>
 </file>
@@ -3079,8 +3082,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E656"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A540" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="E559" sqref="E559"/>
+    <sheetView tabSelected="1" topLeftCell="A83" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="E102" sqref="E102"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4434,6 +4437,9 @@
       </c>
       <c r="D101" t="s">
         <v>772</v>
+      </c>
+      <c r="E101" t="s">
+        <v>873</v>
       </c>
     </row>
     <row r="102" spans="1:5" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
ajoute Philodromus rufus femelle
</commit_message>
<xml_diff>
--- a/photos.xlsx
+++ b/photos.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29426"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29530"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cedri\Documents\web\araignees_idf\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{931DB368-9636-4C09-99CD-98F4EDA9F422}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7EBEC59B-4C1F-47DA-A089-0F4DF34C045A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,12 +16,11 @@
     <sheet name="Sheet 1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
-  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1526" uniqueCount="874">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1527" uniqueCount="875">
   <si>
     <t>taxon</t>
   </si>
@@ -2643,6 +2642,9 @@
   </si>
   <si>
     <t>www/media/fiches/dictyna_uncinata_male.webp</t>
+  </si>
+  <si>
+    <t>www/media/fiches/philodromus_rufus_femelle.webp</t>
   </si>
 </sst>
 </file>
@@ -3082,8 +3084,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E656"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A83" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="E102" sqref="E102"/>
+    <sheetView tabSelected="1" topLeftCell="A427" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="D446" sqref="D446"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -8756,7 +8758,10 @@
       </c>
       <c r="C445" t="b">
         <f>OR(Tableau1[[#This Row],[femelle]]&lt;&gt;"", Tableau1[[#This Row],[male]]&lt;&gt;"")</f>
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="D445" t="s">
+        <v>874</v>
       </c>
     </row>
     <row r="446" spans="1:5" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
compresse photos et ajoute Neriene clathrata femelle
</commit_message>
<xml_diff>
--- a/photos.xlsx
+++ b/photos.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29530"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29628"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cedri\Documents\web\araignees_idf\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7EBEC59B-4C1F-47DA-A089-0F4DF34C045A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D96419D-E2B2-4A96-A4E0-16EEEE0AB251}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1527" uniqueCount="875">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1528" uniqueCount="876">
   <si>
     <t>taxon</t>
   </si>
@@ -2645,6 +2645,9 @@
   </si>
   <si>
     <t>www/media/fiches/philodromus_rufus_femelle.webp</t>
+  </si>
+  <si>
+    <t>www/media/fiches/neriene_clathrata_femelle.webp</t>
   </si>
 </sst>
 </file>
@@ -3084,8 +3087,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E656"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A427" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="D446" sqref="D446"/>
+    <sheetView tabSelected="1" topLeftCell="A256" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="D275" sqref="D275"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -6613,7 +6616,10 @@
       </c>
       <c r="C274" t="b">
         <f>OR(Tableau1[[#This Row],[femelle]]&lt;&gt;"", Tableau1[[#This Row],[male]]&lt;&gt;"")</f>
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="D274" t="s">
+        <v>875</v>
       </c>
     </row>
     <row r="275" spans="1:5" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
ajoute Pachygnatha degeeri femelle
</commit_message>
<xml_diff>
--- a/photos.xlsx
+++ b/photos.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cedri\Documents\web\araignees_idf\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D96419D-E2B2-4A96-A4E0-16EEEE0AB251}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA6A04F8-4D9C-4BA0-B723-E4E017D138B2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1528" uniqueCount="876">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1529" uniqueCount="877">
   <si>
     <t>taxon</t>
   </si>
@@ -2648,6 +2648,9 @@
   </si>
   <si>
     <t>www/media/fiches/neriene_clathrata_femelle.webp</t>
+  </si>
+  <si>
+    <t>www/media/fiches/pachygnatha_degeeri_femelle.webp</t>
   </si>
 </sst>
 </file>
@@ -3087,8 +3090,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E656"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A256" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="D275" sqref="D275"/>
+    <sheetView tabSelected="1" topLeftCell="A517" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="D537" sqref="D537"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -9986,6 +9989,9 @@
       <c r="C536" t="b">
         <f>OR(Tableau1[[#This Row],[femelle]]&lt;&gt;"", Tableau1[[#This Row],[male]]&lt;&gt;"")</f>
         <v>1</v>
+      </c>
+      <c r="D536" t="s">
+        <v>876</v>
       </c>
       <c r="E536" t="s">
         <v>736</v>

</xml_diff>

<commit_message>
ajoute Aelurillus v-insignitus femelle
</commit_message>
<xml_diff>
--- a/photos.xlsx
+++ b/photos.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cedri\Documents\web\araignees_idf\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA6A04F8-4D9C-4BA0-B723-E4E017D138B2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7251789-35C1-4177-B8E6-1A3F20A60296}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1529" uniqueCount="877">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1530" uniqueCount="878">
   <si>
     <t>taxon</t>
   </si>
@@ -2651,6 +2651,9 @@
   </si>
   <si>
     <t>www/media/fiches/pachygnatha_degeeri_femelle.webp</t>
+  </si>
+  <si>
+    <t>www/media/fiches/aelurillus_v-insignatus_femelle.webp</t>
   </si>
 </sst>
 </file>
@@ -3090,8 +3093,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E656"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A517" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="D537" sqref="D537"/>
+    <sheetView tabSelected="1" topLeftCell="A460" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="D466" sqref="D466"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -9034,7 +9037,10 @@
       </c>
       <c r="C465" t="b">
         <f>OR(Tableau1[[#This Row],[femelle]]&lt;&gt;"", Tableau1[[#This Row],[male]]&lt;&gt;"")</f>
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="D465" t="s">
+        <v>877</v>
       </c>
     </row>
     <row r="466" spans="1:5" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
ajoute Agalenatea redii femelle
</commit_message>
<xml_diff>
--- a/photos.xlsx
+++ b/photos.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cedri\Documents\web\araignees_idf\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7251789-35C1-4177-B8E6-1A3F20A60296}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{220917A6-5631-4E41-AC79-39CE4998F046}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1530" uniqueCount="878">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1531" uniqueCount="879">
   <si>
     <t>taxon</t>
   </si>
@@ -2654,6 +2654,9 @@
   </si>
   <si>
     <t>www/media/fiches/aelurillus_v-insignatus_femelle.webp</t>
+  </si>
+  <si>
+    <t>www/media/fiches/agalenatea_redii_femelle.webp</t>
   </si>
 </sst>
 </file>
@@ -3093,8 +3096,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E656"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A460" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="D466" sqref="D466"/>
+    <sheetView tabSelected="1" topLeftCell="A9" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="D28" sqref="D28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3456,7 +3459,10 @@
       </c>
       <c r="C27" t="b">
         <f>OR(Tableau1[[#This Row],[femelle]]&lt;&gt;"", Tableau1[[#This Row],[male]]&lt;&gt;"")</f>
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="D27" t="s">
+        <v>878</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
ajoute Alopecosa cuneata mâle
</commit_message>
<xml_diff>
--- a/photos.xlsx
+++ b/photos.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cedri\Documents\web\araignees_idf\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{220917A6-5631-4E41-AC79-39CE4998F046}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6242C66B-AAA6-46BC-A2D0-51FD29F592DC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1531" uniqueCount="879">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1532" uniqueCount="880">
   <si>
     <t>taxon</t>
   </si>
@@ -2657,6 +2657,9 @@
   </si>
   <si>
     <t>www/media/fiches/agalenatea_redii_femelle.webp</t>
+  </si>
+  <si>
+    <t>www/media/fiches/alopecosa_cuneata_male.webp</t>
   </si>
 </sst>
 </file>
@@ -3096,8 +3099,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E656"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="D28" sqref="D28"/>
+    <sheetView tabSelected="1" topLeftCell="A355" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="E374" sqref="E374"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -7792,7 +7795,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="369" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="369" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A369" t="s">
         <v>339</v>
       </c>
@@ -7804,7 +7807,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="370" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="370" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A370" t="s">
         <v>340</v>
       </c>
@@ -7816,7 +7819,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="371" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="371" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A371" t="s">
         <v>341</v>
       </c>
@@ -7828,7 +7831,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="372" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="372" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A372" t="s">
         <v>342</v>
       </c>
@@ -7840,7 +7843,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="373" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="373" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A373" t="s">
         <v>343</v>
       </c>
@@ -7849,10 +7852,13 @@
       </c>
       <c r="C373" t="b">
         <f>OR(Tableau1[[#This Row],[femelle]]&lt;&gt;"", Tableau1[[#This Row],[male]]&lt;&gt;"")</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="374" spans="1:3" x14ac:dyDescent="0.3">
+        <v>1</v>
+      </c>
+      <c r="E373" t="s">
+        <v>879</v>
+      </c>
+    </row>
+    <row r="374" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A374" t="s">
         <v>344</v>
       </c>
@@ -7864,7 +7870,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="375" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="375" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A375" t="s">
         <v>345</v>
       </c>
@@ -7876,7 +7882,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="376" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="376" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A376" t="s">
         <v>346</v>
       </c>
@@ -7888,7 +7894,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="377" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="377" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A377" t="s">
         <v>347</v>
       </c>
@@ -7900,7 +7906,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="378" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="378" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A378" t="s">
         <v>348</v>
       </c>
@@ -7912,7 +7918,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="379" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="379" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A379" t="s">
         <v>349</v>
       </c>
@@ -7924,7 +7930,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="380" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="380" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A380" t="s">
         <v>350</v>
       </c>
@@ -7936,7 +7942,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="381" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="381" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A381" t="s">
         <v>351</v>
       </c>
@@ -7948,7 +7954,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="382" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="382" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A382" t="s">
         <v>352</v>
       </c>
@@ -7960,7 +7966,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="383" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="383" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A383" t="s">
         <v>353</v>
       </c>
@@ -7972,7 +7978,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="384" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="384" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A384" t="s">
         <v>354</v>
       </c>

</xml_diff>

<commit_message>
ajoute Alopecosa fabrilis femelle
</commit_message>
<xml_diff>
--- a/photos.xlsx
+++ b/photos.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cedri\Documents\web\araignees_idf\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6242C66B-AAA6-46BC-A2D0-51FD29F592DC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1247ECFD-C6A4-44D2-BCEB-D3CA7509330D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,11 +16,12 @@
     <sheet name="Sheet 1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
+  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1532" uniqueCount="880">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1533" uniqueCount="881">
   <si>
     <t>taxon</t>
   </si>
@@ -2660,6 +2661,9 @@
   </si>
   <si>
     <t>www/media/fiches/alopecosa_cuneata_male.webp</t>
+  </si>
+  <si>
+    <t>www/media/fiches/alopecosa_fabrilis_femelle.webp</t>
   </si>
 </sst>
 </file>
@@ -3100,7 +3104,7 @@
   <dimension ref="A1:E656"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A355" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="E374" sqref="E374"/>
+      <selection activeCell="D375" sqref="D375"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -7867,7 +7871,10 @@
       </c>
       <c r="C374" t="b">
         <f>OR(Tableau1[[#This Row],[femelle]]&lt;&gt;"", Tableau1[[#This Row],[male]]&lt;&gt;"")</f>
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="D374" t="s">
+        <v>880</v>
       </c>
     </row>
     <row r="375" spans="1:5" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
ajoute Araneus alsine femelle
</commit_message>
<xml_diff>
--- a/photos.xlsx
+++ b/photos.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cedri\Documents\web\araignees_idf\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1247ECFD-C6A4-44D2-BCEB-D3CA7509330D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E7ABE09-B289-4345-96EA-18D6C391D24F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1533" uniqueCount="881">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1534" uniqueCount="882">
   <si>
     <t>taxon</t>
   </si>
@@ -2664,6 +2664,9 @@
   </si>
   <si>
     <t>www/media/fiches/alopecosa_fabrilis_femelle.webp</t>
+  </si>
+  <si>
+    <t>www/media/fiches/araneus_alsine_femelle.webp</t>
   </si>
 </sst>
 </file>
@@ -3103,8 +3106,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E656"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A355" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="D375" sqref="D375"/>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="D29" sqref="D29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3481,7 +3484,10 @@
       </c>
       <c r="C28" t="b">
         <f>OR(Tableau1[[#This Row],[femelle]]&lt;&gt;"", Tableau1[[#This Row],[male]]&lt;&gt;"")</f>
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="D28" t="s">
+        <v>881</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
ajoute Arctosa perita femelle
</commit_message>
<xml_diff>
--- a/photos.xlsx
+++ b/photos.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cedri\Documents\web\araignees_idf\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E7ABE09-B289-4345-96EA-18D6C391D24F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CCE47B16-F256-4F88-8177-D25EFC3FA449}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1534" uniqueCount="882">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1535" uniqueCount="883">
   <si>
     <t>taxon</t>
   </si>
@@ -2664,6 +2664,9 @@
   </si>
   <si>
     <t>www/media/fiches/alopecosa_fabrilis_femelle.webp</t>
+  </si>
+  <si>
+    <t>www/media/fiches/arctosa_perita_femelle.webp</t>
   </si>
   <si>
     <t>www/media/fiches/araneus_alsine_femelle.webp</t>
@@ -3106,8 +3109,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E656"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="D29" sqref="D29"/>
+    <sheetView tabSelected="1" topLeftCell="A365" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="D384" sqref="D384"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3487,7 +3490,7 @@
         <v>1</v>
       </c>
       <c r="D28" t="s">
-        <v>881</v>
+        <v>882</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.3">
@@ -7988,7 +7991,10 @@
       </c>
       <c r="C383" t="b">
         <f>OR(Tableau1[[#This Row],[femelle]]&lt;&gt;"", Tableau1[[#This Row],[male]]&lt;&gt;"")</f>
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="D383" t="s">
+        <v>881</v>
       </c>
     </row>
     <row r="384" spans="1:5" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
ajoute Asagena phalerata male
</commit_message>
<xml_diff>
--- a/photos.xlsx
+++ b/photos.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cedri\Documents\web\araignees_idf\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CCE47B16-F256-4F88-8177-D25EFC3FA449}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{206193EF-AA60-415A-89EA-B437FF8A306B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1535" uniqueCount="883">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1536" uniqueCount="884">
   <si>
     <t>taxon</t>
   </si>
@@ -2670,6 +2670,9 @@
   </si>
   <si>
     <t>www/media/fiches/araneus_alsine_femelle.webp</t>
+  </si>
+  <si>
+    <t>www/media/fiches/asagena_phalerata_male.webp</t>
   </si>
 </sst>
 </file>
@@ -3109,8 +3112,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E656"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A365" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="D384" sqref="D384"/>
+    <sheetView tabSelected="1" topLeftCell="A529" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="E548" sqref="E548"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -10181,7 +10184,10 @@
       </c>
       <c r="C547" t="b">
         <f>OR(Tableau1[[#This Row],[femelle]]&lt;&gt;"", Tableau1[[#This Row],[male]]&lt;&gt;"")</f>
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="E547" t="s">
+        <v>883</v>
       </c>
     </row>
     <row r="548" spans="1:5" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
ajoute Ballus rufipes femelle
</commit_message>
<xml_diff>
--- a/photos.xlsx
+++ b/photos.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cedri\Documents\web\araignees_idf\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{206193EF-AA60-415A-89EA-B437FF8A306B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1777529B-5605-4E35-97FE-7EE4D670BC68}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1536" uniqueCount="884">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1537" uniqueCount="885">
   <si>
     <t>taxon</t>
   </si>
@@ -2673,6 +2673,9 @@
   </si>
   <si>
     <t>www/media/fiches/asagena_phalerata_male.webp</t>
+  </si>
+  <si>
+    <t>www/media/fiches/ballus_rufipes_femelle.webp</t>
   </si>
 </sst>
 </file>
@@ -3112,8 +3115,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E656"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A529" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="E548" sqref="E548"/>
+    <sheetView tabSelected="1" topLeftCell="A453" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="D473" sqref="D473"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -9164,7 +9167,10 @@
       </c>
       <c r="C472" t="b">
         <f>OR(Tableau1[[#This Row],[femelle]]&lt;&gt;"", Tableau1[[#This Row],[male]]&lt;&gt;"")</f>
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="D472" t="s">
+        <v>884</v>
       </c>
     </row>
     <row r="473" spans="1:5" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
ajoute Evarcha arcuata male
</commit_message>
<xml_diff>
--- a/photos.xlsx
+++ b/photos.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cedri\Documents\web\araignees_idf\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1777529B-5605-4E35-97FE-7EE4D670BC68}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F0928954-1256-41A1-97A4-B6CF1FB79115}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1537" uniqueCount="885">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1538" uniqueCount="886">
   <si>
     <t>taxon</t>
   </si>
@@ -2676,6 +2676,9 @@
   </si>
   <si>
     <t>www/media/fiches/ballus_rufipes_femelle.webp</t>
+  </si>
+  <si>
+    <t>www/media/fiches/evarcha_arcuata_male.webp</t>
   </si>
 </sst>
 </file>
@@ -3116,7 +3119,7 @@
   <dimension ref="A1:E656"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A453" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="D473" sqref="D473"/>
+      <selection activeCell="E478" sqref="E478"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -9243,6 +9246,9 @@
       </c>
       <c r="D477" t="s">
         <v>715</v>
+      </c>
+      <c r="E477" t="s">
+        <v>885</v>
       </c>
     </row>
     <row r="478" spans="1:5" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
ajoute Floronia bucculenta femelle
</commit_message>
<xml_diff>
--- a/photos.xlsx
+++ b/photos.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cedri\Documents\web\araignees_idf\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F0928954-1256-41A1-97A4-B6CF1FB79115}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3DB9F91B-9320-405A-A6B0-14BAD4583A35}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1538" uniqueCount="886">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1539" uniqueCount="887">
   <si>
     <t>taxon</t>
   </si>
@@ -2679,6 +2679,9 @@
   </si>
   <si>
     <t>www/media/fiches/evarcha_arcuata_male.webp</t>
+  </si>
+  <si>
+    <t>www/media/fiches/floronia_bucculenta_femelle.webp</t>
   </si>
 </sst>
 </file>
@@ -3118,8 +3121,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E656"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A453" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="E478" sqref="E478"/>
+    <sheetView tabSelected="1" topLeftCell="A207" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="D226" sqref="D226"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -6035,7 +6038,10 @@
       </c>
       <c r="C225" t="b">
         <f>OR(Tableau1[[#This Row],[femelle]]&lt;&gt;"", Tableau1[[#This Row],[male]]&lt;&gt;"")</f>
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="D225" t="s">
+        <v>886</v>
       </c>
     </row>
     <row r="226" spans="1:5" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
ajoute Gibbaranea bituberculata femelle
</commit_message>
<xml_diff>
--- a/photos.xlsx
+++ b/photos.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cedri\Documents\web\araignees_idf\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3DB9F91B-9320-405A-A6B0-14BAD4583A35}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{167083B6-AB67-4E3A-8E30-8FFE84ADAF86}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1539" uniqueCount="887">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1540" uniqueCount="888">
   <si>
     <t>taxon</t>
   </si>
@@ -2670,6 +2670,9 @@
   </si>
   <si>
     <t>www/media/fiches/araneus_alsine_femelle.webp</t>
+  </si>
+  <si>
+    <t>www/media/fiches/gibbaranea_bituberculata_femelle.webp</t>
   </si>
   <si>
     <t>www/media/fiches/asagena_phalerata_male.webp</t>
@@ -3121,8 +3124,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E656"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A207" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="D226" sqref="D226"/>
+    <sheetView tabSelected="1" topLeftCell="A24" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="D43" sqref="D43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3712,7 +3715,10 @@
       </c>
       <c r="C42" t="b">
         <f>OR(Tableau1[[#This Row],[femelle]]&lt;&gt;"", Tableau1[[#This Row],[male]]&lt;&gt;"")</f>
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="D42" t="s">
+        <v>883</v>
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.3">
@@ -6041,7 +6047,7 @@
         <v>1</v>
       </c>
       <c r="D225" t="s">
-        <v>886</v>
+        <v>887</v>
       </c>
     </row>
     <row r="226" spans="1:5" x14ac:dyDescent="0.3">
@@ -9179,7 +9185,7 @@
         <v>1</v>
       </c>
       <c r="D472" t="s">
-        <v>884</v>
+        <v>885</v>
       </c>
     </row>
     <row r="473" spans="1:5" x14ac:dyDescent="0.3">
@@ -9254,7 +9260,7 @@
         <v>715</v>
       </c>
       <c r="E477" t="s">
-        <v>885</v>
+        <v>886</v>
       </c>
     </row>
     <row r="478" spans="1:5" x14ac:dyDescent="0.3">
@@ -10205,7 +10211,7 @@
         <v>1</v>
       </c>
       <c r="E547" t="s">
-        <v>883</v>
+        <v>884</v>
       </c>
     </row>
     <row r="548" spans="1:5" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
ajoute Heriaeus graminicola femelle
</commit_message>
<xml_diff>
--- a/photos.xlsx
+++ b/photos.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cedri\Documents\web\araignees_idf\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{167083B6-AB67-4E3A-8E30-8FFE84ADAF86}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E8381C9-1F4F-46D6-8BEE-6B33786D64F7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1540" uniqueCount="888">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1541" uniqueCount="889">
   <si>
     <t>taxon</t>
   </si>
@@ -2685,6 +2685,9 @@
   </si>
   <si>
     <t>www/media/fiches/floronia_bucculenta_femelle.webp</t>
+  </si>
+  <si>
+    <t>www/media/fiches/heriaeus_graminicola_femelle.webp</t>
   </si>
 </sst>
 </file>
@@ -3124,8 +3127,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E656"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A24" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="D43" sqref="D43"/>
+    <sheetView tabSelected="1" topLeftCell="A595" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="D613" sqref="D613"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -11093,7 +11096,10 @@
       </c>
       <c r="C613" t="b">
         <f>OR(Tableau1[[#This Row],[femelle]]&lt;&gt;"", Tableau1[[#This Row],[male]]&lt;&gt;"")</f>
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="D613" t="s">
+        <v>888</v>
       </c>
     </row>
     <row r="614" spans="1:5" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
ajoute Hogna radiata mâle
</commit_message>
<xml_diff>
--- a/photos.xlsx
+++ b/photos.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cedri\Documents\web\araignees_idf\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E8381C9-1F4F-46D6-8BEE-6B33786D64F7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{02B49ACA-2661-451C-9EF7-6420BB61E59C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1541" uniqueCount="889">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1542" uniqueCount="890">
   <si>
     <t>taxon</t>
   </si>
@@ -2688,6 +2688,9 @@
   </si>
   <si>
     <t>www/media/fiches/heriaeus_graminicola_femelle.webp</t>
+  </si>
+  <si>
+    <t>www/media/fiches/hogna_radiata_male.webp</t>
   </si>
 </sst>
 </file>
@@ -3127,8 +3130,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E656"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A595" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="D613" sqref="D613"/>
+    <sheetView tabSelected="1" topLeftCell="A368" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="E387" sqref="E387"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -8057,7 +8060,10 @@
       </c>
       <c r="C386" t="b">
         <f>OR(Tableau1[[#This Row],[femelle]]&lt;&gt;"", Tableau1[[#This Row],[male]]&lt;&gt;"")</f>
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="E386" t="s">
+        <v>889</v>
       </c>
     </row>
     <row r="387" spans="1:5" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
ajoute Hypsosinga albovittata femelle
</commit_message>
<xml_diff>
--- a/photos.xlsx
+++ b/photos.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cedri\Documents\web\araignees_idf\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{02B49ACA-2661-451C-9EF7-6420BB61E59C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9FF72D2B-81E2-4503-B33C-65D01F31A38D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1542" uniqueCount="890">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1543" uniqueCount="891">
   <si>
     <t>taxon</t>
   </si>
@@ -2673,6 +2673,9 @@
   </si>
   <si>
     <t>www/media/fiches/gibbaranea_bituberculata_femelle.webp</t>
+  </si>
+  <si>
+    <t>www/media/fiches/hypsosinga_albovittata_femelle.webp</t>
   </si>
   <si>
     <t>www/media/fiches/asagena_phalerata_male.webp</t>
@@ -3130,8 +3133,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E656"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A368" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="E387" sqref="E387"/>
+    <sheetView tabSelected="1" topLeftCell="A27" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="D46" sqref="D46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3763,7 +3766,10 @@
       </c>
       <c r="C45" t="b">
         <f>OR(Tableau1[[#This Row],[femelle]]&lt;&gt;"", Tableau1[[#This Row],[male]]&lt;&gt;"")</f>
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="D45" t="s">
+        <v>884</v>
       </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.3">
@@ -6053,7 +6059,7 @@
         <v>1</v>
       </c>
       <c r="D225" t="s">
-        <v>887</v>
+        <v>888</v>
       </c>
     </row>
     <row r="226" spans="1:5" x14ac:dyDescent="0.3">
@@ -8063,7 +8069,7 @@
         <v>1</v>
       </c>
       <c r="E386" t="s">
-        <v>889</v>
+        <v>890</v>
       </c>
     </row>
     <row r="387" spans="1:5" x14ac:dyDescent="0.3">
@@ -9194,7 +9200,7 @@
         <v>1</v>
       </c>
       <c r="D472" t="s">
-        <v>885</v>
+        <v>886</v>
       </c>
     </row>
     <row r="473" spans="1:5" x14ac:dyDescent="0.3">
@@ -9269,7 +9275,7 @@
         <v>715</v>
       </c>
       <c r="E477" t="s">
-        <v>886</v>
+        <v>887</v>
       </c>
     </row>
     <row r="478" spans="1:5" x14ac:dyDescent="0.3">
@@ -10220,7 +10226,7 @@
         <v>1</v>
       </c>
       <c r="E547" t="s">
-        <v>884</v>
+        <v>885</v>
       </c>
     </row>
     <row r="548" spans="1:5" x14ac:dyDescent="0.3">
@@ -11105,7 +11111,7 @@
         <v>1</v>
       </c>
       <c r="D613" t="s">
-        <v>888</v>
+        <v>889</v>
       </c>
     </row>
     <row r="614" spans="1:5" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
ajoute Liocranum rupicola mâle
</commit_message>
<xml_diff>
--- a/photos.xlsx
+++ b/photos.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cedri\Documents\web\araignees_idf\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3CCECD88-69E1-45BD-8018-A1B48716CF55}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{82F797E9-98D7-4177-98A1-AE25EACA31CB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1544" uniqueCount="892">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1545" uniqueCount="893">
   <si>
     <t>taxon</t>
   </si>
@@ -2697,6 +2697,9 @@
   </si>
   <si>
     <t>www/media/fiches/hogna_radiata_male.webp</t>
+  </si>
+  <si>
+    <t>www/media/fiches/liocranum_rupicola_male.webp</t>
   </si>
 </sst>
 </file>
@@ -3137,7 +3140,7 @@
   <dimension ref="A1:E656"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A369" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="D388" sqref="D388"/>
+      <selection activeCell="E370" sqref="E370"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -7853,7 +7856,10 @@
       </c>
       <c r="C369" t="b">
         <f>OR(Tableau1[[#This Row],[femelle]]&lt;&gt;"", Tableau1[[#This Row],[male]]&lt;&gt;"")</f>
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="E369" t="s">
+        <v>892</v>
       </c>
     </row>
     <row r="370" spans="1:5" x14ac:dyDescent="0.3">

</xml_diff>